<commit_message>
Transition do menu-titulo / resolve tabela de urls dos arquivos da tramitacao
</commit_message>
<xml_diff>
--- a/PIUS_Doc_ParticipacaoPublica.xlsx
+++ b/PIUS_Doc_ParticipacaoPublica.xlsx
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">hiperlinks!$A$1:$D$195</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateCount="117"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -668,7 +668,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6173" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6170" uniqueCount="1000">
   <si>
     <t>DOCUMENTAÇÃO PIUS</t>
   </si>
@@ -6673,6 +6673,12 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6691,6 +6697,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6698,24 +6716,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6743,6 +6743,24 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6761,24 +6779,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -6836,12 +6836,63 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6878,56 +6929,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6940,30 +6964,6 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -8553,10 +8553,10 @@
       </c>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="610"/>
-      <c r="B2" s="611"/>
-      <c r="C2" s="611"/>
-      <c r="D2" s="611"/>
+      <c r="A2" s="598"/>
+      <c r="B2" s="599"/>
+      <c r="C2" s="599"/>
+      <c r="D2" s="599"/>
       <c r="E2" s="548"/>
       <c r="F2" s="58" t="s">
         <v>51</v>
@@ -8598,11 +8598,11 @@
       <c r="T2" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="U2" s="611" t="s">
+      <c r="U2" s="599" t="s">
         <v>57</v>
       </c>
-      <c r="V2" s="611"/>
-      <c r="W2" s="612"/>
+      <c r="V2" s="599"/>
+      <c r="W2" s="606"/>
       <c r="X2" s="61" t="s">
         <v>59</v>
       </c>
@@ -8614,7 +8614,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="598" t="s">
+      <c r="A3" s="600" t="s">
         <v>358</v>
       </c>
       <c r="B3" s="157" t="s">
@@ -8645,7 +8645,7 @@
       <c r="Z3" s="52"/>
     </row>
     <row r="4" spans="1:26" ht="15">
-      <c r="A4" s="599"/>
+      <c r="A4" s="601"/>
       <c r="B4" s="74"/>
       <c r="C4" s="163" t="s">
         <v>116</v>
@@ -8674,7 +8674,7 @@
       <c r="Z4" s="52"/>
     </row>
     <row r="5" spans="1:26" ht="15">
-      <c r="A5" s="599"/>
+      <c r="A5" s="601"/>
       <c r="B5" s="74"/>
       <c r="D5" s="85" t="s">
         <v>81</v>
@@ -8714,17 +8714,17 @@
         <v>91</v>
       </c>
       <c r="T5" s="73"/>
-      <c r="U5" s="601" t="s">
+      <c r="U5" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="V5" s="602"/>
-      <c r="W5" s="603"/>
+      <c r="V5" s="604"/>
+      <c r="W5" s="605"/>
       <c r="X5" s="73"/>
       <c r="Y5" s="73"/>
       <c r="Z5" s="52"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="599"/>
+      <c r="A6" s="601"/>
       <c r="B6" s="73"/>
       <c r="C6" s="164" t="s">
         <v>117</v>
@@ -8754,7 +8754,7 @@
       <c r="Z6" s="52"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="599"/>
+      <c r="A7" s="601"/>
       <c r="B7" s="73"/>
       <c r="C7" s="164"/>
       <c r="D7" s="85" t="s">
@@ -8794,17 +8794,17 @@
       </c>
       <c r="S7" s="76"/>
       <c r="T7" s="73"/>
-      <c r="U7" s="601" t="s">
+      <c r="U7" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="V7" s="602"/>
-      <c r="W7" s="603"/>
+      <c r="V7" s="604"/>
+      <c r="W7" s="605"/>
       <c r="X7" s="73"/>
       <c r="Y7" s="73"/>
       <c r="Z7" s="52"/>
     </row>
     <row r="8" spans="1:26" ht="15.75">
-      <c r="A8" s="598" t="s">
+      <c r="A8" s="600" t="s">
         <v>359</v>
       </c>
       <c r="B8" s="157" t="s">
@@ -8836,7 +8836,7 @@
       <c r="Z8" s="172"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="599"/>
+      <c r="A9" s="601"/>
       <c r="B9" s="73"/>
       <c r="C9" s="166" t="s">
         <v>71</v>
@@ -8874,17 +8874,17 @@
       </c>
       <c r="S9" s="76"/>
       <c r="T9" s="73"/>
-      <c r="U9" s="601" t="s">
+      <c r="U9" s="603" t="s">
         <v>96</v>
       </c>
-      <c r="V9" s="602"/>
-      <c r="W9" s="603"/>
+      <c r="V9" s="604"/>
+      <c r="W9" s="605"/>
       <c r="X9" s="73"/>
       <c r="Y9" s="73"/>
       <c r="Z9" s="52"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="599"/>
+      <c r="A10" s="601"/>
       <c r="B10" s="73"/>
       <c r="C10" s="165" t="s">
         <v>3</v>
@@ -8928,17 +8928,17 @@
       </c>
       <c r="S10" s="76"/>
       <c r="T10" s="73"/>
-      <c r="U10" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="V10" s="602"/>
-      <c r="W10" s="603"/>
+      <c r="U10" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="V10" s="604"/>
+      <c r="W10" s="605"/>
       <c r="X10" s="73"/>
       <c r="Y10" s="73"/>
       <c r="Z10" s="52"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="599"/>
+      <c r="A11" s="601"/>
       <c r="B11" s="73"/>
       <c r="C11" s="165" t="s">
         <v>35</v>
@@ -8982,17 +8982,17 @@
       </c>
       <c r="S11" s="76"/>
       <c r="T11" s="73"/>
-      <c r="U11" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="V11" s="602"/>
-      <c r="W11" s="603"/>
+      <c r="U11" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="V11" s="604"/>
+      <c r="W11" s="605"/>
       <c r="X11" s="73"/>
       <c r="Y11" s="73"/>
       <c r="Z11" s="52"/>
     </row>
     <row r="12" spans="1:26" ht="15.75">
-      <c r="A12" s="599"/>
+      <c r="A12" s="601"/>
       <c r="B12" s="158" t="s">
         <v>127</v>
       </c>
@@ -9022,7 +9022,7 @@
       <c r="Z12" s="52"/>
     </row>
     <row r="13" spans="1:26" ht="15">
-      <c r="A13" s="599"/>
+      <c r="A13" s="601"/>
       <c r="B13" s="74"/>
       <c r="C13" s="165" t="s">
         <v>88</v>
@@ -9052,7 +9052,7 @@
       <c r="Z13" s="52"/>
     </row>
     <row r="14" spans="1:26" ht="15">
-      <c r="A14" s="599"/>
+      <c r="A14" s="601"/>
       <c r="B14" s="74"/>
       <c r="C14" s="165"/>
       <c r="D14" s="53" t="s">
@@ -9098,17 +9098,17 @@
       </c>
       <c r="S14" s="76"/>
       <c r="T14" s="73"/>
-      <c r="U14" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="V14" s="602"/>
-      <c r="W14" s="603"/>
+      <c r="U14" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="V14" s="604"/>
+      <c r="W14" s="605"/>
       <c r="X14" s="73"/>
       <c r="Y14" s="73"/>
       <c r="Z14" s="52"/>
     </row>
     <row r="15" spans="1:26" ht="15">
-      <c r="A15" s="599"/>
+      <c r="A15" s="601"/>
       <c r="B15" s="74"/>
       <c r="C15" s="163"/>
       <c r="D15" s="53" t="s">
@@ -9156,17 +9156,17 @@
       </c>
       <c r="S15" s="76"/>
       <c r="T15" s="73"/>
-      <c r="U15" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="V15" s="602"/>
-      <c r="W15" s="603"/>
+      <c r="U15" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="V15" s="604"/>
+      <c r="W15" s="605"/>
       <c r="X15" s="73"/>
       <c r="Y15" s="73"/>
       <c r="Z15" s="52"/>
     </row>
     <row r="16" spans="1:26" ht="15">
-      <c r="A16" s="599"/>
+      <c r="A16" s="601"/>
       <c r="B16" s="74"/>
       <c r="C16" s="163"/>
       <c r="D16" s="53" t="s">
@@ -9206,17 +9206,17 @@
       </c>
       <c r="S16" s="76"/>
       <c r="T16" s="73"/>
-      <c r="U16" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="V16" s="602"/>
-      <c r="W16" s="603"/>
+      <c r="U16" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="V16" s="604"/>
+      <c r="W16" s="605"/>
       <c r="X16" s="73"/>
       <c r="Y16" s="73"/>
       <c r="Z16" s="52"/>
     </row>
     <row r="17" spans="1:26" ht="15">
-      <c r="A17" s="599"/>
+      <c r="A17" s="601"/>
       <c r="B17" s="74"/>
       <c r="C17" s="163"/>
       <c r="D17" s="53" t="s">
@@ -9250,17 +9250,17 @@
       </c>
       <c r="S17" s="76"/>
       <c r="T17" s="73"/>
-      <c r="U17" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="V17" s="602"/>
-      <c r="W17" s="603"/>
+      <c r="U17" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="V17" s="604"/>
+      <c r="W17" s="605"/>
       <c r="X17" s="73"/>
       <c r="Y17" s="73"/>
       <c r="Z17" s="52"/>
     </row>
     <row r="18" spans="1:26" ht="15">
-      <c r="A18" s="599"/>
+      <c r="A18" s="601"/>
       <c r="B18" s="74"/>
       <c r="C18" s="165" t="s">
         <v>76</v>
@@ -9290,7 +9290,7 @@
       <c r="Z18" s="52"/>
     </row>
     <row r="19" spans="1:26" ht="15">
-      <c r="A19" s="599"/>
+      <c r="A19" s="601"/>
       <c r="B19" s="74"/>
       <c r="C19" s="165"/>
       <c r="D19" s="53" t="s">
@@ -9330,17 +9330,17 @@
       <c r="R19" s="70"/>
       <c r="S19" s="76"/>
       <c r="T19" s="73"/>
-      <c r="U19" s="601" t="s">
+      <c r="U19" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="V19" s="602"/>
-      <c r="W19" s="603"/>
+      <c r="V19" s="604"/>
+      <c r="W19" s="605"/>
       <c r="X19" s="73"/>
       <c r="Y19" s="73"/>
       <c r="Z19" s="52"/>
     </row>
     <row r="20" spans="1:26" ht="15">
-      <c r="A20" s="599"/>
+      <c r="A20" s="601"/>
       <c r="B20" s="74"/>
       <c r="C20" s="163"/>
       <c r="D20" s="53" t="s">
@@ -9380,17 +9380,17 @@
       <c r="R20" s="70"/>
       <c r="S20" s="76"/>
       <c r="T20" s="73"/>
-      <c r="U20" s="601" t="s">
+      <c r="U20" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="V20" s="602"/>
-      <c r="W20" s="603"/>
+      <c r="V20" s="604"/>
+      <c r="W20" s="605"/>
       <c r="X20" s="73"/>
       <c r="Y20" s="73"/>
       <c r="Z20" s="52"/>
     </row>
     <row r="21" spans="1:26" ht="15">
-      <c r="A21" s="599"/>
+      <c r="A21" s="601"/>
       <c r="B21" s="74"/>
       <c r="C21" s="163"/>
       <c r="D21" s="53" t="s">
@@ -9428,17 +9428,17 @@
       <c r="R21" s="70"/>
       <c r="S21" s="76"/>
       <c r="T21" s="73"/>
-      <c r="U21" s="601" t="s">
+      <c r="U21" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="V21" s="602"/>
-      <c r="W21" s="603"/>
+      <c r="V21" s="604"/>
+      <c r="W21" s="605"/>
       <c r="X21" s="73"/>
       <c r="Y21" s="73"/>
       <c r="Z21" s="52"/>
     </row>
     <row r="22" spans="1:26" ht="15">
-      <c r="A22" s="599"/>
+      <c r="A22" s="601"/>
       <c r="B22" s="74"/>
       <c r="C22" s="41"/>
       <c r="D22" s="53" t="s">
@@ -9478,17 +9478,17 @@
       <c r="R22" s="70"/>
       <c r="S22" s="76"/>
       <c r="T22" s="73"/>
-      <c r="U22" s="601" t="s">
+      <c r="U22" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="V22" s="602"/>
-      <c r="W22" s="603"/>
+      <c r="V22" s="604"/>
+      <c r="W22" s="605"/>
       <c r="X22" s="73"/>
       <c r="Y22" s="73"/>
       <c r="Z22" s="52"/>
     </row>
     <row r="23" spans="1:26" ht="15">
-      <c r="A23" s="599"/>
+      <c r="A23" s="601"/>
       <c r="B23" s="74"/>
       <c r="C23" s="41"/>
       <c r="D23" s="53" t="s">
@@ -9524,17 +9524,17 @@
       <c r="R23" s="70"/>
       <c r="S23" s="76"/>
       <c r="T23" s="73"/>
-      <c r="U23" s="601" t="s">
+      <c r="U23" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="V23" s="602"/>
-      <c r="W23" s="603"/>
+      <c r="V23" s="604"/>
+      <c r="W23" s="605"/>
       <c r="X23" s="73"/>
       <c r="Y23" s="73"/>
       <c r="Z23" s="52"/>
     </row>
     <row r="24" spans="1:26" ht="15">
-      <c r="A24" s="600"/>
+      <c r="A24" s="602"/>
       <c r="B24" s="79"/>
       <c r="C24" s="161"/>
       <c r="D24" s="81"/>
@@ -9554,15 +9554,15 @@
       <c r="R24" s="81"/>
       <c r="S24" s="76"/>
       <c r="T24" s="81"/>
-      <c r="U24" s="604"/>
-      <c r="V24" s="605"/>
-      <c r="W24" s="606"/>
+      <c r="U24" s="610"/>
+      <c r="V24" s="611"/>
+      <c r="W24" s="612"/>
       <c r="X24" s="81"/>
       <c r="Y24" s="81"/>
       <c r="Z24" s="160"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A25" s="598" t="s">
+      <c r="A25" s="600" t="s">
         <v>360</v>
       </c>
       <c r="B25" s="175" t="s">
@@ -9604,7 +9604,7 @@
       <c r="Z25" s="172"/>
     </row>
     <row r="26" spans="1:26" ht="15.75">
-      <c r="A26" s="599"/>
+      <c r="A26" s="601"/>
       <c r="B26" s="158" t="s">
         <v>129</v>
       </c>
@@ -9634,7 +9634,7 @@
       <c r="Z26" s="52"/>
     </row>
     <row r="27" spans="1:26" ht="15">
-      <c r="A27" s="599"/>
+      <c r="A27" s="601"/>
       <c r="B27" s="73"/>
       <c r="C27" s="124" t="s">
         <v>74</v>
@@ -9664,7 +9664,7 @@
       <c r="Z27" s="52"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="599"/>
+      <c r="A28" s="601"/>
       <c r="B28" s="73"/>
       <c r="C28" s="124"/>
       <c r="D28" s="73" t="s">
@@ -9694,17 +9694,17 @@
       <c r="R28" s="70"/>
       <c r="S28" s="76"/>
       <c r="T28" s="73"/>
-      <c r="U28" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="V28" s="602"/>
-      <c r="W28" s="603"/>
+      <c r="U28" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="V28" s="604"/>
+      <c r="W28" s="605"/>
       <c r="X28" s="73"/>
       <c r="Y28" s="73"/>
       <c r="Z28" s="52"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="599"/>
+      <c r="A29" s="601"/>
       <c r="B29" s="73"/>
       <c r="C29" s="52"/>
       <c r="D29" s="53" t="s">
@@ -9734,17 +9734,17 @@
       <c r="R29" s="70"/>
       <c r="S29" s="76"/>
       <c r="T29" s="73"/>
-      <c r="U29" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="V29" s="602"/>
-      <c r="W29" s="603"/>
+      <c r="U29" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="V29" s="604"/>
+      <c r="W29" s="605"/>
       <c r="X29" s="73"/>
       <c r="Y29" s="73"/>
       <c r="Z29" s="52"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="599"/>
+      <c r="A30" s="601"/>
       <c r="B30" s="73"/>
       <c r="C30" s="52"/>
       <c r="D30" s="53" t="s">
@@ -9770,15 +9770,15 @@
       <c r="R30" s="70"/>
       <c r="S30" s="76"/>
       <c r="T30" s="73"/>
-      <c r="U30" s="601"/>
-      <c r="V30" s="602"/>
-      <c r="W30" s="603"/>
+      <c r="U30" s="603"/>
+      <c r="V30" s="604"/>
+      <c r="W30" s="605"/>
       <c r="X30" s="73"/>
       <c r="Y30" s="73"/>
       <c r="Z30" s="52"/>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="599"/>
+      <c r="A31" s="601"/>
       <c r="B31" s="73"/>
       <c r="C31" s="52"/>
       <c r="D31" s="53" t="s">
@@ -9804,15 +9804,15 @@
       <c r="R31" s="70"/>
       <c r="S31" s="76"/>
       <c r="T31" s="73"/>
-      <c r="U31" s="601"/>
-      <c r="V31" s="602"/>
-      <c r="W31" s="603"/>
+      <c r="U31" s="603"/>
+      <c r="V31" s="604"/>
+      <c r="W31" s="605"/>
       <c r="X31" s="73"/>
       <c r="Y31" s="73"/>
       <c r="Z31" s="52"/>
     </row>
     <row r="32" spans="1:26" ht="15">
-      <c r="A32" s="599"/>
+      <c r="A32" s="601"/>
       <c r="B32" s="73"/>
       <c r="C32" s="124" t="s">
         <v>76</v>
@@ -9842,7 +9842,7 @@
       <c r="Z32" s="52"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A33" s="599"/>
+      <c r="A33" s="601"/>
       <c r="B33" s="73"/>
       <c r="C33" s="124"/>
       <c r="D33" s="73" t="s">
@@ -9884,7 +9884,7 @@
       <c r="Z33" s="52"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="599"/>
+      <c r="A34" s="601"/>
       <c r="B34" s="73"/>
       <c r="C34" s="52"/>
       <c r="D34" s="53" t="s">
@@ -9926,7 +9926,7 @@
       <c r="Z34" s="52"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="599"/>
+      <c r="A35" s="601"/>
       <c r="B35" s="73"/>
       <c r="C35" s="52"/>
       <c r="D35" s="53" t="s">
@@ -9966,7 +9966,7 @@
       <c r="Z35" s="52"/>
     </row>
     <row r="36" spans="1:26" ht="15">
-      <c r="A36" s="599"/>
+      <c r="A36" s="601"/>
       <c r="B36" s="73"/>
       <c r="C36" s="46"/>
       <c r="D36" s="53" t="s">
@@ -10008,7 +10008,7 @@
       <c r="Z36" s="52"/>
     </row>
     <row r="37" spans="1:26">
-      <c r="A37" s="600"/>
+      <c r="A37" s="602"/>
       <c r="B37" s="73"/>
       <c r="C37" s="52"/>
       <c r="D37" s="53" t="s">
@@ -10554,16 +10554,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="U7:W7"/>
     <mergeCell ref="U21:W21"/>
     <mergeCell ref="U22:W22"/>
     <mergeCell ref="U23:W23"/>
@@ -10580,6 +10570,16 @@
     <mergeCell ref="U11:W11"/>
     <mergeCell ref="U14:W14"/>
     <mergeCell ref="U15:W15"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="U7:W7"/>
   </mergeCells>
   <conditionalFormatting sqref="F12:G22 F25:R38 F23:R23 H24:N24 F10:G10 H8:R8 H10:R22 F7:R7 F5:R5">
     <cfRule type="cellIs" dxfId="33" priority="13" operator="equal">
@@ -15379,6 +15379,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="CO4:CY4"/>
     <mergeCell ref="CZ4:DH4"/>
     <mergeCell ref="DI4:DM4"/>
     <mergeCell ref="DN4:DP4"/>
@@ -15395,7 +15396,6 @@
     <mergeCell ref="BC4:BL4"/>
     <mergeCell ref="DV4:EI4"/>
     <mergeCell ref="BM4:CN4"/>
-    <mergeCell ref="CO4:CY4"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C13">
     <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Projeto">
@@ -15471,14 +15471,14 @@
     </row>
     <row r="3" spans="5:20" ht="15.75" thickBot="1">
       <c r="F3" s="33"/>
-      <c r="G3" s="653" t="s">
+      <c r="G3" s="654" t="s">
         <v>115</v>
       </c>
-      <c r="H3" s="654"/>
-      <c r="J3" s="653" t="s">
+      <c r="H3" s="655"/>
+      <c r="J3" s="654" t="s">
         <v>115</v>
       </c>
-      <c r="K3" s="654"/>
+      <c r="K3" s="655"/>
       <c r="S3" t="s">
         <v>154</v>
       </c>
@@ -15520,11 +15520,11 @@
       </c>
       <c r="M5" s="106"/>
       <c r="N5" s="118"/>
-      <c r="O5" s="671" t="s">
+      <c r="O5" s="662" t="s">
         <v>132</v>
       </c>
-      <c r="P5" s="671"/>
-      <c r="Q5" s="672"/>
+      <c r="P5" s="662"/>
+      <c r="Q5" s="663"/>
     </row>
     <row r="6" spans="5:20" ht="15.75" customHeight="1">
       <c r="E6" s="179"/>
@@ -15534,7 +15534,7 @@
       <c r="G6" s="181" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="655" t="s">
+      <c r="H6" s="672" t="s">
         <v>141</v>
       </c>
       <c r="I6">
@@ -15543,16 +15543,16 @@
       <c r="J6" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="678" t="s">
+      <c r="K6" s="656" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="106"/>
       <c r="N6" s="118"/>
       <c r="O6" s="57"/>
-      <c r="P6" s="669" t="s">
+      <c r="P6" s="666" t="s">
         <v>116</v>
       </c>
-      <c r="Q6" s="670"/>
+      <c r="Q6" s="667"/>
       <c r="S6" s="195">
         <v>1</v>
       </c>
@@ -15568,14 +15568,14 @@
       <c r="G7" s="182" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="656"/>
+      <c r="H7" s="673"/>
       <c r="I7">
         <v>2</v>
       </c>
       <c r="J7" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="679"/>
+      <c r="K7" s="657"/>
       <c r="M7" s="113"/>
       <c r="N7" s="119"/>
       <c r="O7" s="57"/>
@@ -15596,18 +15596,18 @@
       <c r="G8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="657"/>
+      <c r="H8" s="674"/>
       <c r="J8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="680"/>
+      <c r="K8" s="658"/>
       <c r="M8" s="113"/>
       <c r="N8" s="119"/>
       <c r="O8" s="76"/>
-      <c r="P8" s="667" t="s">
+      <c r="P8" s="668" t="s">
         <v>117</v>
       </c>
-      <c r="Q8" s="668"/>
+      <c r="Q8" s="669"/>
       <c r="S8" s="206" t="s">
         <v>148</v>
       </c>
@@ -15735,7 +15735,7 @@
       <c r="G14" s="185" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="658" t="s">
+      <c r="H14" s="675" t="s">
         <v>145</v>
       </c>
       <c r="I14">
@@ -15744,7 +15744,7 @@
       <c r="J14" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="681" t="s">
+      <c r="K14" s="659" t="s">
         <v>19</v>
       </c>
       <c r="M14" s="114"/>
@@ -15765,21 +15765,21 @@
       <c r="G15" s="186" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="659"/>
+      <c r="H15" s="676"/>
       <c r="I15">
         <v>5</v>
       </c>
       <c r="J15" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="682"/>
+      <c r="K15" s="660"/>
       <c r="M15" s="106"/>
       <c r="N15" s="119"/>
-      <c r="O15" s="671" t="s">
+      <c r="O15" s="662" t="s">
         <v>133</v>
       </c>
-      <c r="P15" s="671"/>
-      <c r="Q15" s="672"/>
+      <c r="P15" s="662"/>
+      <c r="Q15" s="663"/>
       <c r="S15" s="206"/>
       <c r="T15" s="208" t="s">
         <v>75</v>
@@ -15793,23 +15793,23 @@
       <c r="G16" s="186" t="s">
         <v>146</v>
       </c>
-      <c r="H16" s="660"/>
+      <c r="H16" s="677"/>
       <c r="I16">
         <v>6</v>
       </c>
       <c r="J16" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="682"/>
+      <c r="K16" s="660"/>
       <c r="M16" s="114" t="s">
         <v>122</v>
       </c>
       <c r="N16" s="119"/>
       <c r="O16" s="76"/>
-      <c r="P16" s="673" t="s">
+      <c r="P16" s="670" t="s">
         <v>71</v>
       </c>
-      <c r="Q16" s="674"/>
+      <c r="Q16" s="671"/>
       <c r="S16" s="206"/>
       <c r="T16" s="208" t="s">
         <v>73</v>
@@ -15823,7 +15823,7 @@
       <c r="G17" s="187" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="661" t="s">
+      <c r="H17" s="678" t="s">
         <v>24</v>
       </c>
       <c r="I17">
@@ -15832,16 +15832,16 @@
       <c r="J17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="683"/>
+      <c r="K17" s="661"/>
       <c r="M17" s="114" t="s">
         <v>121</v>
       </c>
       <c r="N17" s="120"/>
       <c r="O17" s="76"/>
-      <c r="P17" s="673" t="s">
+      <c r="P17" s="670" t="s">
         <v>3</v>
       </c>
-      <c r="Q17" s="674"/>
+      <c r="Q17" s="671"/>
       <c r="S17" s="206"/>
       <c r="T17" s="208" t="s">
         <v>119</v>
@@ -15853,20 +15853,20 @@
       <c r="G18" s="188" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="662"/>
+      <c r="H18" s="679"/>
       <c r="J18" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="678" t="s">
+      <c r="K18" s="656" t="s">
         <v>24</v>
       </c>
       <c r="M18" s="106"/>
       <c r="N18" s="120"/>
       <c r="O18" s="76"/>
-      <c r="P18" s="673" t="s">
+      <c r="P18" s="670" t="s">
         <v>35</v>
       </c>
-      <c r="Q18" s="674"/>
+      <c r="Q18" s="671"/>
       <c r="S18" s="206" t="s">
         <v>162</v>
       </c>
@@ -15880,11 +15880,11 @@
       <c r="G19" s="188" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="662"/>
+      <c r="H19" s="679"/>
       <c r="J19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="679"/>
+      <c r="K19" s="657"/>
       <c r="M19" s="106"/>
       <c r="N19" s="118"/>
       <c r="O19" s="76"/>
@@ -15901,18 +15901,18 @@
       <c r="G20" s="189" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="663"/>
+      <c r="H20" s="680"/>
       <c r="J20" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="680"/>
+      <c r="K20" s="658"/>
       <c r="M20" s="106"/>
       <c r="N20" s="120"/>
-      <c r="O20" s="671" t="s">
+      <c r="O20" s="662" t="s">
         <v>134</v>
       </c>
-      <c r="P20" s="671"/>
-      <c r="Q20" s="672"/>
+      <c r="P20" s="662"/>
+      <c r="Q20" s="663"/>
       <c r="S20" s="206"/>
       <c r="T20" s="208" t="s">
         <v>77</v>
@@ -15941,10 +15941,10 @@
       <c r="M21" s="106"/>
       <c r="N21" s="119"/>
       <c r="O21" s="57"/>
-      <c r="P21" s="669" t="s">
+      <c r="P21" s="666" t="s">
         <v>88</v>
       </c>
-      <c r="Q21" s="670"/>
+      <c r="Q21" s="667"/>
       <c r="S21" s="206"/>
       <c r="T21" s="208" t="s">
         <v>78</v>
@@ -15956,7 +15956,7 @@
       <c r="G22" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="664" t="s">
+      <c r="H22" s="681" t="s">
         <v>30</v>
       </c>
       <c r="J22" s="145"/>
@@ -15981,7 +15981,7 @@
       <c r="G23" s="193" t="s">
         <v>149</v>
       </c>
-      <c r="H23" s="665"/>
+      <c r="H23" s="682"/>
       <c r="J23" s="145"/>
       <c r="K23" s="149"/>
       <c r="M23" s="113"/>
@@ -16002,9 +16002,9 @@
       <c r="G24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="666"/>
+      <c r="H24" s="683"/>
       <c r="J24" s="146"/>
-      <c r="K24" s="677"/>
+      <c r="K24" s="653"/>
       <c r="M24" s="113"/>
       <c r="N24" s="119"/>
       <c r="O24" s="57"/>
@@ -16029,7 +16029,7 @@
         <v>152</v>
       </c>
       <c r="J25" s="147"/>
-      <c r="K25" s="677"/>
+      <c r="K25" s="653"/>
       <c r="M25" s="113"/>
       <c r="N25" s="119"/>
       <c r="O25" s="57"/>
@@ -16047,14 +16047,14 @@
         <v>12</v>
       </c>
       <c r="J26" s="147"/>
-      <c r="K26" s="677"/>
+      <c r="K26" s="653"/>
       <c r="M26" s="113"/>
       <c r="N26" s="119"/>
       <c r="O26" s="57"/>
-      <c r="P26" s="669" t="s">
+      <c r="P26" s="666" t="s">
         <v>76</v>
       </c>
-      <c r="Q26" s="670"/>
+      <c r="Q26" s="667"/>
       <c r="S26" s="196">
         <v>3</v>
       </c>
@@ -16226,11 +16226,11 @@
       <c r="K36" s="148"/>
       <c r="M36" s="113"/>
       <c r="N36" s="119"/>
-      <c r="O36" s="675" t="s">
+      <c r="O36" s="664" t="s">
         <v>135</v>
       </c>
-      <c r="P36" s="675"/>
-      <c r="Q36" s="676"/>
+      <c r="P36" s="664"/>
+      <c r="Q36" s="665"/>
       <c r="S36" s="196">
         <v>7</v>
       </c>
@@ -16244,10 +16244,10 @@
       <c r="M37" s="113"/>
       <c r="N37" s="119"/>
       <c r="O37" s="109"/>
-      <c r="P37" s="669" t="s">
+      <c r="P37" s="666" t="s">
         <v>98</v>
       </c>
-      <c r="Q37" s="670"/>
+      <c r="Q37" s="667"/>
       <c r="T37" s="205" t="s">
         <v>23</v>
       </c>
@@ -16315,20 +16315,20 @@
         <v>19</v>
       </c>
       <c r="N43" s="120"/>
-      <c r="O43" s="671" t="s">
+      <c r="O43" s="662" t="s">
         <v>136</v>
       </c>
-      <c r="P43" s="671"/>
-      <c r="Q43" s="672"/>
+      <c r="P43" s="662"/>
+      <c r="Q43" s="663"/>
     </row>
     <row r="44" spans="6:20" ht="15.75" customHeight="1">
       <c r="M44" s="113"/>
       <c r="N44" s="119"/>
       <c r="O44" s="76"/>
-      <c r="P44" s="669" t="s">
+      <c r="P44" s="666" t="s">
         <v>74</v>
       </c>
-      <c r="Q44" s="670"/>
+      <c r="Q44" s="667"/>
     </row>
     <row r="45" spans="6:20" ht="15" hidden="1" customHeight="1" outlineLevel="1">
       <c r="M45" s="106"/>
@@ -16370,10 +16370,10 @@
       <c r="M49" s="113"/>
       <c r="N49" s="119"/>
       <c r="O49" s="76"/>
-      <c r="P49" s="669" t="s">
+      <c r="P49" s="666" t="s">
         <v>76</v>
       </c>
-      <c r="Q49" s="670"/>
+      <c r="Q49" s="667"/>
     </row>
     <row r="50" spans="11:18" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="M50" s="113"/>
@@ -16451,11 +16451,11 @@
         <v>3</v>
       </c>
       <c r="N58" s="126"/>
-      <c r="O58" s="671" t="s">
+      <c r="O58" s="662" t="s">
         <v>137</v>
       </c>
-      <c r="P58" s="671"/>
-      <c r="Q58" s="672"/>
+      <c r="P58" s="662"/>
+      <c r="Q58" s="663"/>
     </row>
     <row r="59" spans="11:18" ht="15.75" customHeight="1">
       <c r="M59" s="111"/>
@@ -16469,11 +16469,11 @@
         <v>62</v>
       </c>
       <c r="N60" s="123"/>
-      <c r="O60" s="671" t="s">
+      <c r="O60" s="662" t="s">
         <v>138</v>
       </c>
-      <c r="P60" s="671"/>
-      <c r="Q60" s="672"/>
+      <c r="P60" s="662"/>
+      <c r="Q60" s="663"/>
       <c r="R60" s="110"/>
     </row>
     <row r="61" spans="11:18" ht="18">
@@ -16531,21 +16531,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="O36:Q36"/>
-    <mergeCell ref="O43:Q43"/>
-    <mergeCell ref="O58:Q58"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="O60:Q60"/>
-    <mergeCell ref="P49:Q49"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H17:H20"/>
+    <mergeCell ref="H22:H24"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="O5:Q5"/>
@@ -16553,11 +16543,21 @@
     <mergeCell ref="P18:Q18"/>
     <mergeCell ref="O15:Q15"/>
     <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H20"/>
-    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="O60:Q60"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="O43:Q43"/>
+    <mergeCell ref="O58:Q58"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="K18:K20"/>
   </mergeCells>
   <conditionalFormatting sqref="Q50:Q57 O60:O61 Q7 P37 Q45:Q48 Q22:Q25 Q19 Q38:Q41 P42 P44:P57 P21:P35 Q27:Q35 P6:P14 Q9:Q14 O5:O58 N20:N36 M22:M36 M16:M17 P17:P19 Q17 N7:N18 M7:M14">
     <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
@@ -16750,10 +16750,10 @@
         <v>167</v>
       </c>
       <c r="C2" s="241"/>
-      <c r="D2" s="688" t="s">
+      <c r="D2" s="684" t="s">
         <v>166</v>
       </c>
-      <c r="E2" s="689"/>
+      <c r="E2" s="685"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15.75">
@@ -17732,18 +17732,18 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:146" ht="39.75" thickBot="1">
-      <c r="A49" s="690" t="s">
+      <c r="A49" s="686" t="s">
         <v>197</v>
       </c>
-      <c r="B49" s="691"/>
-      <c r="C49" s="691"/>
-      <c r="D49" s="691"/>
-      <c r="E49" s="691"/>
-      <c r="F49" s="691"/>
-      <c r="G49" s="691"/>
-      <c r="H49" s="691"/>
-      <c r="I49" s="691"/>
-      <c r="J49" s="692"/>
+      <c r="B49" s="687"/>
+      <c r="C49" s="687"/>
+      <c r="D49" s="687"/>
+      <c r="E49" s="687"/>
+      <c r="F49" s="687"/>
+      <c r="G49" s="687"/>
+      <c r="H49" s="687"/>
+      <c r="I49" s="687"/>
+      <c r="J49" s="688"/>
       <c r="K49" s="644" t="s">
         <v>198</v>
       </c>
@@ -17886,16 +17886,16 @@
       <c r="EP49" s="259"/>
     </row>
     <row r="50" spans="1:146" ht="31.5">
-      <c r="A50" s="693" t="s">
+      <c r="A50" s="689" t="s">
         <v>200</v>
       </c>
-      <c r="B50" s="694"/>
-      <c r="C50" s="694"/>
-      <c r="D50" s="694"/>
-      <c r="E50" s="694"/>
-      <c r="F50" s="694"/>
-      <c r="G50" s="694"/>
-      <c r="H50" s="695"/>
+      <c r="B50" s="690"/>
+      <c r="C50" s="690"/>
+      <c r="D50" s="690"/>
+      <c r="E50" s="690"/>
+      <c r="F50" s="690"/>
+      <c r="G50" s="690"/>
+      <c r="H50" s="691"/>
       <c r="I50" s="638" t="s">
         <v>201</v>
       </c>
@@ -18066,8 +18066,8 @@
         <v>214</v>
       </c>
       <c r="B51" s="263"/>
-      <c r="C51" s="684"/>
-      <c r="D51" s="685"/>
+      <c r="C51" s="692"/>
+      <c r="D51" s="693"/>
       <c r="E51" s="263"/>
       <c r="F51" s="263"/>
       <c r="G51" s="263"/>
@@ -18282,10 +18282,10 @@
       <c r="B52" s="268" t="s">
         <v>218</v>
       </c>
-      <c r="C52" s="684" t="s">
+      <c r="C52" s="692" t="s">
         <v>218</v>
       </c>
-      <c r="D52" s="685"/>
+      <c r="D52" s="693"/>
       <c r="E52" s="268" t="s">
         <v>218</v>
       </c>
@@ -18574,10 +18574,10 @@
       <c r="B53" s="285" t="s">
         <v>220</v>
       </c>
-      <c r="C53" s="686" t="s">
+      <c r="C53" s="694" t="s">
         <v>221</v>
       </c>
-      <c r="D53" s="687"/>
+      <c r="D53" s="695"/>
       <c r="E53" s="285" t="s">
         <v>222</v>
       </c>
@@ -19224,6 +19224,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="DR50:DV50"/>
+    <mergeCell ref="DW50:EJ50"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C53:D53"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="K49:DN49"/>
@@ -19240,11 +19245,6 @@
     <mergeCell ref="DA50:DI50"/>
     <mergeCell ref="DJ50:DN50"/>
     <mergeCell ref="DO50:DQ50"/>
-    <mergeCell ref="DR50:DV50"/>
-    <mergeCell ref="DW50:EJ50"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C53:D53"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:E39 B26:C30 E29:E32 E15:E20 E10:E13">
     <cfRule type="cellIs" dxfId="6" priority="21" operator="equal">
@@ -19323,10 +19323,10 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="610"/>
-      <c r="B2" s="611"/>
-      <c r="C2" s="611"/>
-      <c r="D2" s="611"/>
+      <c r="A2" s="598"/>
+      <c r="B2" s="599"/>
+      <c r="C2" s="599"/>
+      <c r="D2" s="599"/>
       <c r="E2" s="58" t="s">
         <v>51</v>
       </c>
@@ -19351,11 +19351,11 @@
       <c r="M2" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="611" t="s">
+      <c r="N2" s="599" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="611"/>
-      <c r="P2" s="612"/>
+      <c r="O2" s="599"/>
+      <c r="P2" s="606"/>
       <c r="Q2" s="61" t="s">
         <v>59</v>
       </c>
@@ -19367,7 +19367,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="598" t="s">
+      <c r="A3" s="600" t="s">
         <v>358</v>
       </c>
       <c r="B3" s="157" t="s">
@@ -19391,7 +19391,7 @@
       <c r="S3" s="52"/>
     </row>
     <row r="4" spans="1:19" ht="15">
-      <c r="A4" s="599"/>
+      <c r="A4" s="601"/>
       <c r="B4" s="74"/>
       <c r="C4" s="163" t="s">
         <v>116</v>
@@ -19413,7 +19413,7 @@
       <c r="S4" s="52"/>
     </row>
     <row r="5" spans="1:19" ht="15">
-      <c r="A5" s="599"/>
+      <c r="A5" s="601"/>
       <c r="B5" s="74"/>
       <c r="D5" s="85" t="s">
         <v>81</v>
@@ -19440,17 +19440,17 @@
         <v>91</v>
       </c>
       <c r="M5" s="73"/>
-      <c r="N5" s="601" t="s">
+      <c r="N5" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="O5" s="602"/>
-      <c r="P5" s="603"/>
+      <c r="O5" s="604"/>
+      <c r="P5" s="605"/>
       <c r="Q5" s="73"/>
       <c r="R5" s="73"/>
       <c r="S5" s="52"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="599"/>
+      <c r="A6" s="601"/>
       <c r="B6" s="73"/>
       <c r="C6" s="164" t="s">
         <v>117</v>
@@ -19473,7 +19473,7 @@
       <c r="S6" s="52"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="599"/>
+      <c r="A7" s="601"/>
       <c r="B7" s="73"/>
       <c r="C7" s="164"/>
       <c r="D7" s="85" t="s">
@@ -19502,17 +19502,17 @@
       </c>
       <c r="L7" s="76"/>
       <c r="M7" s="73"/>
-      <c r="N7" s="601" t="s">
+      <c r="N7" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="O7" s="602"/>
-      <c r="P7" s="603"/>
+      <c r="O7" s="604"/>
+      <c r="P7" s="605"/>
       <c r="Q7" s="73"/>
       <c r="R7" s="73"/>
       <c r="S7" s="52"/>
     </row>
     <row r="8" spans="1:19" ht="15.75">
-      <c r="A8" s="598" t="s">
+      <c r="A8" s="600" t="s">
         <v>359</v>
       </c>
       <c r="B8" s="157" t="s">
@@ -19537,7 +19537,7 @@
       <c r="S8" s="172"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A9" s="599"/>
+      <c r="A9" s="601"/>
       <c r="B9" s="73"/>
       <c r="C9" s="166" t="s">
         <v>71</v>
@@ -19566,17 +19566,17 @@
       </c>
       <c r="L9" s="76"/>
       <c r="M9" s="73"/>
-      <c r="N9" s="601" t="s">
+      <c r="N9" s="603" t="s">
         <v>96</v>
       </c>
-      <c r="O9" s="602"/>
-      <c r="P9" s="603"/>
+      <c r="O9" s="604"/>
+      <c r="P9" s="605"/>
       <c r="Q9" s="73"/>
       <c r="R9" s="73"/>
       <c r="S9" s="52"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="599"/>
+      <c r="A10" s="601"/>
       <c r="B10" s="73"/>
       <c r="C10" s="165" t="s">
         <v>3</v>
@@ -19605,17 +19605,17 @@
       </c>
       <c r="L10" s="76"/>
       <c r="M10" s="73"/>
-      <c r="N10" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="O10" s="602"/>
-      <c r="P10" s="603"/>
+      <c r="N10" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="604"/>
+      <c r="P10" s="605"/>
       <c r="Q10" s="73"/>
       <c r="R10" s="73"/>
       <c r="S10" s="52"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="599"/>
+      <c r="A11" s="601"/>
       <c r="B11" s="73"/>
       <c r="C11" s="165" t="s">
         <v>35</v>
@@ -19644,17 +19644,17 @@
       </c>
       <c r="L11" s="76"/>
       <c r="M11" s="73"/>
-      <c r="N11" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="O11" s="602"/>
-      <c r="P11" s="603"/>
+      <c r="N11" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" s="604"/>
+      <c r="P11" s="605"/>
       <c r="Q11" s="73"/>
       <c r="R11" s="73"/>
       <c r="S11" s="52"/>
     </row>
     <row r="12" spans="1:19" ht="15.75">
-      <c r="A12" s="599"/>
+      <c r="A12" s="601"/>
       <c r="B12" s="158" t="s">
         <v>127</v>
       </c>
@@ -19677,7 +19677,7 @@
       <c r="S12" s="52"/>
     </row>
     <row r="13" spans="1:19" ht="15">
-      <c r="A13" s="599"/>
+      <c r="A13" s="601"/>
       <c r="B13" s="74"/>
       <c r="C13" s="165" t="s">
         <v>88</v>
@@ -19700,7 +19700,7 @@
       <c r="S13" s="52"/>
     </row>
     <row r="14" spans="1:19" ht="15">
-      <c r="A14" s="599"/>
+      <c r="A14" s="601"/>
       <c r="B14" s="74"/>
       <c r="C14" s="165"/>
       <c r="D14" s="53" t="s">
@@ -19729,17 +19729,17 @@
       </c>
       <c r="L14" s="76"/>
       <c r="M14" s="73"/>
-      <c r="N14" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="O14" s="602"/>
-      <c r="P14" s="603"/>
+      <c r="N14" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="O14" s="604"/>
+      <c r="P14" s="605"/>
       <c r="Q14" s="73"/>
       <c r="R14" s="73"/>
       <c r="S14" s="52"/>
     </row>
     <row r="15" spans="1:19" ht="15">
-      <c r="A15" s="599"/>
+      <c r="A15" s="601"/>
       <c r="B15" s="74"/>
       <c r="C15" s="163"/>
       <c r="D15" s="53" t="s">
@@ -19768,17 +19768,17 @@
       </c>
       <c r="L15" s="76"/>
       <c r="M15" s="73"/>
-      <c r="N15" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="O15" s="602"/>
-      <c r="P15" s="603"/>
+      <c r="N15" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="604"/>
+      <c r="P15" s="605"/>
       <c r="Q15" s="73"/>
       <c r="R15" s="73"/>
       <c r="S15" s="52"/>
     </row>
     <row r="16" spans="1:19" ht="15">
-      <c r="A16" s="599"/>
+      <c r="A16" s="601"/>
       <c r="B16" s="74"/>
       <c r="C16" s="163"/>
       <c r="D16" s="53" t="s">
@@ -19803,17 +19803,17 @@
       </c>
       <c r="L16" s="76"/>
       <c r="M16" s="73"/>
-      <c r="N16" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="O16" s="602"/>
-      <c r="P16" s="603"/>
+      <c r="N16" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" s="604"/>
+      <c r="P16" s="605"/>
       <c r="Q16" s="73"/>
       <c r="R16" s="73"/>
       <c r="S16" s="52"/>
     </row>
     <row r="17" spans="1:19" ht="15">
-      <c r="A17" s="599"/>
+      <c r="A17" s="601"/>
       <c r="B17" s="74"/>
       <c r="C17" s="163"/>
       <c r="D17" s="53" t="s">
@@ -19838,17 +19838,17 @@
       </c>
       <c r="L17" s="76"/>
       <c r="M17" s="73"/>
-      <c r="N17" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="O17" s="602"/>
-      <c r="P17" s="603"/>
+      <c r="N17" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="604"/>
+      <c r="P17" s="605"/>
       <c r="Q17" s="73"/>
       <c r="R17" s="73"/>
       <c r="S17" s="52"/>
     </row>
     <row r="18" spans="1:19" ht="15">
-      <c r="A18" s="599"/>
+      <c r="A18" s="601"/>
       <c r="B18" s="74"/>
       <c r="C18" s="165" t="s">
         <v>76</v>
@@ -19871,7 +19871,7 @@
       <c r="S18" s="52"/>
     </row>
     <row r="19" spans="1:19" ht="15">
-      <c r="A19" s="599"/>
+      <c r="A19" s="601"/>
       <c r="B19" s="74"/>
       <c r="C19" s="165"/>
       <c r="D19" s="53" t="s">
@@ -19896,17 +19896,17 @@
       <c r="K19" s="70"/>
       <c r="L19" s="76"/>
       <c r="M19" s="73"/>
-      <c r="N19" s="601" t="s">
+      <c r="N19" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="O19" s="602"/>
-      <c r="P19" s="603"/>
+      <c r="O19" s="604"/>
+      <c r="P19" s="605"/>
       <c r="Q19" s="73"/>
       <c r="R19" s="73"/>
       <c r="S19" s="52"/>
     </row>
     <row r="20" spans="1:19" ht="15">
-      <c r="A20" s="599"/>
+      <c r="A20" s="601"/>
       <c r="B20" s="74"/>
       <c r="C20" s="163"/>
       <c r="D20" s="53" t="s">
@@ -19931,17 +19931,17 @@
       <c r="K20" s="70"/>
       <c r="L20" s="76"/>
       <c r="M20" s="73"/>
-      <c r="N20" s="601" t="s">
+      <c r="N20" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="O20" s="602"/>
-      <c r="P20" s="603"/>
+      <c r="O20" s="604"/>
+      <c r="P20" s="605"/>
       <c r="Q20" s="73"/>
       <c r="R20" s="73"/>
       <c r="S20" s="52"/>
     </row>
     <row r="21" spans="1:19" ht="15">
-      <c r="A21" s="599"/>
+      <c r="A21" s="601"/>
       <c r="B21" s="74"/>
       <c r="C21" s="163"/>
       <c r="D21" s="53" t="s">
@@ -19966,17 +19966,17 @@
       <c r="K21" s="70"/>
       <c r="L21" s="76"/>
       <c r="M21" s="73"/>
-      <c r="N21" s="601" t="s">
+      <c r="N21" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="O21" s="602"/>
-      <c r="P21" s="603"/>
+      <c r="O21" s="604"/>
+      <c r="P21" s="605"/>
       <c r="Q21" s="73"/>
       <c r="R21" s="73"/>
       <c r="S21" s="52"/>
     </row>
     <row r="22" spans="1:19" ht="15">
-      <c r="A22" s="599"/>
+      <c r="A22" s="601"/>
       <c r="B22" s="74"/>
       <c r="C22" s="41"/>
       <c r="D22" s="53" t="s">
@@ -20001,17 +20001,17 @@
       <c r="K22" s="70"/>
       <c r="L22" s="76"/>
       <c r="M22" s="73"/>
-      <c r="N22" s="601" t="s">
+      <c r="N22" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="O22" s="602"/>
-      <c r="P22" s="603"/>
+      <c r="O22" s="604"/>
+      <c r="P22" s="605"/>
       <c r="Q22" s="73"/>
       <c r="R22" s="73"/>
       <c r="S22" s="52"/>
     </row>
     <row r="23" spans="1:19" ht="15">
-      <c r="A23" s="599"/>
+      <c r="A23" s="601"/>
       <c r="B23" s="74"/>
       <c r="C23" s="41"/>
       <c r="D23" s="53" t="s">
@@ -20036,17 +20036,17 @@
       <c r="K23" s="70"/>
       <c r="L23" s="76"/>
       <c r="M23" s="73"/>
-      <c r="N23" s="601" t="s">
+      <c r="N23" s="603" t="s">
         <v>91</v>
       </c>
-      <c r="O23" s="602"/>
-      <c r="P23" s="603"/>
+      <c r="O23" s="604"/>
+      <c r="P23" s="605"/>
       <c r="Q23" s="73"/>
       <c r="R23" s="73"/>
       <c r="S23" s="52"/>
     </row>
     <row r="24" spans="1:19" ht="15">
-      <c r="A24" s="600"/>
+      <c r="A24" s="602"/>
       <c r="B24" s="79"/>
       <c r="C24" s="161"/>
       <c r="D24" s="81" t="s">
@@ -20071,17 +20071,17 @@
       <c r="K24" s="81"/>
       <c r="L24" s="76"/>
       <c r="M24" s="81"/>
-      <c r="N24" s="604" t="s">
+      <c r="N24" s="610" t="s">
         <v>91</v>
       </c>
-      <c r="O24" s="605"/>
-      <c r="P24" s="606"/>
+      <c r="O24" s="611"/>
+      <c r="P24" s="612"/>
       <c r="Q24" s="81"/>
       <c r="R24" s="81"/>
       <c r="S24" s="160"/>
     </row>
     <row r="25" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A25" s="598" t="s">
+      <c r="A25" s="600" t="s">
         <v>360</v>
       </c>
       <c r="B25" s="175" t="s">
@@ -20116,7 +20116,7 @@
       <c r="S25" s="172"/>
     </row>
     <row r="26" spans="1:19" ht="15.75">
-      <c r="A26" s="599"/>
+      <c r="A26" s="601"/>
       <c r="B26" s="158" t="s">
         <v>129</v>
       </c>
@@ -20139,7 +20139,7 @@
       <c r="S26" s="52"/>
     </row>
     <row r="27" spans="1:19" ht="15">
-      <c r="A27" s="599"/>
+      <c r="A27" s="601"/>
       <c r="B27" s="73"/>
       <c r="C27" s="124" t="s">
         <v>74</v>
@@ -20162,7 +20162,7 @@
       <c r="S27" s="52"/>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="599"/>
+      <c r="A28" s="601"/>
       <c r="B28" s="73"/>
       <c r="C28" s="124"/>
       <c r="D28" s="73" t="s">
@@ -20181,17 +20181,17 @@
       <c r="K28" s="70"/>
       <c r="L28" s="76"/>
       <c r="M28" s="73"/>
-      <c r="N28" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="O28" s="602"/>
-      <c r="P28" s="603"/>
+      <c r="N28" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="O28" s="604"/>
+      <c r="P28" s="605"/>
       <c r="Q28" s="73"/>
       <c r="R28" s="73"/>
       <c r="S28" s="52"/>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="599"/>
+      <c r="A29" s="601"/>
       <c r="B29" s="73"/>
       <c r="C29" s="52"/>
       <c r="D29" s="53" t="s">
@@ -20212,17 +20212,17 @@
       <c r="K29" s="70"/>
       <c r="L29" s="76"/>
       <c r="M29" s="73"/>
-      <c r="N29" s="601" t="s">
-        <v>63</v>
-      </c>
-      <c r="O29" s="602"/>
-      <c r="P29" s="603"/>
+      <c r="N29" s="603" t="s">
+        <v>63</v>
+      </c>
+      <c r="O29" s="604"/>
+      <c r="P29" s="605"/>
       <c r="Q29" s="73"/>
       <c r="R29" s="73"/>
       <c r="S29" s="52"/>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="599"/>
+      <c r="A30" s="601"/>
       <c r="B30" s="73"/>
       <c r="C30" s="52"/>
       <c r="D30" s="53" t="s">
@@ -20239,15 +20239,15 @@
       <c r="K30" s="70"/>
       <c r="L30" s="76"/>
       <c r="M30" s="73"/>
-      <c r="N30" s="601"/>
-      <c r="O30" s="602"/>
-      <c r="P30" s="603"/>
+      <c r="N30" s="603"/>
+      <c r="O30" s="604"/>
+      <c r="P30" s="605"/>
       <c r="Q30" s="73"/>
       <c r="R30" s="73"/>
       <c r="S30" s="52"/>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="599"/>
+      <c r="A31" s="601"/>
       <c r="B31" s="73"/>
       <c r="C31" s="52"/>
       <c r="D31" s="53" t="s">
@@ -20264,15 +20264,15 @@
       <c r="K31" s="70"/>
       <c r="L31" s="76"/>
       <c r="M31" s="73"/>
-      <c r="N31" s="601"/>
-      <c r="O31" s="602"/>
-      <c r="P31" s="603"/>
+      <c r="N31" s="603"/>
+      <c r="O31" s="604"/>
+      <c r="P31" s="605"/>
       <c r="Q31" s="73"/>
       <c r="R31" s="73"/>
       <c r="S31" s="52"/>
     </row>
     <row r="32" spans="1:19" ht="15">
-      <c r="A32" s="599"/>
+      <c r="A32" s="601"/>
       <c r="B32" s="73"/>
       <c r="C32" s="124" t="s">
         <v>76</v>
@@ -20295,7 +20295,7 @@
       <c r="S32" s="52"/>
     </row>
     <row r="33" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A33" s="599"/>
+      <c r="A33" s="601"/>
       <c r="B33" s="73"/>
       <c r="C33" s="124"/>
       <c r="D33" s="73" t="s">
@@ -20326,7 +20326,7 @@
       <c r="S33" s="52"/>
     </row>
     <row r="34" spans="1:19">
-      <c r="A34" s="599"/>
+      <c r="A34" s="601"/>
       <c r="B34" s="73"/>
       <c r="C34" s="52"/>
       <c r="D34" s="53" t="s">
@@ -20357,7 +20357,7 @@
       <c r="S34" s="52"/>
     </row>
     <row r="35" spans="1:19">
-      <c r="A35" s="599"/>
+      <c r="A35" s="601"/>
       <c r="B35" s="73"/>
       <c r="C35" s="52"/>
       <c r="D35" s="53" t="s">
@@ -20388,7 +20388,7 @@
       <c r="S35" s="52"/>
     </row>
     <row r="36" spans="1:19" ht="15">
-      <c r="A36" s="599"/>
+      <c r="A36" s="601"/>
       <c r="B36" s="73"/>
       <c r="C36" s="46"/>
       <c r="D36" s="53" t="s">
@@ -20419,7 +20419,7 @@
       <c r="S36" s="52"/>
     </row>
     <row r="37" spans="1:19">
-      <c r="A37" s="600"/>
+      <c r="A37" s="602"/>
       <c r="B37" s="73"/>
       <c r="C37" s="52"/>
       <c r="D37" s="53" t="s">
@@ -20679,6 +20679,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A24"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="N28:P28"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A25:A37"/>
     <mergeCell ref="N20:P20"/>
@@ -20695,16 +20705,6 @@
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="N31:P31"/>
     <mergeCell ref="N21:P21"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A24"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="N28:P28"/>
   </mergeCells>
   <conditionalFormatting sqref="E12:E22 E25:K38 E23:K23 F24:H24 E10 F8:K8 F10:K22 E7:K7 E5:K5">
     <cfRule type="cellIs" dxfId="77" priority="17" operator="equal">
@@ -24402,7 +24402,7 @@
       <c r="FA11" s="320"/>
     </row>
     <row r="12" spans="1:157" ht="15.75" customHeight="1">
-      <c r="A12" s="599" t="s">
+      <c r="A12" s="601" t="s">
         <v>358</v>
       </c>
       <c r="B12" s="426" t="s">
@@ -24564,7 +24564,7 @@
       <c r="EZ12" s="160"/>
     </row>
     <row r="13" spans="1:157" ht="15" customHeight="1">
-      <c r="A13" s="599"/>
+      <c r="A13" s="601"/>
       <c r="B13" s="74"/>
       <c r="C13" s="163" t="s">
         <v>116</v>
@@ -24635,7 +24635,7 @@
       <c r="BO13" s="353"/>
     </row>
     <row r="14" spans="1:157" ht="15" customHeight="1">
-      <c r="A14" s="599"/>
+      <c r="A14" s="601"/>
       <c r="B14" s="74"/>
       <c r="D14" s="85" t="s">
         <v>81</v>
@@ -25101,7 +25101,7 @@
       </c>
     </row>
     <row r="15" spans="1:157" ht="15" customHeight="1">
-      <c r="A15" s="599"/>
+      <c r="A15" s="601"/>
       <c r="B15" s="73"/>
       <c r="C15" s="164" t="s">
         <v>117</v>
@@ -25172,7 +25172,7 @@
       <c r="BO15" s="353"/>
     </row>
     <row r="16" spans="1:157">
-      <c r="A16" s="599"/>
+      <c r="A16" s="601"/>
       <c r="B16" s="73"/>
       <c r="C16" s="164"/>
       <c r="D16" s="85" t="s">
@@ -25639,7 +25639,7 @@
       </c>
     </row>
     <row r="17" spans="1:157" ht="15.75">
-      <c r="A17" s="598" t="s">
+      <c r="A17" s="600" t="s">
         <v>359</v>
       </c>
       <c r="B17" s="157" t="s">
@@ -25712,7 +25712,7 @@
       <c r="BO17" s="353"/>
     </row>
     <row r="18" spans="1:157" ht="15.75" customHeight="1">
-      <c r="A18" s="599"/>
+      <c r="A18" s="601"/>
       <c r="B18" s="73"/>
       <c r="C18" s="166" t="s">
         <v>71</v>
@@ -26179,7 +26179,7 @@
       </c>
     </row>
     <row r="19" spans="1:157">
-      <c r="A19" s="599"/>
+      <c r="A19" s="601"/>
       <c r="B19" s="73"/>
       <c r="C19" s="165" t="s">
         <v>3</v>
@@ -26646,7 +26646,7 @@
       </c>
     </row>
     <row r="20" spans="1:157">
-      <c r="A20" s="599"/>
+      <c r="A20" s="601"/>
       <c r="B20" s="73"/>
       <c r="C20" s="165" t="s">
         <v>35</v>
@@ -27113,7 +27113,7 @@
       </c>
     </row>
     <row r="21" spans="1:157" ht="15.75">
-      <c r="A21" s="599"/>
+      <c r="A21" s="601"/>
       <c r="B21" s="158" t="s">
         <v>127</v>
       </c>
@@ -27184,7 +27184,7 @@
       <c r="BO21" s="353"/>
     </row>
     <row r="22" spans="1:157" ht="15">
-      <c r="A22" s="599"/>
+      <c r="A22" s="601"/>
       <c r="B22" s="74"/>
       <c r="C22" s="165" t="s">
         <v>88</v>
@@ -27255,7 +27255,7 @@
       <c r="BO22" s="353"/>
     </row>
     <row r="23" spans="1:157" ht="15">
-      <c r="A23" s="599"/>
+      <c r="A23" s="601"/>
       <c r="B23" s="74"/>
       <c r="C23" s="165"/>
       <c r="D23" s="53" t="s">
@@ -27722,7 +27722,7 @@
       </c>
     </row>
     <row r="24" spans="1:157" ht="15">
-      <c r="A24" s="599"/>
+      <c r="A24" s="601"/>
       <c r="B24" s="74"/>
       <c r="C24" s="163"/>
       <c r="D24" s="53" t="s">
@@ -28189,7 +28189,7 @@
       </c>
     </row>
     <row r="25" spans="1:157" ht="15">
-      <c r="A25" s="599"/>
+      <c r="A25" s="601"/>
       <c r="B25" s="74"/>
       <c r="C25" s="163"/>
       <c r="D25" s="53" t="s">
@@ -28656,7 +28656,7 @@
       </c>
     </row>
     <row r="26" spans="1:157" ht="15">
-      <c r="A26" s="599"/>
+      <c r="A26" s="601"/>
       <c r="B26" s="74"/>
       <c r="C26" s="163"/>
       <c r="D26" s="53" t="s">
@@ -29123,7 +29123,7 @@
       </c>
     </row>
     <row r="27" spans="1:157" ht="15">
-      <c r="A27" s="599"/>
+      <c r="A27" s="601"/>
       <c r="B27" s="74"/>
       <c r="C27" s="165" t="s">
         <v>76</v>
@@ -29194,7 +29194,7 @@
       <c r="BO27" s="353"/>
     </row>
     <row r="28" spans="1:157" ht="15">
-      <c r="A28" s="599"/>
+      <c r="A28" s="601"/>
       <c r="B28" s="74"/>
       <c r="C28" s="165"/>
       <c r="D28" s="53" t="s">
@@ -29661,7 +29661,7 @@
       </c>
     </row>
     <row r="29" spans="1:157" ht="15">
-      <c r="A29" s="599"/>
+      <c r="A29" s="601"/>
       <c r="B29" s="74"/>
       <c r="C29" s="163"/>
       <c r="D29" s="53" t="s">
@@ -29753,7 +29753,7 @@
       <c r="BO29" s="353"/>
     </row>
     <row r="30" spans="1:157" ht="15">
-      <c r="A30" s="599"/>
+      <c r="A30" s="601"/>
       <c r="B30" s="74"/>
       <c r="C30" s="163"/>
       <c r="D30" s="53" t="s">
@@ -29845,7 +29845,7 @@
       <c r="BO30" s="353"/>
     </row>
     <row r="31" spans="1:157" ht="15">
-      <c r="A31" s="599"/>
+      <c r="A31" s="601"/>
       <c r="B31" s="74"/>
       <c r="C31" s="41"/>
       <c r="D31" s="53" t="s">
@@ -29937,7 +29937,7 @@
       <c r="BO31" s="353"/>
     </row>
     <row r="32" spans="1:157" ht="15">
-      <c r="A32" s="599"/>
+      <c r="A32" s="601"/>
       <c r="B32" s="74"/>
       <c r="C32" s="41"/>
       <c r="D32" s="53" t="s">
@@ -30405,7 +30405,7 @@
       <c r="FA32" s="353"/>
     </row>
     <row r="33" spans="1:156" ht="15">
-      <c r="A33" s="600"/>
+      <c r="A33" s="602"/>
       <c r="B33" s="79"/>
       <c r="C33" s="161"/>
       <c r="D33" s="81"/>
@@ -30870,7 +30870,7 @@
       </c>
     </row>
     <row r="34" spans="1:156" ht="15.75" customHeight="1">
-      <c r="A34" s="598" t="s">
+      <c r="A34" s="600" t="s">
         <v>360</v>
       </c>
       <c r="B34" s="175" t="s">
@@ -31341,7 +31341,7 @@
       </c>
     </row>
     <row r="35" spans="1:156" ht="15.75">
-      <c r="A35" s="599"/>
+      <c r="A35" s="601"/>
       <c r="B35" s="158" t="s">
         <v>129</v>
       </c>
@@ -31412,7 +31412,7 @@
       <c r="BO35" s="353"/>
     </row>
     <row r="36" spans="1:156" ht="15">
-      <c r="A36" s="599"/>
+      <c r="A36" s="601"/>
       <c r="B36" s="73"/>
       <c r="C36" s="124" t="s">
         <v>74</v>
@@ -31483,7 +31483,7 @@
       <c r="BO36" s="353"/>
     </row>
     <row r="37" spans="1:156">
-      <c r="A37" s="599"/>
+      <c r="A37" s="601"/>
       <c r="B37" s="73"/>
       <c r="C37" s="124"/>
       <c r="D37" s="73" t="s">
@@ -31950,7 +31950,7 @@
       </c>
     </row>
     <row r="38" spans="1:156">
-      <c r="A38" s="599"/>
+      <c r="A38" s="601"/>
       <c r="B38" s="73"/>
       <c r="C38" s="52"/>
       <c r="D38" s="53" t="s">
@@ -32043,7 +32043,7 @@
       </c>
     </row>
     <row r="39" spans="1:156">
-      <c r="A39" s="599"/>
+      <c r="A39" s="601"/>
       <c r="B39" s="73"/>
       <c r="C39" s="52"/>
       <c r="D39" s="53" t="s">
@@ -32510,7 +32510,7 @@
       </c>
     </row>
     <row r="40" spans="1:156">
-      <c r="A40" s="599"/>
+      <c r="A40" s="601"/>
       <c r="B40" s="73"/>
       <c r="C40" s="52"/>
       <c r="D40" s="53" t="s">
@@ -32977,7 +32977,7 @@
       </c>
     </row>
     <row r="41" spans="1:156" ht="15">
-      <c r="A41" s="599"/>
+      <c r="A41" s="601"/>
       <c r="B41" s="73"/>
       <c r="C41" s="124" t="s">
         <v>76</v>
@@ -33048,7 +33048,7 @@
       <c r="BO41" s="353"/>
     </row>
     <row r="42" spans="1:156" ht="15.75" customHeight="1">
-      <c r="A42" s="599"/>
+      <c r="A42" s="601"/>
       <c r="B42" s="73"/>
       <c r="C42" s="124"/>
       <c r="D42" s="73" t="s">
@@ -33515,7 +33515,7 @@
       </c>
     </row>
     <row r="43" spans="1:156">
-      <c r="A43" s="599"/>
+      <c r="A43" s="601"/>
       <c r="B43" s="73"/>
       <c r="C43" s="52"/>
       <c r="D43" s="53" t="s">
@@ -33982,7 +33982,7 @@
       </c>
     </row>
     <row r="44" spans="1:156">
-      <c r="A44" s="599"/>
+      <c r="A44" s="601"/>
       <c r="B44" s="73"/>
       <c r="C44" s="52"/>
       <c r="D44" s="53" t="s">
@@ -34078,7 +34078,7 @@
       </c>
     </row>
     <row r="45" spans="1:156" ht="15">
-      <c r="A45" s="599"/>
+      <c r="A45" s="601"/>
       <c r="B45" s="73"/>
       <c r="C45" s="46"/>
       <c r="D45" s="53" t="s">
@@ -34174,7 +34174,7 @@
       </c>
     </row>
     <row r="46" spans="1:156">
-      <c r="A46" s="600"/>
+      <c r="A46" s="602"/>
       <c r="B46" s="73"/>
       <c r="C46" s="52"/>
       <c r="D46" s="53" t="s">
@@ -42287,13 +42287,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C191" sqref="C191"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42301,7 +42301,7 @@
     <col min="1" max="1" width="10.42578125" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" style="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.7109375" style="34" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="583" customWidth="1"/>
+    <col min="4" max="4" width="139" style="583" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="34"/>
     <col min="6" max="6" width="3.28515625" style="34" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" style="34" customWidth="1"/>
@@ -42330,7 +42330,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="2" spans="1:8" s="552" customFormat="1">
       <c r="A2" s="550">
         <v>1</v>
       </c>
@@ -42352,7 +42352,7 @@
         <v>http://minutapiuriobranco.gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/04/PIU_RioBranco_ConsultaPublica_V03.pdf</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="3" spans="1:8" s="552" customFormat="1">
       <c r="A3" s="553">
         <v>1</v>
       </c>
@@ -42372,7 +42372,7 @@
         <v>http://minutapiuriobranco.gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/04/PIU_RioBranco_ConsultaPublica_ANEXOI_reduzido.pdf</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="4" spans="1:8" s="552" customFormat="1">
       <c r="A4" s="553">
         <v>1</v>
       </c>
@@ -42416,7 +42416,7 @@
         <v>http://minutapiuriobranco.gestaourbana.prefeitura.sp.gov.br/</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="6" spans="1:8" s="552" customFormat="1">
       <c r="A6" s="553">
         <v>1</v>
       </c>
@@ -42435,7 +42435,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/Contribui%C3%A7%C3%B5es.pdf</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="7" spans="1:8" s="552" customFormat="1">
       <c r="A7" s="553">
         <v>2</v>
       </c>
@@ -42454,7 +42454,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/01_-MIP_PIU_Vila-Leopoldina-Villa-Lobos_motiva%C3%A7%C3%A3o.pdf</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="8" spans="1:8" s="552" customFormat="1">
       <c r="A8" s="553">
         <v>2</v>
       </c>
@@ -42473,7 +42473,7 @@
         <v>http://minuta.gestaourbana.prefeitura.sp.gov.br/piu-leopoldina/wp-content/uploads/2016/08/02_MIP_PIU_Vila_Leopoldina-Villa-Lobos_diagnostico_e_programa.pdf</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="9" spans="1:8" s="552" customFormat="1">
       <c r="A9" s="553">
         <v>2</v>
       </c>
@@ -42492,7 +42492,7 @@
         <v>http://minuta.gestaourbana.prefeitura.sp.gov.br/piu-leopoldina/wp-content/uploads/2016/08/03_MIP_PIU_Vila_Leopoldina-Villa-Lobos_mapas.pdf</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="10" spans="1:8" s="552" customFormat="1">
       <c r="A10" s="553">
         <v>2</v>
       </c>
@@ -42530,7 +42530,7 @@
         <v>http://minuta.gestaourbana.prefeitura.sp.gov.br/piu-leopoldina/</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="12" spans="1:8" s="552" customFormat="1">
       <c r="A12" s="553">
         <v>2</v>
       </c>
@@ -42549,7 +42549,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/PIU-Leopoldina.pdf</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="13" spans="1:8" s="552" customFormat="1">
       <c r="A13" s="553">
         <v>2</v>
       </c>
@@ -42568,7 +42568,7 @@
         <v>print DOSP</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="14" spans="1:8" s="552" customFormat="1">
       <c r="A14" s="553">
         <v>2</v>
       </c>
@@ -42587,7 +42587,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/PIU_VL_AudienciaPublica_01_11_SPURB-2.pdf</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="15" spans="1:8" s="552" customFormat="1">
       <c r="A15" s="553">
         <v>2</v>
       </c>
@@ -42606,7 +42606,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/PIU_VL_AudienciaPublica_01_11_Proponente.pdf</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="16" spans="1:8" s="552" customFormat="1">
       <c r="A16" s="553">
         <v>2</v>
       </c>
@@ -42625,7 +42625,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/Lista-de-Presen%C3%A7a-Sem-contato.pdf</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="17" spans="1:8" s="552" customFormat="1">
       <c r="A17" s="553">
         <v>2</v>
       </c>
@@ -42660,7 +42660,7 @@
       <c r="G18" s="170"/>
       <c r="H18" s="563"/>
     </row>
-    <row r="19" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="19" spans="1:8" s="552" customFormat="1">
       <c r="A19" s="553">
         <v>2</v>
       </c>
@@ -42676,7 +42676,7 @@
       <c r="G19" s="170"/>
       <c r="H19" s="563"/>
     </row>
-    <row r="20" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="20" spans="1:8" s="552" customFormat="1">
       <c r="A20" s="553">
         <v>2</v>
       </c>
@@ -42692,7 +42692,7 @@
       <c r="G20" s="170"/>
       <c r="H20" s="563"/>
     </row>
-    <row r="21" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="21" spans="1:8" s="552" customFormat="1">
       <c r="A21" s="553">
         <v>2</v>
       </c>
@@ -42708,7 +42708,7 @@
       <c r="G21" s="170"/>
       <c r="H21" s="563"/>
     </row>
-    <row r="22" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="22" spans="1:8" s="552" customFormat="1">
       <c r="A22" s="553">
         <v>2</v>
       </c>
@@ -42724,7 +42724,7 @@
       <c r="G22" s="170"/>
       <c r="H22" s="563"/>
     </row>
-    <row r="23" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="23" spans="1:8" s="552" customFormat="1">
       <c r="A23" s="553">
         <v>2</v>
       </c>
@@ -42740,7 +42740,7 @@
       <c r="G23" s="170"/>
       <c r="H23" s="563"/>
     </row>
-    <row r="24" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="24" spans="1:8" s="552" customFormat="1">
       <c r="A24" s="553">
         <v>2</v>
       </c>
@@ -42756,7 +42756,7 @@
       <c r="G24" s="170"/>
       <c r="H24" s="563"/>
     </row>
-    <row r="25" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="25" spans="1:8" s="552" customFormat="1">
       <c r="A25" s="553">
         <v>2</v>
       </c>
@@ -42772,7 +42772,7 @@
       <c r="G25" s="170"/>
       <c r="H25" s="563"/>
     </row>
-    <row r="26" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="26" spans="1:8" s="552" customFormat="1">
       <c r="A26" s="559">
         <v>3</v>
       </c>
@@ -42789,7 +42789,7 @@
       <c r="G26" s="170"/>
       <c r="H26" s="564"/>
     </row>
-    <row r="27" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="27" spans="1:8" s="552" customFormat="1">
       <c r="A27" s="559">
         <v>3</v>
       </c>
@@ -42806,7 +42806,7 @@
       <c r="G27" s="170"/>
       <c r="H27" s="564"/>
     </row>
-    <row r="28" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="28" spans="1:8" s="552" customFormat="1">
       <c r="A28" s="559">
         <v>3</v>
       </c>
@@ -42823,7 +42823,7 @@
       <c r="G28" s="170"/>
       <c r="H28" s="564"/>
     </row>
-    <row r="29" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="29" spans="1:8" s="552" customFormat="1">
       <c r="A29" s="559">
         <v>3</v>
       </c>
@@ -42840,7 +42840,7 @@
       <c r="G29" s="170"/>
       <c r="H29" s="564"/>
     </row>
-    <row r="30" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="30" spans="1:8" s="552" customFormat="1">
       <c r="A30" s="559">
         <v>3</v>
       </c>
@@ -42857,7 +42857,7 @@
       <c r="G30" s="170"/>
       <c r="H30" s="564"/>
     </row>
-    <row r="31" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="31" spans="1:8" s="552" customFormat="1">
       <c r="A31" s="559">
         <v>3</v>
       </c>
@@ -42874,7 +42874,7 @@
       <c r="G31" s="170"/>
       <c r="H31" s="564"/>
     </row>
-    <row r="32" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="32" spans="1:8" s="552" customFormat="1">
       <c r="A32" s="559">
         <v>3</v>
       </c>
@@ -42891,7 +42891,7 @@
       <c r="G32" s="170"/>
       <c r="H32" s="564"/>
     </row>
-    <row r="33" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="33" spans="1:8" s="552" customFormat="1">
       <c r="A33" s="559">
         <v>3</v>
       </c>
@@ -42908,7 +42908,7 @@
       <c r="G33" s="170"/>
       <c r="H33" s="564"/>
     </row>
-    <row r="34" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="34" spans="1:8" s="552" customFormat="1">
       <c r="A34" s="559">
         <v>3</v>
       </c>
@@ -42925,7 +42925,7 @@
       <c r="G34" s="170"/>
       <c r="H34" s="564"/>
     </row>
-    <row r="35" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="35" spans="1:8" s="552" customFormat="1">
       <c r="A35" s="559">
         <v>3</v>
       </c>
@@ -42942,7 +42942,7 @@
       <c r="G35" s="170"/>
       <c r="H35" s="564"/>
     </row>
-    <row r="36" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="36" spans="1:8" s="552" customFormat="1">
       <c r="A36" s="559">
         <v>3</v>
       </c>
@@ -42959,7 +42959,7 @@
       <c r="G36" s="170"/>
       <c r="H36" s="564"/>
     </row>
-    <row r="37" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="37" spans="1:8" s="552" customFormat="1">
       <c r="A37" s="559">
         <v>3</v>
       </c>
@@ -42976,7 +42976,7 @@
       <c r="G37" s="170"/>
       <c r="H37" s="564"/>
     </row>
-    <row r="38" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="38" spans="1:8" s="552" customFormat="1">
       <c r="A38" s="559">
         <v>3</v>
       </c>
@@ -42993,7 +42993,7 @@
       <c r="G38" s="170"/>
       <c r="H38" s="564"/>
     </row>
-    <row r="39" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="39" spans="1:8" s="552" customFormat="1">
       <c r="A39" s="559">
         <v>3</v>
       </c>
@@ -43010,7 +43010,7 @@
       <c r="G39" s="170"/>
       <c r="H39" s="564"/>
     </row>
-    <row r="40" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="40" spans="1:8" s="552" customFormat="1">
       <c r="A40" s="559">
         <v>3</v>
       </c>
@@ -43027,7 +43027,7 @@
       <c r="G40" s="170"/>
       <c r="H40" s="564"/>
     </row>
-    <row r="41" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="41" spans="1:8" s="552" customFormat="1">
       <c r="A41" s="559">
         <v>3</v>
       </c>
@@ -43044,7 +43044,7 @@
       <c r="G41" s="170"/>
       <c r="H41" s="564"/>
     </row>
-    <row r="42" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="42" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A42" s="559">
         <v>3</v>
       </c>
@@ -43061,7 +43061,7 @@
       <c r="G42" s="170"/>
       <c r="H42" s="564"/>
     </row>
-    <row r="43" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="43" spans="1:8" s="552" customFormat="1">
       <c r="A43" s="559">
         <v>3</v>
       </c>
@@ -43078,7 +43078,7 @@
       <c r="G43" s="170"/>
       <c r="H43" s="564"/>
     </row>
-    <row r="44" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="44" spans="1:8" s="552" customFormat="1">
       <c r="A44" s="559">
         <v>3</v>
       </c>
@@ -43095,7 +43095,7 @@
       <c r="G44" s="170"/>
       <c r="H44" s="564"/>
     </row>
-    <row r="45" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="45" spans="1:8" s="552" customFormat="1">
       <c r="A45" s="559">
         <v>3</v>
       </c>
@@ -43112,7 +43112,7 @@
       <c r="G45" s="170"/>
       <c r="H45" s="564"/>
     </row>
-    <row r="46" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="46" spans="1:8" s="552" customFormat="1">
       <c r="A46" s="559">
         <v>3</v>
       </c>
@@ -43129,7 +43129,7 @@
       <c r="G46" s="170"/>
       <c r="H46" s="564"/>
     </row>
-    <row r="47" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="47" spans="1:8" s="552" customFormat="1">
       <c r="A47" s="559">
         <v>3</v>
       </c>
@@ -43146,7 +43146,7 @@
       <c r="G47" s="170"/>
       <c r="H47" s="564"/>
     </row>
-    <row r="48" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="48" spans="1:8" s="552" customFormat="1">
       <c r="A48" s="559">
         <v>3</v>
       </c>
@@ -43163,7 +43163,7 @@
       <c r="G48" s="170"/>
       <c r="H48" s="564"/>
     </row>
-    <row r="49" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="49" spans="1:8" s="552" customFormat="1">
       <c r="A49" s="559">
         <v>3</v>
       </c>
@@ -43180,7 +43180,7 @@
       <c r="G49" s="170"/>
       <c r="H49" s="564"/>
     </row>
-    <row r="50" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="50" spans="1:8" s="552" customFormat="1">
       <c r="A50" s="559"/>
       <c r="B50" s="559">
         <v>1</v>
@@ -43195,7 +43195,7 @@
       <c r="G50" s="170"/>
       <c r="H50" s="564"/>
     </row>
-    <row r="51" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="51" spans="1:8" s="552" customFormat="1">
       <c r="A51" s="559">
         <v>3</v>
       </c>
@@ -43212,7 +43212,7 @@
       <c r="G51" s="170"/>
       <c r="H51" s="564"/>
     </row>
-    <row r="52" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="52" spans="1:8" s="552" customFormat="1">
       <c r="A52" s="559">
         <v>3</v>
       </c>
@@ -43229,7 +43229,7 @@
       <c r="G52" s="170"/>
       <c r="H52" s="564"/>
     </row>
-    <row r="53" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="53" spans="1:8" s="552" customFormat="1">
       <c r="A53" s="559">
         <v>3</v>
       </c>
@@ -43246,7 +43246,7 @@
       <c r="G53" s="170"/>
       <c r="H53" s="564"/>
     </row>
-    <row r="54" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="54" spans="1:8" s="552" customFormat="1">
       <c r="A54" s="559">
         <v>3</v>
       </c>
@@ -43263,7 +43263,7 @@
       <c r="G54" s="170"/>
       <c r="H54" s="564"/>
     </row>
-    <row r="55" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="55" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A55" s="559">
         <v>3</v>
       </c>
@@ -43280,7 +43280,7 @@
       <c r="G55" s="170"/>
       <c r="H55" s="564"/>
     </row>
-    <row r="56" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="56" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A56" s="559">
         <v>3</v>
       </c>
@@ -43297,7 +43297,7 @@
       <c r="G56" s="170"/>
       <c r="H56" s="564"/>
     </row>
-    <row r="57" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="57" spans="1:8" s="552" customFormat="1">
       <c r="A57" s="559">
         <v>3</v>
       </c>
@@ -43314,7 +43314,7 @@
       <c r="G57" s="170"/>
       <c r="H57" s="564"/>
     </row>
-    <row r="58" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="58" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A58" s="559">
         <v>3</v>
       </c>
@@ -43331,7 +43331,7 @@
       <c r="G58" s="170"/>
       <c r="H58" s="564"/>
     </row>
-    <row r="59" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="59" spans="1:8" s="552" customFormat="1">
       <c r="A59" s="559">
         <v>3</v>
       </c>
@@ -43348,7 +43348,7 @@
       <c r="G59" s="170"/>
       <c r="H59" s="564"/>
     </row>
-    <row r="60" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="60" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A60" s="559">
         <v>3</v>
       </c>
@@ -43365,7 +43365,7 @@
       <c r="G60" s="170"/>
       <c r="H60" s="564"/>
     </row>
-    <row r="61" spans="1:8" s="552" customFormat="1" ht="38.25" hidden="1">
+    <row r="61" spans="1:8" s="552" customFormat="1" ht="38.25">
       <c r="A61" s="559">
         <v>3</v>
       </c>
@@ -43382,7 +43382,7 @@
       <c r="G61" s="170"/>
       <c r="H61" s="564"/>
     </row>
-    <row r="62" spans="1:8" s="552" customFormat="1" ht="38.25" hidden="1">
+    <row r="62" spans="1:8" s="552" customFormat="1" ht="38.25">
       <c r="A62" s="559">
         <v>3</v>
       </c>
@@ -43399,7 +43399,7 @@
       <c r="G62" s="170"/>
       <c r="H62" s="564"/>
     </row>
-    <row r="63" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="63" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A63" s="559">
         <v>3</v>
       </c>
@@ -43416,7 +43416,7 @@
       <c r="G63" s="170"/>
       <c r="H63" s="564"/>
     </row>
-    <row r="64" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="64" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A64" s="559">
         <v>3</v>
       </c>
@@ -43433,7 +43433,7 @@
       <c r="G64" s="170"/>
       <c r="H64" s="564"/>
     </row>
-    <row r="65" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="65" spans="1:8" s="552" customFormat="1">
       <c r="A65" s="559">
         <v>3</v>
       </c>
@@ -43450,7 +43450,7 @@
       <c r="G65" s="170"/>
       <c r="H65" s="564"/>
     </row>
-    <row r="66" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="66" spans="1:8" s="552" customFormat="1">
       <c r="A66" s="559">
         <v>3</v>
       </c>
@@ -43467,7 +43467,7 @@
       <c r="G66" s="170"/>
       <c r="H66" s="564"/>
     </row>
-    <row r="67" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="67" spans="1:8" s="552" customFormat="1">
       <c r="A67" s="559">
         <v>3</v>
       </c>
@@ -43484,7 +43484,7 @@
       <c r="G67" s="170"/>
       <c r="H67" s="564"/>
     </row>
-    <row r="68" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="68" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A68" s="559">
         <v>3</v>
       </c>
@@ -43501,7 +43501,7 @@
       <c r="G68" s="170"/>
       <c r="H68" s="564"/>
     </row>
-    <row r="69" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="69" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A69" s="559">
         <v>3</v>
       </c>
@@ -43518,7 +43518,7 @@
       <c r="G69" s="170"/>
       <c r="H69" s="564"/>
     </row>
-    <row r="70" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="70" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A70" s="559">
         <v>3</v>
       </c>
@@ -43535,7 +43535,7 @@
       <c r="G70" s="170"/>
       <c r="H70" s="564"/>
     </row>
-    <row r="71" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="71" spans="1:8" s="552" customFormat="1">
       <c r="A71" s="559">
         <v>3</v>
       </c>
@@ -43552,7 +43552,7 @@
       <c r="G71" s="170"/>
       <c r="H71" s="564"/>
     </row>
-    <row r="72" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="72" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A72" s="559">
         <v>3</v>
       </c>
@@ -43569,7 +43569,7 @@
       <c r="G72" s="170"/>
       <c r="H72" s="564"/>
     </row>
-    <row r="73" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="73" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A73" s="559">
         <v>3</v>
       </c>
@@ -43586,12 +43586,12 @@
       <c r="G73" s="170"/>
       <c r="H73" s="564"/>
     </row>
-    <row r="74" spans="1:8" s="552" customFormat="1" ht="25.5" hidden="1">
+    <row r="74" spans="1:8" s="552" customFormat="1" ht="25.5">
       <c r="A74" s="557">
         <v>3</v>
       </c>
-      <c r="B74" s="557" t="s">
-        <v>353</v>
+      <c r="B74" s="557">
+        <v>0</v>
       </c>
       <c r="C74" s="574" t="s">
         <v>827</v>
@@ -43602,12 +43602,12 @@
       <c r="G74" s="170"/>
       <c r="H74" s="564"/>
     </row>
-    <row r="75" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="75" spans="1:8" s="552" customFormat="1">
       <c r="A75" s="557">
         <v>3</v>
       </c>
-      <c r="B75" s="557" t="s">
-        <v>41</v>
+      <c r="B75" s="557">
+        <v>0</v>
       </c>
       <c r="C75" s="574" t="s">
         <v>828</v>
@@ -43618,12 +43618,12 @@
       <c r="G75" s="170"/>
       <c r="H75" s="564"/>
     </row>
-    <row r="76" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="76" spans="1:8" s="552" customFormat="1">
       <c r="A76" s="557">
         <v>3</v>
       </c>
-      <c r="B76" s="557" t="s">
-        <v>41</v>
+      <c r="B76" s="557">
+        <v>0</v>
       </c>
       <c r="C76" s="574" t="s">
         <v>829</v>
@@ -43634,7 +43634,7 @@
       <c r="G76" s="170"/>
       <c r="H76" s="564"/>
     </row>
-    <row r="77" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="77" spans="1:8" s="552" customFormat="1">
       <c r="A77" s="559">
         <v>3</v>
       </c>
@@ -43650,7 +43650,7 @@
       <c r="G77" s="170"/>
       <c r="H77" s="564"/>
     </row>
-    <row r="78" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="78" spans="1:8" s="552" customFormat="1">
       <c r="A78" s="559">
         <v>3</v>
       </c>
@@ -43666,7 +43666,7 @@
       <c r="G78" s="170"/>
       <c r="H78" s="564"/>
     </row>
-    <row r="79" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="79" spans="1:8" s="552" customFormat="1">
       <c r="A79" s="559">
         <v>3</v>
       </c>
@@ -43682,7 +43682,7 @@
       <c r="G79" s="170"/>
       <c r="H79" s="564"/>
     </row>
-    <row r="80" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="80" spans="1:8" s="552" customFormat="1">
       <c r="A80" s="559">
         <v>3</v>
       </c>
@@ -43698,7 +43698,7 @@
       <c r="G80" s="170"/>
       <c r="H80" s="564"/>
     </row>
-    <row r="81" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="81" spans="1:8" s="552" customFormat="1">
       <c r="A81" s="553">
         <v>3</v>
       </c>
@@ -43714,7 +43714,7 @@
       <c r="G81" s="170"/>
       <c r="H81" s="563"/>
     </row>
-    <row r="82" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="82" spans="1:8" s="552" customFormat="1">
       <c r="A82" s="553">
         <v>3</v>
       </c>
@@ -43730,7 +43730,7 @@
       <c r="G82" s="170"/>
       <c r="H82" s="563"/>
     </row>
-    <row r="83" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="83" spans="1:8" s="552" customFormat="1">
       <c r="A83" s="553">
         <v>3</v>
       </c>
@@ -43746,7 +43746,7 @@
       <c r="G83" s="170"/>
       <c r="H83" s="563"/>
     </row>
-    <row r="84" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="84" spans="1:8" s="552" customFormat="1">
       <c r="A84" s="553">
         <v>3</v>
       </c>
@@ -43762,7 +43762,7 @@
       <c r="G84" s="170"/>
       <c r="H84" s="563"/>
     </row>
-    <row r="85" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="85" spans="1:8" s="552" customFormat="1">
       <c r="A85" s="553">
         <v>3</v>
       </c>
@@ -43778,7 +43778,7 @@
       <c r="G85" s="170"/>
       <c r="H85" s="563"/>
     </row>
-    <row r="86" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="86" spans="1:8" s="552" customFormat="1">
       <c r="A86" s="553">
         <v>3</v>
       </c>
@@ -43794,7 +43794,7 @@
       <c r="G86" s="170"/>
       <c r="H86" s="563"/>
     </row>
-    <row r="87" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="87" spans="1:8" s="552" customFormat="1">
       <c r="A87" s="553">
         <v>3</v>
       </c>
@@ -43810,7 +43810,7 @@
       <c r="G87" s="170"/>
       <c r="H87" s="563"/>
     </row>
-    <row r="88" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="88" spans="1:8" s="552" customFormat="1">
       <c r="A88" s="553">
         <v>3</v>
       </c>
@@ -43826,7 +43826,7 @@
       <c r="G88" s="170"/>
       <c r="H88" s="563"/>
     </row>
-    <row r="89" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="89" spans="1:8" s="552" customFormat="1">
       <c r="A89" s="553">
         <v>3</v>
       </c>
@@ -43842,7 +43842,7 @@
       <c r="G89" s="170"/>
       <c r="H89" s="563"/>
     </row>
-    <row r="90" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="90" spans="1:8" s="552" customFormat="1">
       <c r="A90" s="553">
         <v>3</v>
       </c>
@@ -43858,7 +43858,7 @@
       <c r="G90" s="170"/>
       <c r="H90" s="563"/>
     </row>
-    <row r="91" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="91" spans="1:8" s="552" customFormat="1">
       <c r="A91" s="553">
         <v>3</v>
       </c>
@@ -43874,7 +43874,7 @@
       <c r="G91" s="170"/>
       <c r="H91" s="563"/>
     </row>
-    <row r="92" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="92" spans="1:8" s="552" customFormat="1">
       <c r="A92" s="553">
         <v>3</v>
       </c>
@@ -43890,7 +43890,7 @@
       <c r="G92" s="170"/>
       <c r="H92" s="563"/>
     </row>
-    <row r="93" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="93" spans="1:8" s="552" customFormat="1">
       <c r="A93" s="553">
         <v>3</v>
       </c>
@@ -43906,7 +43906,7 @@
       <c r="G93" s="170"/>
       <c r="H93" s="563"/>
     </row>
-    <row r="94" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="94" spans="1:8" s="552" customFormat="1">
       <c r="A94" s="553">
         <v>3</v>
       </c>
@@ -43922,7 +43922,7 @@
       <c r="G94" s="170"/>
       <c r="H94" s="563"/>
     </row>
-    <row r="95" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="95" spans="1:8" s="552" customFormat="1">
       <c r="A95" s="553">
         <v>3</v>
       </c>
@@ -43938,7 +43938,7 @@
       <c r="G95" s="170"/>
       <c r="H95" s="563"/>
     </row>
-    <row r="96" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="96" spans="1:8" s="552" customFormat="1">
       <c r="A96" s="553">
         <v>3</v>
       </c>
@@ -43954,7 +43954,7 @@
       <c r="G96" s="170"/>
       <c r="H96" s="563"/>
     </row>
-    <row r="97" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="97" spans="1:8" s="552" customFormat="1">
       <c r="A97" s="553">
         <v>3</v>
       </c>
@@ -43970,7 +43970,7 @@
       <c r="G97" s="170"/>
       <c r="H97" s="563"/>
     </row>
-    <row r="98" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="98" spans="1:8" s="552" customFormat="1">
       <c r="A98" s="553">
         <v>3</v>
       </c>
@@ -43986,7 +43986,7 @@
       <c r="G98" s="170"/>
       <c r="H98" s="563"/>
     </row>
-    <row r="99" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="99" spans="1:8" s="552" customFormat="1">
       <c r="A99" s="559">
         <v>3</v>
       </c>
@@ -44002,7 +44002,7 @@
       <c r="G99" s="170"/>
       <c r="H99" s="564"/>
     </row>
-    <row r="100" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="100" spans="1:8" s="552" customFormat="1">
       <c r="A100" s="559">
         <v>3</v>
       </c>
@@ -44018,7 +44018,7 @@
       <c r="G100" s="170"/>
       <c r="H100" s="564"/>
     </row>
-    <row r="101" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="101" spans="1:8" s="552" customFormat="1">
       <c r="A101" s="559">
         <v>3</v>
       </c>
@@ -44034,7 +44034,7 @@
       <c r="G101" s="170"/>
       <c r="H101" s="564"/>
     </row>
-    <row r="102" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="102" spans="1:8" s="552" customFormat="1">
       <c r="A102" s="559">
         <v>3</v>
       </c>
@@ -44050,7 +44050,7 @@
       <c r="G102" s="170"/>
       <c r="H102" s="564"/>
     </row>
-    <row r="103" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="103" spans="1:8" s="552" customFormat="1">
       <c r="A103" s="553">
         <v>4</v>
       </c>
@@ -44069,7 +44069,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/PIU_NESP_REQUERIMENTO-1.pdf</v>
       </c>
     </row>
-    <row r="104" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="104" spans="1:8" s="552" customFormat="1">
       <c r="A104" s="553">
         <v>4</v>
       </c>
@@ -44088,7 +44088,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/PIU_NESP_DIAGN%C3%93STICO-1.pdf</v>
       </c>
     </row>
-    <row r="105" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="105" spans="1:8" s="552" customFormat="1">
       <c r="A105" s="553">
         <v>4</v>
       </c>
@@ -44107,7 +44107,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/PIU_NESP_PER%C3%8DMETRO-1.pdf</v>
       </c>
     </row>
-    <row r="106" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="106" spans="1:8" s="552" customFormat="1">
       <c r="A106" s="553">
         <v>4</v>
       </c>
@@ -44145,7 +44145,7 @@
         <v>http://minuta.gestaourbana.prefeitura.sp.gov.br/piunesp/</v>
       </c>
     </row>
-    <row r="108" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="108" spans="1:8" s="552" customFormat="1">
       <c r="A108" s="553">
         <v>4</v>
       </c>
@@ -44164,7 +44164,7 @@
         <v>print DOSP</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="109" spans="1:8" s="552" customFormat="1">
       <c r="A109" s="553">
         <v>4</v>
       </c>
@@ -44183,7 +44183,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/NESP_apresentacao_2016_08_27.pdf</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="110" spans="1:8" s="552" customFormat="1">
       <c r="A110" s="553">
         <v>4</v>
       </c>
@@ -44202,7 +44202,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/NESP_lista_presenca_2016_08_27-3.pdf</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="111" spans="1:8" s="552" customFormat="1">
       <c r="A111" s="553">
         <v>4</v>
       </c>
@@ -44221,7 +44221,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/NESP_ata_2016_08_27.pdf</v>
       </c>
     </row>
-    <row r="112" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="112" spans="1:8" s="552" customFormat="1">
       <c r="A112" s="553">
         <v>4</v>
       </c>
@@ -44240,7 +44240,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/NESP_contribuicoes_2016_08_27.pdf</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="113" spans="1:8" s="552" customFormat="1">
       <c r="A113" s="553">
         <v>4</v>
       </c>
@@ -44259,7 +44259,7 @@
         <v>print DOSP</v>
       </c>
     </row>
-    <row r="114" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="114" spans="1:8" s="552" customFormat="1">
       <c r="A114" s="553">
         <v>4</v>
       </c>
@@ -44278,7 +44278,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/NESP_apresentacao_2016_08_27.pdf</v>
       </c>
     </row>
-    <row r="115" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="115" spans="1:8" s="552" customFormat="1">
       <c r="A115" s="553">
         <v>4</v>
       </c>
@@ -44297,7 +44297,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/NESP_ata_2016_08_27.pdf</v>
       </c>
     </row>
-    <row r="116" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="116" spans="1:8" s="552" customFormat="1">
       <c r="A116" s="553">
         <v>4</v>
       </c>
@@ -44316,7 +44316,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/03/PIU-NESP-Relat%C3%B3rio-Final_161215_reduzido.pdf</v>
       </c>
     </row>
-    <row r="117" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="117" spans="1:8" s="552" customFormat="1">
       <c r="A117" s="553">
         <v>4</v>
       </c>
@@ -44335,7 +44335,7 @@
         <v xml:space="preserve">http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/12/DECRETO-N%C2%BA-57569.pdf </v>
       </c>
     </row>
-    <row r="118" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="118" spans="1:8" s="552" customFormat="1">
       <c r="A118" s="553">
         <v>4</v>
       </c>
@@ -44354,7 +44354,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/12/mapa-e-quadros.pdf</v>
       </c>
     </row>
-    <row r="119" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="119" spans="1:8" s="552" customFormat="1">
       <c r="A119" s="553">
         <v>5</v>
       </c>
@@ -44370,7 +44370,7 @@
       <c r="G119" s="170"/>
       <c r="H119" s="565"/>
     </row>
-    <row r="120" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="120" spans="1:8" s="552" customFormat="1">
       <c r="A120" s="553">
         <v>5</v>
       </c>
@@ -44386,7 +44386,7 @@
       <c r="G120" s="170"/>
       <c r="H120" s="565"/>
     </row>
-    <row r="121" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="121" spans="1:8" s="552" customFormat="1">
       <c r="A121" s="553">
         <v>5</v>
       </c>
@@ -44402,7 +44402,7 @@
       <c r="G121" s="170"/>
       <c r="H121" s="566"/>
     </row>
-    <row r="122" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="122" spans="1:8" s="552" customFormat="1">
       <c r="A122" s="553">
         <v>5</v>
       </c>
@@ -44418,7 +44418,7 @@
       <c r="G122" s="170"/>
       <c r="H122" s="566"/>
     </row>
-    <row r="123" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="123" spans="1:8" s="552" customFormat="1">
       <c r="A123" s="553">
         <v>5</v>
       </c>
@@ -44434,7 +44434,7 @@
       <c r="G123" s="170"/>
       <c r="H123" s="566"/>
     </row>
-    <row r="124" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="124" spans="1:8" s="552" customFormat="1">
       <c r="A124" s="553">
         <v>5</v>
       </c>
@@ -44450,7 +44450,7 @@
       <c r="G124" s="170"/>
       <c r="H124" s="566"/>
     </row>
-    <row r="125" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="125" spans="1:8" s="552" customFormat="1">
       <c r="A125" s="553">
         <v>5</v>
       </c>
@@ -44466,7 +44466,7 @@
       <c r="G125" s="170"/>
       <c r="H125" s="566"/>
     </row>
-    <row r="126" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="126" spans="1:8" s="552" customFormat="1">
       <c r="A126" s="553">
         <v>5</v>
       </c>
@@ -44482,7 +44482,7 @@
       <c r="G126" s="170"/>
       <c r="H126" s="566"/>
     </row>
-    <row r="127" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="127" spans="1:8" s="552" customFormat="1">
       <c r="A127" s="553">
         <v>5</v>
       </c>
@@ -44498,7 +44498,7 @@
       <c r="G127" s="170"/>
       <c r="H127" s="566"/>
     </row>
-    <row r="128" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="128" spans="1:8" s="552" customFormat="1">
       <c r="A128" s="553">
         <v>5</v>
       </c>
@@ -44514,7 +44514,7 @@
       <c r="G128" s="170"/>
       <c r="H128" s="566"/>
     </row>
-    <row r="129" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="129" spans="1:8" s="552" customFormat="1">
       <c r="A129" s="553">
         <v>5</v>
       </c>
@@ -44530,7 +44530,7 @@
       <c r="G129" s="170"/>
       <c r="H129" s="566"/>
     </row>
-    <row r="130" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="130" spans="1:8" s="552" customFormat="1">
       <c r="A130" s="553">
         <v>5</v>
       </c>
@@ -44546,7 +44546,7 @@
       <c r="G130" s="170"/>
       <c r="H130" s="566"/>
     </row>
-    <row r="131" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="131" spans="1:8" s="552" customFormat="1">
       <c r="A131" s="553">
         <v>5</v>
       </c>
@@ -44562,7 +44562,7 @@
       <c r="G131" s="170"/>
       <c r="H131" s="566"/>
     </row>
-    <row r="132" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="132" spans="1:8" s="552" customFormat="1">
       <c r="A132" s="553">
         <v>5</v>
       </c>
@@ -44578,7 +44578,7 @@
       <c r="G132" s="170"/>
       <c r="H132" s="566"/>
     </row>
-    <row r="133" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="133" spans="1:8" s="552" customFormat="1">
       <c r="A133" s="553">
         <v>5</v>
       </c>
@@ -44594,7 +44594,7 @@
       <c r="G133" s="170"/>
       <c r="H133" s="566"/>
     </row>
-    <row r="134" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="134" spans="1:8" s="552" customFormat="1">
       <c r="A134" s="553">
         <v>5</v>
       </c>
@@ -44610,7 +44610,7 @@
       <c r="G134" s="170"/>
       <c r="H134" s="566"/>
     </row>
-    <row r="135" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="135" spans="1:8" s="552" customFormat="1">
       <c r="A135" s="553">
         <v>5</v>
       </c>
@@ -44626,7 +44626,7 @@
       <c r="G135" s="170"/>
       <c r="H135" s="566"/>
     </row>
-    <row r="136" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="136" spans="1:8" s="552" customFormat="1">
       <c r="A136" s="553">
         <v>5</v>
       </c>
@@ -44642,7 +44642,7 @@
       <c r="G136" s="170"/>
       <c r="H136" s="566"/>
     </row>
-    <row r="137" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="137" spans="1:8" s="552" customFormat="1">
       <c r="A137" s="553">
         <v>5</v>
       </c>
@@ -44658,7 +44658,7 @@
       <c r="G137" s="170"/>
       <c r="H137" s="566"/>
     </row>
-    <row r="138" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="138" spans="1:8" s="552" customFormat="1">
       <c r="A138" s="553">
         <v>5</v>
       </c>
@@ -44674,7 +44674,7 @@
       <c r="G138" s="170"/>
       <c r="H138" s="566"/>
     </row>
-    <row r="139" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="139" spans="1:8" s="552" customFormat="1">
       <c r="A139" s="553">
         <v>5</v>
       </c>
@@ -44690,7 +44690,7 @@
       <c r="G139" s="170"/>
       <c r="H139" s="566"/>
     </row>
-    <row r="140" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="140" spans="1:8" s="552" customFormat="1">
       <c r="A140" s="553">
         <v>5</v>
       </c>
@@ -44720,7 +44720,7 @@
       </c>
       <c r="H141" s="567"/>
     </row>
-    <row r="142" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="142" spans="1:8" s="552" customFormat="1">
       <c r="A142" s="553">
         <v>5</v>
       </c>
@@ -44735,7 +44735,7 @@
       </c>
       <c r="H142" s="567"/>
     </row>
-    <row r="143" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="143" spans="1:8" s="552" customFormat="1">
       <c r="A143" s="553">
         <v>5</v>
       </c>
@@ -44750,7 +44750,7 @@
       </c>
       <c r="H143" s="567"/>
     </row>
-    <row r="144" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="144" spans="1:8" s="552" customFormat="1">
       <c r="A144" s="553">
         <v>5</v>
       </c>
@@ -44765,7 +44765,7 @@
       </c>
       <c r="H144" s="567"/>
     </row>
-    <row r="145" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="145" spans="1:8" s="552" customFormat="1">
       <c r="A145" s="553">
         <v>5</v>
       </c>
@@ -44795,7 +44795,7 @@
       </c>
       <c r="H146" s="567"/>
     </row>
-    <row r="147" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="147" spans="1:8" s="552" customFormat="1">
       <c r="A147" s="553">
         <v>5</v>
       </c>
@@ -44810,7 +44810,7 @@
       </c>
       <c r="H147" s="567"/>
     </row>
-    <row r="148" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="148" spans="1:8" s="552" customFormat="1">
       <c r="A148" s="553">
         <v>5</v>
       </c>
@@ -44825,7 +44825,7 @@
       </c>
       <c r="H148" s="567"/>
     </row>
-    <row r="149" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="149" spans="1:8" s="552" customFormat="1">
       <c r="A149" s="553">
         <v>5</v>
       </c>
@@ -44840,7 +44840,7 @@
       </c>
       <c r="H149" s="567"/>
     </row>
-    <row r="150" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="150" spans="1:8" s="552" customFormat="1">
       <c r="A150" s="553">
         <v>5</v>
       </c>
@@ -44855,7 +44855,7 @@
       </c>
       <c r="H150" s="567"/>
     </row>
-    <row r="151" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="151" spans="1:8" s="552" customFormat="1">
       <c r="A151" s="553">
         <v>5</v>
       </c>
@@ -44870,7 +44870,7 @@
       </c>
       <c r="H151" s="567"/>
     </row>
-    <row r="152" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="152" spans="1:8" s="552" customFormat="1">
       <c r="A152" s="553">
         <v>5</v>
       </c>
@@ -44885,7 +44885,7 @@
       </c>
       <c r="H152" s="567"/>
     </row>
-    <row r="153" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="153" spans="1:8" s="552" customFormat="1">
       <c r="A153" s="553">
         <v>5</v>
       </c>
@@ -44900,7 +44900,7 @@
       </c>
       <c r="H153" s="567"/>
     </row>
-    <row r="154" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="154" spans="1:8" s="552" customFormat="1">
       <c r="A154" s="553">
         <v>5</v>
       </c>
@@ -44915,7 +44915,7 @@
       </c>
       <c r="H154" s="567"/>
     </row>
-    <row r="155" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="155" spans="1:8" s="552" customFormat="1">
       <c r="A155" s="553">
         <v>5</v>
       </c>
@@ -44975,7 +44975,7 @@
       </c>
       <c r="H158" s="567"/>
     </row>
-    <row r="159" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="159" spans="1:8" s="552" customFormat="1">
       <c r="A159" s="553">
         <v>6</v>
       </c>
@@ -44990,7 +44990,7 @@
       </c>
       <c r="H159" s="567"/>
     </row>
-    <row r="160" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="160" spans="1:8" s="552" customFormat="1">
       <c r="A160" s="553">
         <v>6</v>
       </c>
@@ -45065,7 +45065,7 @@
       </c>
       <c r="H164" s="567"/>
     </row>
-    <row r="165" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="165" spans="1:8" s="552" customFormat="1">
       <c r="A165" s="553">
         <v>6</v>
       </c>
@@ -45080,7 +45080,7 @@
       </c>
       <c r="H165" s="567"/>
     </row>
-    <row r="166" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="166" spans="1:8" s="552" customFormat="1">
       <c r="A166" s="553">
         <v>6</v>
       </c>
@@ -45095,7 +45095,7 @@
       </c>
       <c r="H166" s="567"/>
     </row>
-    <row r="167" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="167" spans="1:8" s="552" customFormat="1">
       <c r="A167" s="553">
         <v>6</v>
       </c>
@@ -45110,7 +45110,7 @@
       </c>
       <c r="H167" s="567"/>
     </row>
-    <row r="168" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="168" spans="1:8" s="552" customFormat="1">
       <c r="A168" s="553">
         <v>6</v>
       </c>
@@ -45125,7 +45125,7 @@
       </c>
       <c r="H168" s="567"/>
     </row>
-    <row r="169" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="169" spans="1:8" s="552" customFormat="1">
       <c r="A169" s="553">
         <v>6</v>
       </c>
@@ -45140,7 +45140,7 @@
       </c>
       <c r="H169" s="567"/>
     </row>
-    <row r="170" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="170" spans="1:8" s="552" customFormat="1">
       <c r="A170" s="553">
         <v>6</v>
       </c>
@@ -45155,7 +45155,7 @@
       </c>
       <c r="H170" s="567"/>
     </row>
-    <row r="171" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="171" spans="1:8" s="552" customFormat="1">
       <c r="A171" s="553">
         <v>6</v>
       </c>
@@ -45170,7 +45170,7 @@
       </c>
       <c r="H171" s="567"/>
     </row>
-    <row r="172" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="172" spans="1:8" s="552" customFormat="1">
       <c r="A172" s="553">
         <v>6</v>
       </c>
@@ -45185,7 +45185,7 @@
       </c>
       <c r="H172" s="567"/>
     </row>
-    <row r="173" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="173" spans="1:8" s="552" customFormat="1">
       <c r="A173" s="553">
         <v>6</v>
       </c>
@@ -45200,7 +45200,7 @@
       </c>
       <c r="H173" s="567"/>
     </row>
-    <row r="174" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="174" spans="1:8" s="552" customFormat="1">
       <c r="A174" s="553">
         <v>6</v>
       </c>
@@ -45215,7 +45215,7 @@
       </c>
       <c r="H174" s="567"/>
     </row>
-    <row r="175" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="175" spans="1:8" s="552" customFormat="1">
       <c r="A175" s="553">
         <v>6</v>
       </c>
@@ -45230,7 +45230,7 @@
       </c>
       <c r="H175" s="567"/>
     </row>
-    <row r="176" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="176" spans="1:8" s="552" customFormat="1">
       <c r="A176" s="553">
         <v>6</v>
       </c>
@@ -45245,7 +45245,7 @@
       </c>
       <c r="H176" s="567"/>
     </row>
-    <row r="177" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="177" spans="1:8" s="552" customFormat="1">
       <c r="A177" s="557">
         <v>6</v>
       </c>
@@ -45260,7 +45260,7 @@
       </c>
       <c r="H177" s="567"/>
     </row>
-    <row r="178" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="178" spans="1:8" s="552" customFormat="1">
       <c r="A178" s="553">
         <v>6</v>
       </c>
@@ -45275,7 +45275,7 @@
       </c>
       <c r="H178" s="567"/>
     </row>
-    <row r="179" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="179" spans="1:8" s="552" customFormat="1">
       <c r="A179" s="553">
         <v>6</v>
       </c>
@@ -45290,7 +45290,7 @@
       </c>
       <c r="H179" s="567"/>
     </row>
-    <row r="180" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="180" spans="1:8" s="552" customFormat="1">
       <c r="A180" s="553">
         <v>7</v>
       </c>
@@ -45326,7 +45326,7 @@
         <v>http://minuta.gestaourbana.prefeitura.sp.gov.br/piu-anhembi/</v>
       </c>
     </row>
-    <row r="182" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="182" spans="1:8" s="552" customFormat="1">
       <c r="A182" s="553">
         <v>7</v>
       </c>
@@ -45362,7 +45362,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/estruturacao-territorial/piu/piu-pacaembu/</v>
       </c>
     </row>
-    <row r="184" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="184" spans="1:8" s="552" customFormat="1">
       <c r="A184" s="553">
         <v>8</v>
       </c>
@@ -45380,7 +45380,7 @@
         <v>http://minuta.gestaourbana.prefeitura.sp.gov.br/piu-pacaembu/static/xls/piu-pacaembu_consulta_respostas_2018-02-08.zip</v>
       </c>
     </row>
-    <row r="185" spans="1:8" s="552" customFormat="1" hidden="1">
+    <row r="185" spans="1:8" s="552" customFormat="1">
       <c r="A185" s="553">
         <v>8</v>
       </c>
@@ -45416,7 +45416,7 @@
         <v>http://gestaourbana.prefeitura.sp.gov.br/estruturacao-territorial/piu/piu-pacaembu/</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1">
+    <row r="187" spans="1:8">
       <c r="A187" s="556">
         <v>9</v>
       </c>
@@ -45430,7 +45430,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1">
+    <row r="188" spans="1:8">
       <c r="A188" s="556">
         <v>9</v>
       </c>
@@ -45444,7 +45444,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1">
+    <row r="189" spans="1:8">
       <c r="A189" s="556">
         <v>9</v>
       </c>
@@ -45458,7 +45458,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1">
+    <row r="190" spans="1:8">
       <c r="A190" s="556">
         <v>9</v>
       </c>
@@ -45486,7 +45486,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1">
+    <row r="192" spans="1:8">
       <c r="A192" s="547">
         <v>10</v>
       </c>
@@ -45500,7 +45500,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="193" spans="1:4" hidden="1">
+    <row r="193" spans="1:4">
       <c r="A193" s="547">
         <v>10</v>
       </c>
@@ -45514,7 +45514,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="194" spans="1:4" hidden="1">
+    <row r="194" spans="1:4">
       <c r="A194" s="547">
         <v>10</v>
       </c>
@@ -45604,18 +45604,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D195">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Texto Consulta Pública - Terminal Campo Limpo"/>
-        <filter val="Texto Consulta Pública - Terminal Capelinha"/>
-        <filter val="Texto Consulta Pública - Terminal Princesa Isabel"/>
-        <filter val="Texto da Consulta Pública"/>
-        <filter val="Texto da Consulta Pública - Introdução"/>
-        <filter val="Texto da Consulta Pública - Terminal Campo Limpo"/>
-        <filter val="Texto da Consulta Pública - Terminal Capelinha"/>
-        <filter val="Texto da Consulta Pública - Terminal Princesa Isabel"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="2"/>
   </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="F4:G4"/>
@@ -45763,10 +45752,10 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="610"/>
-      <c r="B2" s="611"/>
-      <c r="C2" s="611"/>
-      <c r="D2" s="611"/>
+      <c r="A2" s="598"/>
+      <c r="B2" s="599"/>
+      <c r="C2" s="599"/>
+      <c r="D2" s="599"/>
       <c r="E2" s="58" t="s">
         <v>51</v>
       </c>
@@ -46692,18 +46681,18 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="610"/>
-      <c r="B3" s="611"/>
-      <c r="C3" s="611"/>
-      <c r="D3" s="611"/>
+      <c r="A3" s="598"/>
+      <c r="B3" s="599"/>
+      <c r="C3" s="599"/>
+      <c r="D3" s="599"/>
       <c r="E3" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="610" t="s">
+      <c r="F3" s="598" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="611"/>
-      <c r="H3" s="612"/>
+      <c r="G3" s="599"/>
+      <c r="H3" s="606"/>
       <c r="I3" s="61" t="s">
         <v>59</v>
       </c>
@@ -46739,11 +46728,11 @@
       </c>
       <c r="D5" s="74"/>
       <c r="E5" s="91"/>
-      <c r="F5" s="631" t="s">
+      <c r="F5" s="622" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="632"/>
-      <c r="H5" s="633"/>
+      <c r="G5" s="623"/>
+      <c r="H5" s="624"/>
       <c r="I5" s="91"/>
       <c r="J5" s="65"/>
       <c r="K5" s="65"/>
@@ -46756,11 +46745,11 @@
       </c>
       <c r="D6" s="92"/>
       <c r="E6" s="91"/>
-      <c r="F6" s="631" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="632"/>
-      <c r="H6" s="633"/>
+      <c r="F6" s="622" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="623"/>
+      <c r="H6" s="624"/>
       <c r="I6" s="91"/>
       <c r="J6" s="65"/>
       <c r="K6" s="65"/>
@@ -46773,11 +46762,11 @@
       </c>
       <c r="D7" s="75"/>
       <c r="E7" s="91"/>
-      <c r="F7" s="631" t="s">
+      <c r="F7" s="622" t="s">
         <v>96</v>
       </c>
-      <c r="G7" s="632"/>
-      <c r="H7" s="633"/>
+      <c r="G7" s="623"/>
+      <c r="H7" s="624"/>
       <c r="I7" s="91"/>
       <c r="J7" s="65"/>
       <c r="K7" s="65"/>
@@ -46790,11 +46779,11 @@
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="91"/>
-      <c r="F8" s="631" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="632"/>
-      <c r="H8" s="633"/>
+      <c r="F8" s="622" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="623"/>
+      <c r="H8" s="624"/>
       <c r="I8" s="91"/>
       <c r="J8" s="65"/>
       <c r="K8" s="65"/>
@@ -46807,11 +46796,11 @@
         <v>103</v>
       </c>
       <c r="E9" s="91"/>
-      <c r="F9" s="631" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="632"/>
-      <c r="H9" s="633"/>
+      <c r="F9" s="622" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="623"/>
+      <c r="H9" s="624"/>
       <c r="I9" s="91"/>
       <c r="J9" s="65"/>
       <c r="K9" s="65"/>
@@ -46854,11 +46843,11 @@
         <v>100</v>
       </c>
       <c r="E12" s="91"/>
-      <c r="F12" s="631" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="632"/>
-      <c r="H12" s="633"/>
+      <c r="F12" s="622" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="623"/>
+      <c r="H12" s="624"/>
       <c r="I12" s="91"/>
       <c r="J12" s="65"/>
       <c r="K12" s="65"/>
@@ -46871,11 +46860,11 @@
         <v>75</v>
       </c>
       <c r="E13" s="91"/>
-      <c r="F13" s="631" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="632"/>
-      <c r="H13" s="633"/>
+      <c r="F13" s="622" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="623"/>
+      <c r="H13" s="624"/>
       <c r="I13" s="91"/>
       <c r="J13" s="65"/>
       <c r="K13" s="65"/>
@@ -46888,11 +46877,11 @@
         <v>73</v>
       </c>
       <c r="E14" s="91"/>
-      <c r="F14" s="631" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="632"/>
-      <c r="H14" s="633"/>
+      <c r="F14" s="622" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="623"/>
+      <c r="H14" s="624"/>
       <c r="I14" s="91"/>
       <c r="J14" s="65"/>
       <c r="K14" s="65"/>
@@ -46905,11 +46894,11 @@
         <v>101</v>
       </c>
       <c r="E15" s="91"/>
-      <c r="F15" s="631" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="632"/>
-      <c r="H15" s="633"/>
+      <c r="F15" s="622" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="623"/>
+      <c r="H15" s="624"/>
       <c r="I15" s="91"/>
       <c r="J15" s="65"/>
       <c r="K15" s="65"/>
@@ -46937,11 +46926,11 @@
         <v>100</v>
       </c>
       <c r="E17" s="91"/>
-      <c r="F17" s="631" t="s">
+      <c r="F17" s="622" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="632"/>
-      <c r="H17" s="633"/>
+      <c r="G17" s="623"/>
+      <c r="H17" s="624"/>
       <c r="I17" s="91"/>
       <c r="J17" s="65"/>
       <c r="K17" s="65"/>
@@ -46954,11 +46943,11 @@
         <v>77</v>
       </c>
       <c r="E18" s="91"/>
-      <c r="F18" s="631" t="s">
+      <c r="F18" s="622" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="632"/>
-      <c r="H18" s="633"/>
+      <c r="G18" s="623"/>
+      <c r="H18" s="624"/>
       <c r="I18" s="91"/>
       <c r="J18" s="65"/>
       <c r="K18" s="65"/>
@@ -46971,11 +46960,11 @@
         <v>78</v>
       </c>
       <c r="E19" s="65"/>
-      <c r="F19" s="628" t="s">
+      <c r="F19" s="625" t="s">
         <v>91</v>
       </c>
-      <c r="G19" s="629"/>
-      <c r="H19" s="630"/>
+      <c r="G19" s="626"/>
+      <c r="H19" s="627"/>
       <c r="I19" s="65"/>
       <c r="J19" s="65"/>
       <c r="K19" s="65"/>
@@ -46988,11 +46977,11 @@
         <v>79</v>
       </c>
       <c r="E20" s="65"/>
-      <c r="F20" s="628" t="s">
+      <c r="F20" s="625" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="629"/>
-      <c r="H20" s="630"/>
+      <c r="G20" s="626"/>
+      <c r="H20" s="627"/>
       <c r="I20" s="65"/>
       <c r="J20" s="65"/>
       <c r="K20" s="65"/>
@@ -47005,11 +46994,11 @@
         <v>89</v>
       </c>
       <c r="E21" s="66"/>
-      <c r="F21" s="625" t="s">
+      <c r="F21" s="631" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="626"/>
-      <c r="H21" s="627"/>
+      <c r="G21" s="632"/>
+      <c r="H21" s="633"/>
       <c r="I21" s="66"/>
       <c r="J21" s="66"/>
       <c r="K21" s="66"/>
@@ -47039,11 +47028,11 @@
       </c>
       <c r="D23" s="53"/>
       <c r="E23" s="65"/>
-      <c r="F23" s="628" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="629"/>
-      <c r="H23" s="630"/>
+      <c r="F23" s="625" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="626"/>
+      <c r="H23" s="627"/>
       <c r="I23" s="65"/>
       <c r="J23" s="65"/>
       <c r="K23" s="65"/>
@@ -47056,11 +47045,11 @@
       </c>
       <c r="D24" s="53"/>
       <c r="E24" s="65"/>
-      <c r="F24" s="628" t="s">
+      <c r="F24" s="625" t="s">
         <v>96</v>
       </c>
-      <c r="G24" s="629"/>
-      <c r="H24" s="630"/>
+      <c r="G24" s="626"/>
+      <c r="H24" s="627"/>
       <c r="I24" s="65"/>
       <c r="J24" s="65"/>
       <c r="K24" s="65"/>
@@ -47073,11 +47062,11 @@
         <v>103</v>
       </c>
       <c r="E25" s="65"/>
-      <c r="F25" s="628" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="629"/>
-      <c r="H25" s="630"/>
+      <c r="F25" s="625" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="626"/>
+      <c r="H25" s="627"/>
       <c r="I25" s="65"/>
       <c r="J25" s="65"/>
       <c r="K25" s="65"/>
@@ -47090,11 +47079,11 @@
       </c>
       <c r="D26" s="53"/>
       <c r="E26" s="65"/>
-      <c r="F26" s="628" t="s">
+      <c r="F26" s="625" t="s">
         <v>96</v>
       </c>
-      <c r="G26" s="629"/>
-      <c r="H26" s="630"/>
+      <c r="G26" s="626"/>
+      <c r="H26" s="627"/>
       <c r="I26" s="65"/>
       <c r="J26" s="65"/>
       <c r="K26" s="65"/>
@@ -47107,11 +47096,11 @@
         <v>105</v>
       </c>
       <c r="E27" s="65"/>
-      <c r="F27" s="628" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="629"/>
-      <c r="H27" s="630"/>
+      <c r="F27" s="625" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="626"/>
+      <c r="H27" s="627"/>
       <c r="I27" s="65"/>
       <c r="J27" s="65"/>
       <c r="K27" s="65"/>
@@ -47124,11 +47113,11 @@
       </c>
       <c r="D28" s="100"/>
       <c r="E28" s="65"/>
-      <c r="F28" s="628" t="s">
+      <c r="F28" s="625" t="s">
         <v>64</v>
       </c>
-      <c r="G28" s="629"/>
-      <c r="H28" s="630"/>
+      <c r="G28" s="626"/>
+      <c r="H28" s="627"/>
       <c r="I28" s="65"/>
       <c r="J28" s="65"/>
       <c r="K28" s="65"/>
@@ -47171,11 +47160,11 @@
         <v>100</v>
       </c>
       <c r="E31" s="65"/>
-      <c r="F31" s="628" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="629"/>
-      <c r="H31" s="630"/>
+      <c r="F31" s="625" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="626"/>
+      <c r="H31" s="627"/>
       <c r="I31" s="65"/>
       <c r="J31" s="65"/>
       <c r="K31" s="65"/>
@@ -47188,11 +47177,11 @@
         <v>75</v>
       </c>
       <c r="E32" s="65"/>
-      <c r="F32" s="628" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="629"/>
-      <c r="H32" s="630"/>
+      <c r="F32" s="625" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="626"/>
+      <c r="H32" s="627"/>
       <c r="I32" s="65"/>
       <c r="J32" s="65"/>
       <c r="K32" s="65"/>
@@ -47205,11 +47194,11 @@
         <v>73</v>
       </c>
       <c r="E33" s="65"/>
-      <c r="F33" s="628" t="s">
+      <c r="F33" s="625" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="629"/>
-      <c r="H33" s="630"/>
+      <c r="G33" s="626"/>
+      <c r="H33" s="627"/>
       <c r="I33" s="65"/>
       <c r="J33" s="65"/>
       <c r="K33" s="65"/>
@@ -47355,9 +47344,9 @@
       <c r="C41" s="73"/>
       <c r="D41" s="53"/>
       <c r="E41" s="66"/>
-      <c r="F41" s="625"/>
-      <c r="G41" s="626"/>
-      <c r="H41" s="627"/>
+      <c r="F41" s="631"/>
+      <c r="G41" s="632"/>
+      <c r="H41" s="633"/>
       <c r="I41" s="66"/>
       <c r="J41" s="66"/>
       <c r="K41" s="66"/>
@@ -47372,9 +47361,9 @@
       <c r="C42" s="83"/>
       <c r="D42" s="55"/>
       <c r="E42" s="66"/>
-      <c r="F42" s="622"/>
-      <c r="G42" s="623"/>
-      <c r="H42" s="624"/>
+      <c r="F42" s="628"/>
+      <c r="G42" s="629"/>
+      <c r="H42" s="630"/>
       <c r="I42" s="66"/>
       <c r="J42" s="66"/>
       <c r="K42" s="66"/>
@@ -47435,6 +47424,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F23:H23"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A22:A41"/>
     <mergeCell ref="A4:A21"/>
@@ -47451,19 +47453,6 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F23:H23"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:D42">
     <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">

</xml_diff>

<commit_message>
View do Open Layers alterada pelo clickedId do Vue. Simplificacao de gulpfile
</commit_message>
<xml_diff>
--- a/PIUS_Doc_ParticipacaoPublica.xlsx
+++ b/PIUS_Doc_ParticipacaoPublica.xlsx
@@ -668,7 +668,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6170" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6170" uniqueCount="1001">
   <si>
     <t>DOCUMENTAÇÃO PIUS</t>
   </si>
@@ -3670,6 +3670,9 @@
   </si>
   <si>
     <t>resolver os que estão de vermelho</t>
+  </si>
+  <si>
+    <t>Diagnóstico olar</t>
   </si>
 </sst>
 </file>
@@ -6673,49 +6676,49 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6743,6 +6746,33 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6752,33 +6782,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -6836,15 +6839,81 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6863,71 +6932,17 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6952,18 +6967,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -8553,10 +8556,10 @@
       </c>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="598"/>
-      <c r="B2" s="599"/>
-      <c r="C2" s="599"/>
-      <c r="D2" s="599"/>
+      <c r="A2" s="610"/>
+      <c r="B2" s="611"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
       <c r="E2" s="548"/>
       <c r="F2" s="58" t="s">
         <v>51</v>
@@ -8598,11 +8601,11 @@
       <c r="T2" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="U2" s="599" t="s">
+      <c r="U2" s="611" t="s">
         <v>57</v>
       </c>
-      <c r="V2" s="599"/>
-      <c r="W2" s="606"/>
+      <c r="V2" s="611"/>
+      <c r="W2" s="612"/>
       <c r="X2" s="61" t="s">
         <v>59</v>
       </c>
@@ -8614,7 +8617,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="600" t="s">
+      <c r="A3" s="598" t="s">
         <v>358</v>
       </c>
       <c r="B3" s="157" t="s">
@@ -8645,7 +8648,7 @@
       <c r="Z3" s="52"/>
     </row>
     <row r="4" spans="1:26" ht="15">
-      <c r="A4" s="601"/>
+      <c r="A4" s="599"/>
       <c r="B4" s="74"/>
       <c r="C4" s="163" t="s">
         <v>116</v>
@@ -8674,7 +8677,7 @@
       <c r="Z4" s="52"/>
     </row>
     <row r="5" spans="1:26" ht="15">
-      <c r="A5" s="601"/>
+      <c r="A5" s="599"/>
       <c r="B5" s="74"/>
       <c r="D5" s="85" t="s">
         <v>81</v>
@@ -8714,17 +8717,17 @@
         <v>91</v>
       </c>
       <c r="T5" s="73"/>
-      <c r="U5" s="603" t="s">
+      <c r="U5" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="V5" s="604"/>
-      <c r="W5" s="605"/>
+      <c r="V5" s="602"/>
+      <c r="W5" s="603"/>
       <c r="X5" s="73"/>
       <c r="Y5" s="73"/>
       <c r="Z5" s="52"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="601"/>
+      <c r="A6" s="599"/>
       <c r="B6" s="73"/>
       <c r="C6" s="164" t="s">
         <v>117</v>
@@ -8754,7 +8757,7 @@
       <c r="Z6" s="52"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="601"/>
+      <c r="A7" s="599"/>
       <c r="B7" s="73"/>
       <c r="C7" s="164"/>
       <c r="D7" s="85" t="s">
@@ -8794,17 +8797,17 @@
       </c>
       <c r="S7" s="76"/>
       <c r="T7" s="73"/>
-      <c r="U7" s="603" t="s">
+      <c r="U7" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="V7" s="604"/>
-      <c r="W7" s="605"/>
+      <c r="V7" s="602"/>
+      <c r="W7" s="603"/>
       <c r="X7" s="73"/>
       <c r="Y7" s="73"/>
       <c r="Z7" s="52"/>
     </row>
     <row r="8" spans="1:26" ht="15.75">
-      <c r="A8" s="600" t="s">
+      <c r="A8" s="598" t="s">
         <v>359</v>
       </c>
       <c r="B8" s="157" t="s">
@@ -8836,7 +8839,7 @@
       <c r="Z8" s="172"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="601"/>
+      <c r="A9" s="599"/>
       <c r="B9" s="73"/>
       <c r="C9" s="166" t="s">
         <v>71</v>
@@ -8874,17 +8877,17 @@
       </c>
       <c r="S9" s="76"/>
       <c r="T9" s="73"/>
-      <c r="U9" s="603" t="s">
+      <c r="U9" s="601" t="s">
         <v>96</v>
       </c>
-      <c r="V9" s="604"/>
-      <c r="W9" s="605"/>
+      <c r="V9" s="602"/>
+      <c r="W9" s="603"/>
       <c r="X9" s="73"/>
       <c r="Y9" s="73"/>
       <c r="Z9" s="52"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="601"/>
+      <c r="A10" s="599"/>
       <c r="B10" s="73"/>
       <c r="C10" s="165" t="s">
         <v>3</v>
@@ -8928,17 +8931,17 @@
       </c>
       <c r="S10" s="76"/>
       <c r="T10" s="73"/>
-      <c r="U10" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="V10" s="604"/>
-      <c r="W10" s="605"/>
+      <c r="U10" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="V10" s="602"/>
+      <c r="W10" s="603"/>
       <c r="X10" s="73"/>
       <c r="Y10" s="73"/>
       <c r="Z10" s="52"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="601"/>
+      <c r="A11" s="599"/>
       <c r="B11" s="73"/>
       <c r="C11" s="165" t="s">
         <v>35</v>
@@ -8982,17 +8985,17 @@
       </c>
       <c r="S11" s="76"/>
       <c r="T11" s="73"/>
-      <c r="U11" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="V11" s="604"/>
-      <c r="W11" s="605"/>
+      <c r="U11" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="V11" s="602"/>
+      <c r="W11" s="603"/>
       <c r="X11" s="73"/>
       <c r="Y11" s="73"/>
       <c r="Z11" s="52"/>
     </row>
     <row r="12" spans="1:26" ht="15.75">
-      <c r="A12" s="601"/>
+      <c r="A12" s="599"/>
       <c r="B12" s="158" t="s">
         <v>127</v>
       </c>
@@ -9022,7 +9025,7 @@
       <c r="Z12" s="52"/>
     </row>
     <row r="13" spans="1:26" ht="15">
-      <c r="A13" s="601"/>
+      <c r="A13" s="599"/>
       <c r="B13" s="74"/>
       <c r="C13" s="165" t="s">
         <v>88</v>
@@ -9052,7 +9055,7 @@
       <c r="Z13" s="52"/>
     </row>
     <row r="14" spans="1:26" ht="15">
-      <c r="A14" s="601"/>
+      <c r="A14" s="599"/>
       <c r="B14" s="74"/>
       <c r="C14" s="165"/>
       <c r="D14" s="53" t="s">
@@ -9098,17 +9101,17 @@
       </c>
       <c r="S14" s="76"/>
       <c r="T14" s="73"/>
-      <c r="U14" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="V14" s="604"/>
-      <c r="W14" s="605"/>
+      <c r="U14" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="V14" s="602"/>
+      <c r="W14" s="603"/>
       <c r="X14" s="73"/>
       <c r="Y14" s="73"/>
       <c r="Z14" s="52"/>
     </row>
     <row r="15" spans="1:26" ht="15">
-      <c r="A15" s="601"/>
+      <c r="A15" s="599"/>
       <c r="B15" s="74"/>
       <c r="C15" s="163"/>
       <c r="D15" s="53" t="s">
@@ -9156,17 +9159,17 @@
       </c>
       <c r="S15" s="76"/>
       <c r="T15" s="73"/>
-      <c r="U15" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="V15" s="604"/>
-      <c r="W15" s="605"/>
+      <c r="U15" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="V15" s="602"/>
+      <c r="W15" s="603"/>
       <c r="X15" s="73"/>
       <c r="Y15" s="73"/>
       <c r="Z15" s="52"/>
     </row>
     <row r="16" spans="1:26" ht="15">
-      <c r="A16" s="601"/>
+      <c r="A16" s="599"/>
       <c r="B16" s="74"/>
       <c r="C16" s="163"/>
       <c r="D16" s="53" t="s">
@@ -9206,17 +9209,17 @@
       </c>
       <c r="S16" s="76"/>
       <c r="T16" s="73"/>
-      <c r="U16" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="V16" s="604"/>
-      <c r="W16" s="605"/>
+      <c r="U16" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="V16" s="602"/>
+      <c r="W16" s="603"/>
       <c r="X16" s="73"/>
       <c r="Y16" s="73"/>
       <c r="Z16" s="52"/>
     </row>
     <row r="17" spans="1:26" ht="15">
-      <c r="A17" s="601"/>
+      <c r="A17" s="599"/>
       <c r="B17" s="74"/>
       <c r="C17" s="163"/>
       <c r="D17" s="53" t="s">
@@ -9250,17 +9253,17 @@
       </c>
       <c r="S17" s="76"/>
       <c r="T17" s="73"/>
-      <c r="U17" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="V17" s="604"/>
-      <c r="W17" s="605"/>
+      <c r="U17" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="V17" s="602"/>
+      <c r="W17" s="603"/>
       <c r="X17" s="73"/>
       <c r="Y17" s="73"/>
       <c r="Z17" s="52"/>
     </row>
     <row r="18" spans="1:26" ht="15">
-      <c r="A18" s="601"/>
+      <c r="A18" s="599"/>
       <c r="B18" s="74"/>
       <c r="C18" s="165" t="s">
         <v>76</v>
@@ -9290,7 +9293,7 @@
       <c r="Z18" s="52"/>
     </row>
     <row r="19" spans="1:26" ht="15">
-      <c r="A19" s="601"/>
+      <c r="A19" s="599"/>
       <c r="B19" s="74"/>
       <c r="C19" s="165"/>
       <c r="D19" s="53" t="s">
@@ -9330,17 +9333,17 @@
       <c r="R19" s="70"/>
       <c r="S19" s="76"/>
       <c r="T19" s="73"/>
-      <c r="U19" s="603" t="s">
+      <c r="U19" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="V19" s="604"/>
-      <c r="W19" s="605"/>
+      <c r="V19" s="602"/>
+      <c r="W19" s="603"/>
       <c r="X19" s="73"/>
       <c r="Y19" s="73"/>
       <c r="Z19" s="52"/>
     </row>
     <row r="20" spans="1:26" ht="15">
-      <c r="A20" s="601"/>
+      <c r="A20" s="599"/>
       <c r="B20" s="74"/>
       <c r="C20" s="163"/>
       <c r="D20" s="53" t="s">
@@ -9380,17 +9383,17 @@
       <c r="R20" s="70"/>
       <c r="S20" s="76"/>
       <c r="T20" s="73"/>
-      <c r="U20" s="603" t="s">
+      <c r="U20" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="V20" s="604"/>
-      <c r="W20" s="605"/>
+      <c r="V20" s="602"/>
+      <c r="W20" s="603"/>
       <c r="X20" s="73"/>
       <c r="Y20" s="73"/>
       <c r="Z20" s="52"/>
     </row>
     <row r="21" spans="1:26" ht="15">
-      <c r="A21" s="601"/>
+      <c r="A21" s="599"/>
       <c r="B21" s="74"/>
       <c r="C21" s="163"/>
       <c r="D21" s="53" t="s">
@@ -9428,17 +9431,17 @@
       <c r="R21" s="70"/>
       <c r="S21" s="76"/>
       <c r="T21" s="73"/>
-      <c r="U21" s="603" t="s">
+      <c r="U21" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="V21" s="604"/>
-      <c r="W21" s="605"/>
+      <c r="V21" s="602"/>
+      <c r="W21" s="603"/>
       <c r="X21" s="73"/>
       <c r="Y21" s="73"/>
       <c r="Z21" s="52"/>
     </row>
     <row r="22" spans="1:26" ht="15">
-      <c r="A22" s="601"/>
+      <c r="A22" s="599"/>
       <c r="B22" s="74"/>
       <c r="C22" s="41"/>
       <c r="D22" s="53" t="s">
@@ -9478,17 +9481,17 @@
       <c r="R22" s="70"/>
       <c r="S22" s="76"/>
       <c r="T22" s="73"/>
-      <c r="U22" s="603" t="s">
+      <c r="U22" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="V22" s="604"/>
-      <c r="W22" s="605"/>
+      <c r="V22" s="602"/>
+      <c r="W22" s="603"/>
       <c r="X22" s="73"/>
       <c r="Y22" s="73"/>
       <c r="Z22" s="52"/>
     </row>
     <row r="23" spans="1:26" ht="15">
-      <c r="A23" s="601"/>
+      <c r="A23" s="599"/>
       <c r="B23" s="74"/>
       <c r="C23" s="41"/>
       <c r="D23" s="53" t="s">
@@ -9524,17 +9527,17 @@
       <c r="R23" s="70"/>
       <c r="S23" s="76"/>
       <c r="T23" s="73"/>
-      <c r="U23" s="603" t="s">
+      <c r="U23" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="V23" s="604"/>
-      <c r="W23" s="605"/>
+      <c r="V23" s="602"/>
+      <c r="W23" s="603"/>
       <c r="X23" s="73"/>
       <c r="Y23" s="73"/>
       <c r="Z23" s="52"/>
     </row>
     <row r="24" spans="1:26" ht="15">
-      <c r="A24" s="602"/>
+      <c r="A24" s="600"/>
       <c r="B24" s="79"/>
       <c r="C24" s="161"/>
       <c r="D24" s="81"/>
@@ -9554,15 +9557,15 @@
       <c r="R24" s="81"/>
       <c r="S24" s="76"/>
       <c r="T24" s="81"/>
-      <c r="U24" s="610"/>
-      <c r="V24" s="611"/>
-      <c r="W24" s="612"/>
+      <c r="U24" s="604"/>
+      <c r="V24" s="605"/>
+      <c r="W24" s="606"/>
       <c r="X24" s="81"/>
       <c r="Y24" s="81"/>
       <c r="Z24" s="160"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A25" s="600" t="s">
+      <c r="A25" s="598" t="s">
         <v>360</v>
       </c>
       <c r="B25" s="175" t="s">
@@ -9604,7 +9607,7 @@
       <c r="Z25" s="172"/>
     </row>
     <row r="26" spans="1:26" ht="15.75">
-      <c r="A26" s="601"/>
+      <c r="A26" s="599"/>
       <c r="B26" s="158" t="s">
         <v>129</v>
       </c>
@@ -9634,7 +9637,7 @@
       <c r="Z26" s="52"/>
     </row>
     <row r="27" spans="1:26" ht="15">
-      <c r="A27" s="601"/>
+      <c r="A27" s="599"/>
       <c r="B27" s="73"/>
       <c r="C27" s="124" t="s">
         <v>74</v>
@@ -9664,7 +9667,7 @@
       <c r="Z27" s="52"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="601"/>
+      <c r="A28" s="599"/>
       <c r="B28" s="73"/>
       <c r="C28" s="124"/>
       <c r="D28" s="73" t="s">
@@ -9694,17 +9697,17 @@
       <c r="R28" s="70"/>
       <c r="S28" s="76"/>
       <c r="T28" s="73"/>
-      <c r="U28" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="V28" s="604"/>
-      <c r="W28" s="605"/>
+      <c r="U28" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="V28" s="602"/>
+      <c r="W28" s="603"/>
       <c r="X28" s="73"/>
       <c r="Y28" s="73"/>
       <c r="Z28" s="52"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="601"/>
+      <c r="A29" s="599"/>
       <c r="B29" s="73"/>
       <c r="C29" s="52"/>
       <c r="D29" s="53" t="s">
@@ -9734,17 +9737,17 @@
       <c r="R29" s="70"/>
       <c r="S29" s="76"/>
       <c r="T29" s="73"/>
-      <c r="U29" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="V29" s="604"/>
-      <c r="W29" s="605"/>
+      <c r="U29" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="V29" s="602"/>
+      <c r="W29" s="603"/>
       <c r="X29" s="73"/>
       <c r="Y29" s="73"/>
       <c r="Z29" s="52"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="601"/>
+      <c r="A30" s="599"/>
       <c r="B30" s="73"/>
       <c r="C30" s="52"/>
       <c r="D30" s="53" t="s">
@@ -9770,15 +9773,15 @@
       <c r="R30" s="70"/>
       <c r="S30" s="76"/>
       <c r="T30" s="73"/>
-      <c r="U30" s="603"/>
-      <c r="V30" s="604"/>
-      <c r="W30" s="605"/>
+      <c r="U30" s="601"/>
+      <c r="V30" s="602"/>
+      <c r="W30" s="603"/>
       <c r="X30" s="73"/>
       <c r="Y30" s="73"/>
       <c r="Z30" s="52"/>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="601"/>
+      <c r="A31" s="599"/>
       <c r="B31" s="73"/>
       <c r="C31" s="52"/>
       <c r="D31" s="53" t="s">
@@ -9804,15 +9807,15 @@
       <c r="R31" s="70"/>
       <c r="S31" s="76"/>
       <c r="T31" s="73"/>
-      <c r="U31" s="603"/>
-      <c r="V31" s="604"/>
-      <c r="W31" s="605"/>
+      <c r="U31" s="601"/>
+      <c r="V31" s="602"/>
+      <c r="W31" s="603"/>
       <c r="X31" s="73"/>
       <c r="Y31" s="73"/>
       <c r="Z31" s="52"/>
     </row>
     <row r="32" spans="1:26" ht="15">
-      <c r="A32" s="601"/>
+      <c r="A32" s="599"/>
       <c r="B32" s="73"/>
       <c r="C32" s="124" t="s">
         <v>76</v>
@@ -9842,7 +9845,7 @@
       <c r="Z32" s="52"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A33" s="601"/>
+      <c r="A33" s="599"/>
       <c r="B33" s="73"/>
       <c r="C33" s="124"/>
       <c r="D33" s="73" t="s">
@@ -9884,7 +9887,7 @@
       <c r="Z33" s="52"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="601"/>
+      <c r="A34" s="599"/>
       <c r="B34" s="73"/>
       <c r="C34" s="52"/>
       <c r="D34" s="53" t="s">
@@ -9926,7 +9929,7 @@
       <c r="Z34" s="52"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="601"/>
+      <c r="A35" s="599"/>
       <c r="B35" s="73"/>
       <c r="C35" s="52"/>
       <c r="D35" s="53" t="s">
@@ -9966,7 +9969,7 @@
       <c r="Z35" s="52"/>
     </row>
     <row r="36" spans="1:26" ht="15">
-      <c r="A36" s="601"/>
+      <c r="A36" s="599"/>
       <c r="B36" s="73"/>
       <c r="C36" s="46"/>
       <c r="D36" s="53" t="s">
@@ -10008,7 +10011,7 @@
       <c r="Z36" s="52"/>
     </row>
     <row r="37" spans="1:26">
-      <c r="A37" s="602"/>
+      <c r="A37" s="600"/>
       <c r="B37" s="73"/>
       <c r="C37" s="52"/>
       <c r="D37" s="53" t="s">
@@ -10554,6 +10557,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="U7:W7"/>
     <mergeCell ref="U21:W21"/>
     <mergeCell ref="U22:W22"/>
     <mergeCell ref="U23:W23"/>
@@ -10570,16 +10583,6 @@
     <mergeCell ref="U11:W11"/>
     <mergeCell ref="U14:W14"/>
     <mergeCell ref="U15:W15"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="U7:W7"/>
   </mergeCells>
   <conditionalFormatting sqref="F12:G22 F25:R38 F23:R23 H24:N24 F10:G10 H8:R8 H10:R22 F7:R7 F5:R5">
     <cfRule type="cellIs" dxfId="33" priority="13" operator="equal">
@@ -15379,11 +15382,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="CO4:CY4"/>
-    <mergeCell ref="CZ4:DH4"/>
-    <mergeCell ref="DI4:DM4"/>
-    <mergeCell ref="DN4:DP4"/>
-    <mergeCell ref="DQ4:DU4"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="J3:DM3"/>
     <mergeCell ref="DN3:EI3"/>
@@ -15396,6 +15394,11 @@
     <mergeCell ref="BC4:BL4"/>
     <mergeCell ref="DV4:EI4"/>
     <mergeCell ref="BM4:CN4"/>
+    <mergeCell ref="CO4:CY4"/>
+    <mergeCell ref="CZ4:DH4"/>
+    <mergeCell ref="DI4:DM4"/>
+    <mergeCell ref="DN4:DP4"/>
+    <mergeCell ref="DQ4:DU4"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C13">
     <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Projeto">
@@ -15471,14 +15474,14 @@
     </row>
     <row r="3" spans="5:20" ht="15.75" thickBot="1">
       <c r="F3" s="33"/>
-      <c r="G3" s="654" t="s">
+      <c r="G3" s="653" t="s">
         <v>115</v>
       </c>
-      <c r="H3" s="655"/>
-      <c r="J3" s="654" t="s">
+      <c r="H3" s="654"/>
+      <c r="J3" s="653" t="s">
         <v>115</v>
       </c>
-      <c r="K3" s="655"/>
+      <c r="K3" s="654"/>
       <c r="S3" t="s">
         <v>154</v>
       </c>
@@ -15520,11 +15523,11 @@
       </c>
       <c r="M5" s="106"/>
       <c r="N5" s="118"/>
-      <c r="O5" s="662" t="s">
+      <c r="O5" s="671" t="s">
         <v>132</v>
       </c>
-      <c r="P5" s="662"/>
-      <c r="Q5" s="663"/>
+      <c r="P5" s="671"/>
+      <c r="Q5" s="672"/>
     </row>
     <row r="6" spans="5:20" ht="15.75" customHeight="1">
       <c r="E6" s="179"/>
@@ -15534,7 +15537,7 @@
       <c r="G6" s="181" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="672" t="s">
+      <c r="H6" s="655" t="s">
         <v>141</v>
       </c>
       <c r="I6">
@@ -15543,16 +15546,16 @@
       <c r="J6" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="656" t="s">
+      <c r="K6" s="678" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="106"/>
       <c r="N6" s="118"/>
       <c r="O6" s="57"/>
-      <c r="P6" s="666" t="s">
+      <c r="P6" s="669" t="s">
         <v>116</v>
       </c>
-      <c r="Q6" s="667"/>
+      <c r="Q6" s="670"/>
       <c r="S6" s="195">
         <v>1</v>
       </c>
@@ -15568,14 +15571,14 @@
       <c r="G7" s="182" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="673"/>
+      <c r="H7" s="656"/>
       <c r="I7">
         <v>2</v>
       </c>
       <c r="J7" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="657"/>
+      <c r="K7" s="679"/>
       <c r="M7" s="113"/>
       <c r="N7" s="119"/>
       <c r="O7" s="57"/>
@@ -15596,18 +15599,18 @@
       <c r="G8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="674"/>
+      <c r="H8" s="657"/>
       <c r="J8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="658"/>
+      <c r="K8" s="680"/>
       <c r="M8" s="113"/>
       <c r="N8" s="119"/>
       <c r="O8" s="76"/>
-      <c r="P8" s="668" t="s">
+      <c r="P8" s="667" t="s">
         <v>117</v>
       </c>
-      <c r="Q8" s="669"/>
+      <c r="Q8" s="668"/>
       <c r="S8" s="206" t="s">
         <v>148</v>
       </c>
@@ -15735,7 +15738,7 @@
       <c r="G14" s="185" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="675" t="s">
+      <c r="H14" s="658" t="s">
         <v>145</v>
       </c>
       <c r="I14">
@@ -15744,7 +15747,7 @@
       <c r="J14" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="659" t="s">
+      <c r="K14" s="681" t="s">
         <v>19</v>
       </c>
       <c r="M14" s="114"/>
@@ -15765,21 +15768,21 @@
       <c r="G15" s="186" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="676"/>
+      <c r="H15" s="659"/>
       <c r="I15">
         <v>5</v>
       </c>
       <c r="J15" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="660"/>
+      <c r="K15" s="682"/>
       <c r="M15" s="106"/>
       <c r="N15" s="119"/>
-      <c r="O15" s="662" t="s">
+      <c r="O15" s="671" t="s">
         <v>133</v>
       </c>
-      <c r="P15" s="662"/>
-      <c r="Q15" s="663"/>
+      <c r="P15" s="671"/>
+      <c r="Q15" s="672"/>
       <c r="S15" s="206"/>
       <c r="T15" s="208" t="s">
         <v>75</v>
@@ -15793,23 +15796,23 @@
       <c r="G16" s="186" t="s">
         <v>146</v>
       </c>
-      <c r="H16" s="677"/>
+      <c r="H16" s="660"/>
       <c r="I16">
         <v>6</v>
       </c>
       <c r="J16" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="660"/>
+      <c r="K16" s="682"/>
       <c r="M16" s="114" t="s">
         <v>122</v>
       </c>
       <c r="N16" s="119"/>
       <c r="O16" s="76"/>
-      <c r="P16" s="670" t="s">
+      <c r="P16" s="673" t="s">
         <v>71</v>
       </c>
-      <c r="Q16" s="671"/>
+      <c r="Q16" s="674"/>
       <c r="S16" s="206"/>
       <c r="T16" s="208" t="s">
         <v>73</v>
@@ -15823,7 +15826,7 @@
       <c r="G17" s="187" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="678" t="s">
+      <c r="H17" s="661" t="s">
         <v>24</v>
       </c>
       <c r="I17">
@@ -15832,16 +15835,16 @@
       <c r="J17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="661"/>
+      <c r="K17" s="683"/>
       <c r="M17" s="114" t="s">
         <v>121</v>
       </c>
       <c r="N17" s="120"/>
       <c r="O17" s="76"/>
-      <c r="P17" s="670" t="s">
+      <c r="P17" s="673" t="s">
         <v>3</v>
       </c>
-      <c r="Q17" s="671"/>
+      <c r="Q17" s="674"/>
       <c r="S17" s="206"/>
       <c r="T17" s="208" t="s">
         <v>119</v>
@@ -15853,20 +15856,20 @@
       <c r="G18" s="188" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="679"/>
+      <c r="H18" s="662"/>
       <c r="J18" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="656" t="s">
+      <c r="K18" s="678" t="s">
         <v>24</v>
       </c>
       <c r="M18" s="106"/>
       <c r="N18" s="120"/>
       <c r="O18" s="76"/>
-      <c r="P18" s="670" t="s">
+      <c r="P18" s="673" t="s">
         <v>35</v>
       </c>
-      <c r="Q18" s="671"/>
+      <c r="Q18" s="674"/>
       <c r="S18" s="206" t="s">
         <v>162</v>
       </c>
@@ -15880,11 +15883,11 @@
       <c r="G19" s="188" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="679"/>
+      <c r="H19" s="662"/>
       <c r="J19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="657"/>
+      <c r="K19" s="679"/>
       <c r="M19" s="106"/>
       <c r="N19" s="118"/>
       <c r="O19" s="76"/>
@@ -15901,18 +15904,18 @@
       <c r="G20" s="189" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="680"/>
+      <c r="H20" s="663"/>
       <c r="J20" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="658"/>
+      <c r="K20" s="680"/>
       <c r="M20" s="106"/>
       <c r="N20" s="120"/>
-      <c r="O20" s="662" t="s">
+      <c r="O20" s="671" t="s">
         <v>134</v>
       </c>
-      <c r="P20" s="662"/>
-      <c r="Q20" s="663"/>
+      <c r="P20" s="671"/>
+      <c r="Q20" s="672"/>
       <c r="S20" s="206"/>
       <c r="T20" s="208" t="s">
         <v>77</v>
@@ -15941,10 +15944,10 @@
       <c r="M21" s="106"/>
       <c r="N21" s="119"/>
       <c r="O21" s="57"/>
-      <c r="P21" s="666" t="s">
+      <c r="P21" s="669" t="s">
         <v>88</v>
       </c>
-      <c r="Q21" s="667"/>
+      <c r="Q21" s="670"/>
       <c r="S21" s="206"/>
       <c r="T21" s="208" t="s">
         <v>78</v>
@@ -15956,7 +15959,7 @@
       <c r="G22" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="681" t="s">
+      <c r="H22" s="664" t="s">
         <v>30</v>
       </c>
       <c r="J22" s="145"/>
@@ -15981,7 +15984,7 @@
       <c r="G23" s="193" t="s">
         <v>149</v>
       </c>
-      <c r="H23" s="682"/>
+      <c r="H23" s="665"/>
       <c r="J23" s="145"/>
       <c r="K23" s="149"/>
       <c r="M23" s="113"/>
@@ -16002,9 +16005,9 @@
       <c r="G24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="683"/>
+      <c r="H24" s="666"/>
       <c r="J24" s="146"/>
-      <c r="K24" s="653"/>
+      <c r="K24" s="677"/>
       <c r="M24" s="113"/>
       <c r="N24" s="119"/>
       <c r="O24" s="57"/>
@@ -16029,7 +16032,7 @@
         <v>152</v>
       </c>
       <c r="J25" s="147"/>
-      <c r="K25" s="653"/>
+      <c r="K25" s="677"/>
       <c r="M25" s="113"/>
       <c r="N25" s="119"/>
       <c r="O25" s="57"/>
@@ -16047,14 +16050,14 @@
         <v>12</v>
       </c>
       <c r="J26" s="147"/>
-      <c r="K26" s="653"/>
+      <c r="K26" s="677"/>
       <c r="M26" s="113"/>
       <c r="N26" s="119"/>
       <c r="O26" s="57"/>
-      <c r="P26" s="666" t="s">
+      <c r="P26" s="669" t="s">
         <v>76</v>
       </c>
-      <c r="Q26" s="667"/>
+      <c r="Q26" s="670"/>
       <c r="S26" s="196">
         <v>3</v>
       </c>
@@ -16226,11 +16229,11 @@
       <c r="K36" s="148"/>
       <c r="M36" s="113"/>
       <c r="N36" s="119"/>
-      <c r="O36" s="664" t="s">
+      <c r="O36" s="675" t="s">
         <v>135</v>
       </c>
-      <c r="P36" s="664"/>
-      <c r="Q36" s="665"/>
+      <c r="P36" s="675"/>
+      <c r="Q36" s="676"/>
       <c r="S36" s="196">
         <v>7</v>
       </c>
@@ -16244,10 +16247,10 @@
       <c r="M37" s="113"/>
       <c r="N37" s="119"/>
       <c r="O37" s="109"/>
-      <c r="P37" s="666" t="s">
+      <c r="P37" s="669" t="s">
         <v>98</v>
       </c>
-      <c r="Q37" s="667"/>
+      <c r="Q37" s="670"/>
       <c r="T37" s="205" t="s">
         <v>23</v>
       </c>
@@ -16315,20 +16318,20 @@
         <v>19</v>
       </c>
       <c r="N43" s="120"/>
-      <c r="O43" s="662" t="s">
+      <c r="O43" s="671" t="s">
         <v>136</v>
       </c>
-      <c r="P43" s="662"/>
-      <c r="Q43" s="663"/>
+      <c r="P43" s="671"/>
+      <c r="Q43" s="672"/>
     </row>
     <row r="44" spans="6:20" ht="15.75" customHeight="1">
       <c r="M44" s="113"/>
       <c r="N44" s="119"/>
       <c r="O44" s="76"/>
-      <c r="P44" s="666" t="s">
+      <c r="P44" s="669" t="s">
         <v>74</v>
       </c>
-      <c r="Q44" s="667"/>
+      <c r="Q44" s="670"/>
     </row>
     <row r="45" spans="6:20" ht="15" hidden="1" customHeight="1" outlineLevel="1">
       <c r="M45" s="106"/>
@@ -16370,10 +16373,10 @@
       <c r="M49" s="113"/>
       <c r="N49" s="119"/>
       <c r="O49" s="76"/>
-      <c r="P49" s="666" t="s">
+      <c r="P49" s="669" t="s">
         <v>76</v>
       </c>
-      <c r="Q49" s="667"/>
+      <c r="Q49" s="670"/>
     </row>
     <row r="50" spans="11:18" ht="15.75" hidden="1" customHeight="1" outlineLevel="1">
       <c r="M50" s="113"/>
@@ -16451,11 +16454,11 @@
         <v>3</v>
       </c>
       <c r="N58" s="126"/>
-      <c r="O58" s="662" t="s">
+      <c r="O58" s="671" t="s">
         <v>137</v>
       </c>
-      <c r="P58" s="662"/>
-      <c r="Q58" s="663"/>
+      <c r="P58" s="671"/>
+      <c r="Q58" s="672"/>
     </row>
     <row r="59" spans="11:18" ht="15.75" customHeight="1">
       <c r="M59" s="111"/>
@@ -16469,11 +16472,11 @@
         <v>62</v>
       </c>
       <c r="N60" s="123"/>
-      <c r="O60" s="662" t="s">
+      <c r="O60" s="671" t="s">
         <v>138</v>
       </c>
-      <c r="P60" s="662"/>
-      <c r="Q60" s="663"/>
+      <c r="P60" s="671"/>
+      <c r="Q60" s="672"/>
       <c r="R60" s="110"/>
     </row>
     <row r="61" spans="11:18" ht="18">
@@ -16531,11 +16534,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H20"/>
-    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="O43:Q43"/>
+    <mergeCell ref="O58:Q58"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="O60:Q60"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="P26:Q26"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="O5:Q5"/>
@@ -16543,21 +16556,11 @@
     <mergeCell ref="P18:Q18"/>
     <mergeCell ref="O15:Q15"/>
     <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="O60:Q60"/>
-    <mergeCell ref="P49:Q49"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="O36:Q36"/>
-    <mergeCell ref="O43:Q43"/>
-    <mergeCell ref="O58:Q58"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H17:H20"/>
+    <mergeCell ref="H22:H24"/>
   </mergeCells>
   <conditionalFormatting sqref="Q50:Q57 O60:O61 Q7 P37 Q45:Q48 Q22:Q25 Q19 Q38:Q41 P42 P44:P57 P21:P35 Q27:Q35 P6:P14 Q9:Q14 O5:O58 N20:N36 M22:M36 M16:M17 P17:P19 Q17 N7:N18 M7:M14">
     <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
@@ -16750,10 +16753,10 @@
         <v>167</v>
       </c>
       <c r="C2" s="241"/>
-      <c r="D2" s="684" t="s">
+      <c r="D2" s="688" t="s">
         <v>166</v>
       </c>
-      <c r="E2" s="685"/>
+      <c r="E2" s="689"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15.75">
@@ -17732,18 +17735,18 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:146" ht="39.75" thickBot="1">
-      <c r="A49" s="686" t="s">
+      <c r="A49" s="690" t="s">
         <v>197</v>
       </c>
-      <c r="B49" s="687"/>
-      <c r="C49" s="687"/>
-      <c r="D49" s="687"/>
-      <c r="E49" s="687"/>
-      <c r="F49" s="687"/>
-      <c r="G49" s="687"/>
-      <c r="H49" s="687"/>
-      <c r="I49" s="687"/>
-      <c r="J49" s="688"/>
+      <c r="B49" s="691"/>
+      <c r="C49" s="691"/>
+      <c r="D49" s="691"/>
+      <c r="E49" s="691"/>
+      <c r="F49" s="691"/>
+      <c r="G49" s="691"/>
+      <c r="H49" s="691"/>
+      <c r="I49" s="691"/>
+      <c r="J49" s="692"/>
       <c r="K49" s="644" t="s">
         <v>198</v>
       </c>
@@ -17886,16 +17889,16 @@
       <c r="EP49" s="259"/>
     </row>
     <row r="50" spans="1:146" ht="31.5">
-      <c r="A50" s="689" t="s">
+      <c r="A50" s="693" t="s">
         <v>200</v>
       </c>
-      <c r="B50" s="690"/>
-      <c r="C50" s="690"/>
-      <c r="D50" s="690"/>
-      <c r="E50" s="690"/>
-      <c r="F50" s="690"/>
-      <c r="G50" s="690"/>
-      <c r="H50" s="691"/>
+      <c r="B50" s="694"/>
+      <c r="C50" s="694"/>
+      <c r="D50" s="694"/>
+      <c r="E50" s="694"/>
+      <c r="F50" s="694"/>
+      <c r="G50" s="694"/>
+      <c r="H50" s="695"/>
       <c r="I50" s="638" t="s">
         <v>201</v>
       </c>
@@ -18066,8 +18069,8 @@
         <v>214</v>
       </c>
       <c r="B51" s="263"/>
-      <c r="C51" s="692"/>
-      <c r="D51" s="693"/>
+      <c r="C51" s="684"/>
+      <c r="D51" s="685"/>
       <c r="E51" s="263"/>
       <c r="F51" s="263"/>
       <c r="G51" s="263"/>
@@ -18282,10 +18285,10 @@
       <c r="B52" s="268" t="s">
         <v>218</v>
       </c>
-      <c r="C52" s="692" t="s">
+      <c r="C52" s="684" t="s">
         <v>218</v>
       </c>
-      <c r="D52" s="693"/>
+      <c r="D52" s="685"/>
       <c r="E52" s="268" t="s">
         <v>218</v>
       </c>
@@ -18574,10 +18577,10 @@
       <c r="B53" s="285" t="s">
         <v>220</v>
       </c>
-      <c r="C53" s="694" t="s">
+      <c r="C53" s="686" t="s">
         <v>221</v>
       </c>
-      <c r="D53" s="695"/>
+      <c r="D53" s="687"/>
       <c r="E53" s="285" t="s">
         <v>222</v>
       </c>
@@ -19224,11 +19227,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="DR50:DV50"/>
-    <mergeCell ref="DW50:EJ50"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C53:D53"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="K49:DN49"/>
@@ -19245,6 +19243,11 @@
     <mergeCell ref="DA50:DI50"/>
     <mergeCell ref="DJ50:DN50"/>
     <mergeCell ref="DO50:DQ50"/>
+    <mergeCell ref="DR50:DV50"/>
+    <mergeCell ref="DW50:EJ50"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C53:D53"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:E39 B26:C30 E29:E32 E15:E20 E10:E13">
     <cfRule type="cellIs" dxfId="6" priority="21" operator="equal">
@@ -19323,10 +19326,10 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="598"/>
-      <c r="B2" s="599"/>
-      <c r="C2" s="599"/>
-      <c r="D2" s="599"/>
+      <c r="A2" s="610"/>
+      <c r="B2" s="611"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
       <c r="E2" s="58" t="s">
         <v>51</v>
       </c>
@@ -19351,11 +19354,11 @@
       <c r="M2" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="599" t="s">
+      <c r="N2" s="611" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="599"/>
-      <c r="P2" s="606"/>
+      <c r="O2" s="611"/>
+      <c r="P2" s="612"/>
       <c r="Q2" s="61" t="s">
         <v>59</v>
       </c>
@@ -19367,7 +19370,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="600" t="s">
+      <c r="A3" s="598" t="s">
         <v>358</v>
       </c>
       <c r="B3" s="157" t="s">
@@ -19391,7 +19394,7 @@
       <c r="S3" s="52"/>
     </row>
     <row r="4" spans="1:19" ht="15">
-      <c r="A4" s="601"/>
+      <c r="A4" s="599"/>
       <c r="B4" s="74"/>
       <c r="C4" s="163" t="s">
         <v>116</v>
@@ -19413,7 +19416,7 @@
       <c r="S4" s="52"/>
     </row>
     <row r="5" spans="1:19" ht="15">
-      <c r="A5" s="601"/>
+      <c r="A5" s="599"/>
       <c r="B5" s="74"/>
       <c r="D5" s="85" t="s">
         <v>81</v>
@@ -19440,17 +19443,17 @@
         <v>91</v>
       </c>
       <c r="M5" s="73"/>
-      <c r="N5" s="603" t="s">
+      <c r="N5" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="O5" s="604"/>
-      <c r="P5" s="605"/>
+      <c r="O5" s="602"/>
+      <c r="P5" s="603"/>
       <c r="Q5" s="73"/>
       <c r="R5" s="73"/>
       <c r="S5" s="52"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="601"/>
+      <c r="A6" s="599"/>
       <c r="B6" s="73"/>
       <c r="C6" s="164" t="s">
         <v>117</v>
@@ -19473,7 +19476,7 @@
       <c r="S6" s="52"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="601"/>
+      <c r="A7" s="599"/>
       <c r="B7" s="73"/>
       <c r="C7" s="164"/>
       <c r="D7" s="85" t="s">
@@ -19502,17 +19505,17 @@
       </c>
       <c r="L7" s="76"/>
       <c r="M7" s="73"/>
-      <c r="N7" s="603" t="s">
+      <c r="N7" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="O7" s="604"/>
-      <c r="P7" s="605"/>
+      <c r="O7" s="602"/>
+      <c r="P7" s="603"/>
       <c r="Q7" s="73"/>
       <c r="R7" s="73"/>
       <c r="S7" s="52"/>
     </row>
     <row r="8" spans="1:19" ht="15.75">
-      <c r="A8" s="600" t="s">
+      <c r="A8" s="598" t="s">
         <v>359</v>
       </c>
       <c r="B8" s="157" t="s">
@@ -19537,7 +19540,7 @@
       <c r="S8" s="172"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A9" s="601"/>
+      <c r="A9" s="599"/>
       <c r="B9" s="73"/>
       <c r="C9" s="166" t="s">
         <v>71</v>
@@ -19566,17 +19569,17 @@
       </c>
       <c r="L9" s="76"/>
       <c r="M9" s="73"/>
-      <c r="N9" s="603" t="s">
+      <c r="N9" s="601" t="s">
         <v>96</v>
       </c>
-      <c r="O9" s="604"/>
-      <c r="P9" s="605"/>
+      <c r="O9" s="602"/>
+      <c r="P9" s="603"/>
       <c r="Q9" s="73"/>
       <c r="R9" s="73"/>
       <c r="S9" s="52"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="601"/>
+      <c r="A10" s="599"/>
       <c r="B10" s="73"/>
       <c r="C10" s="165" t="s">
         <v>3</v>
@@ -19605,17 +19608,17 @@
       </c>
       <c r="L10" s="76"/>
       <c r="M10" s="73"/>
-      <c r="N10" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="O10" s="604"/>
-      <c r="P10" s="605"/>
+      <c r="N10" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="602"/>
+      <c r="P10" s="603"/>
       <c r="Q10" s="73"/>
       <c r="R10" s="73"/>
       <c r="S10" s="52"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="601"/>
+      <c r="A11" s="599"/>
       <c r="B11" s="73"/>
       <c r="C11" s="165" t="s">
         <v>35</v>
@@ -19644,17 +19647,17 @@
       </c>
       <c r="L11" s="76"/>
       <c r="M11" s="73"/>
-      <c r="N11" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="O11" s="604"/>
-      <c r="P11" s="605"/>
+      <c r="N11" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" s="602"/>
+      <c r="P11" s="603"/>
       <c r="Q11" s="73"/>
       <c r="R11" s="73"/>
       <c r="S11" s="52"/>
     </row>
     <row r="12" spans="1:19" ht="15.75">
-      <c r="A12" s="601"/>
+      <c r="A12" s="599"/>
       <c r="B12" s="158" t="s">
         <v>127</v>
       </c>
@@ -19677,7 +19680,7 @@
       <c r="S12" s="52"/>
     </row>
     <row r="13" spans="1:19" ht="15">
-      <c r="A13" s="601"/>
+      <c r="A13" s="599"/>
       <c r="B13" s="74"/>
       <c r="C13" s="165" t="s">
         <v>88</v>
@@ -19700,7 +19703,7 @@
       <c r="S13" s="52"/>
     </row>
     <row r="14" spans="1:19" ht="15">
-      <c r="A14" s="601"/>
+      <c r="A14" s="599"/>
       <c r="B14" s="74"/>
       <c r="C14" s="165"/>
       <c r="D14" s="53" t="s">
@@ -19729,17 +19732,17 @@
       </c>
       <c r="L14" s="76"/>
       <c r="M14" s="73"/>
-      <c r="N14" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="O14" s="604"/>
-      <c r="P14" s="605"/>
+      <c r="N14" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="O14" s="602"/>
+      <c r="P14" s="603"/>
       <c r="Q14" s="73"/>
       <c r="R14" s="73"/>
       <c r="S14" s="52"/>
     </row>
     <row r="15" spans="1:19" ht="15">
-      <c r="A15" s="601"/>
+      <c r="A15" s="599"/>
       <c r="B15" s="74"/>
       <c r="C15" s="163"/>
       <c r="D15" s="53" t="s">
@@ -19768,17 +19771,17 @@
       </c>
       <c r="L15" s="76"/>
       <c r="M15" s="73"/>
-      <c r="N15" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="O15" s="604"/>
-      <c r="P15" s="605"/>
+      <c r="N15" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="602"/>
+      <c r="P15" s="603"/>
       <c r="Q15" s="73"/>
       <c r="R15" s="73"/>
       <c r="S15" s="52"/>
     </row>
     <row r="16" spans="1:19" ht="15">
-      <c r="A16" s="601"/>
+      <c r="A16" s="599"/>
       <c r="B16" s="74"/>
       <c r="C16" s="163"/>
       <c r="D16" s="53" t="s">
@@ -19803,17 +19806,17 @@
       </c>
       <c r="L16" s="76"/>
       <c r="M16" s="73"/>
-      <c r="N16" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="O16" s="604"/>
-      <c r="P16" s="605"/>
+      <c r="N16" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" s="602"/>
+      <c r="P16" s="603"/>
       <c r="Q16" s="73"/>
       <c r="R16" s="73"/>
       <c r="S16" s="52"/>
     </row>
     <row r="17" spans="1:19" ht="15">
-      <c r="A17" s="601"/>
+      <c r="A17" s="599"/>
       <c r="B17" s="74"/>
       <c r="C17" s="163"/>
       <c r="D17" s="53" t="s">
@@ -19838,17 +19841,17 @@
       </c>
       <c r="L17" s="76"/>
       <c r="M17" s="73"/>
-      <c r="N17" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="O17" s="604"/>
-      <c r="P17" s="605"/>
+      <c r="N17" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="602"/>
+      <c r="P17" s="603"/>
       <c r="Q17" s="73"/>
       <c r="R17" s="73"/>
       <c r="S17" s="52"/>
     </row>
     <row r="18" spans="1:19" ht="15">
-      <c r="A18" s="601"/>
+      <c r="A18" s="599"/>
       <c r="B18" s="74"/>
       <c r="C18" s="165" t="s">
         <v>76</v>
@@ -19871,7 +19874,7 @@
       <c r="S18" s="52"/>
     </row>
     <row r="19" spans="1:19" ht="15">
-      <c r="A19" s="601"/>
+      <c r="A19" s="599"/>
       <c r="B19" s="74"/>
       <c r="C19" s="165"/>
       <c r="D19" s="53" t="s">
@@ -19896,17 +19899,17 @@
       <c r="K19" s="70"/>
       <c r="L19" s="76"/>
       <c r="M19" s="73"/>
-      <c r="N19" s="603" t="s">
+      <c r="N19" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="O19" s="604"/>
-      <c r="P19" s="605"/>
+      <c r="O19" s="602"/>
+      <c r="P19" s="603"/>
       <c r="Q19" s="73"/>
       <c r="R19" s="73"/>
       <c r="S19" s="52"/>
     </row>
     <row r="20" spans="1:19" ht="15">
-      <c r="A20" s="601"/>
+      <c r="A20" s="599"/>
       <c r="B20" s="74"/>
       <c r="C20" s="163"/>
       <c r="D20" s="53" t="s">
@@ -19931,17 +19934,17 @@
       <c r="K20" s="70"/>
       <c r="L20" s="76"/>
       <c r="M20" s="73"/>
-      <c r="N20" s="603" t="s">
+      <c r="N20" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="O20" s="604"/>
-      <c r="P20" s="605"/>
+      <c r="O20" s="602"/>
+      <c r="P20" s="603"/>
       <c r="Q20" s="73"/>
       <c r="R20" s="73"/>
       <c r="S20" s="52"/>
     </row>
     <row r="21" spans="1:19" ht="15">
-      <c r="A21" s="601"/>
+      <c r="A21" s="599"/>
       <c r="B21" s="74"/>
       <c r="C21" s="163"/>
       <c r="D21" s="53" t="s">
@@ -19966,17 +19969,17 @@
       <c r="K21" s="70"/>
       <c r="L21" s="76"/>
       <c r="M21" s="73"/>
-      <c r="N21" s="603" t="s">
+      <c r="N21" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="O21" s="604"/>
-      <c r="P21" s="605"/>
+      <c r="O21" s="602"/>
+      <c r="P21" s="603"/>
       <c r="Q21" s="73"/>
       <c r="R21" s="73"/>
       <c r="S21" s="52"/>
     </row>
     <row r="22" spans="1:19" ht="15">
-      <c r="A22" s="601"/>
+      <c r="A22" s="599"/>
       <c r="B22" s="74"/>
       <c r="C22" s="41"/>
       <c r="D22" s="53" t="s">
@@ -20001,17 +20004,17 @@
       <c r="K22" s="70"/>
       <c r="L22" s="76"/>
       <c r="M22" s="73"/>
-      <c r="N22" s="603" t="s">
+      <c r="N22" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="O22" s="604"/>
-      <c r="P22" s="605"/>
+      <c r="O22" s="602"/>
+      <c r="P22" s="603"/>
       <c r="Q22" s="73"/>
       <c r="R22" s="73"/>
       <c r="S22" s="52"/>
     </row>
     <row r="23" spans="1:19" ht="15">
-      <c r="A23" s="601"/>
+      <c r="A23" s="599"/>
       <c r="B23" s="74"/>
       <c r="C23" s="41"/>
       <c r="D23" s="53" t="s">
@@ -20036,17 +20039,17 @@
       <c r="K23" s="70"/>
       <c r="L23" s="76"/>
       <c r="M23" s="73"/>
-      <c r="N23" s="603" t="s">
+      <c r="N23" s="601" t="s">
         <v>91</v>
       </c>
-      <c r="O23" s="604"/>
-      <c r="P23" s="605"/>
+      <c r="O23" s="602"/>
+      <c r="P23" s="603"/>
       <c r="Q23" s="73"/>
       <c r="R23" s="73"/>
       <c r="S23" s="52"/>
     </row>
     <row r="24" spans="1:19" ht="15">
-      <c r="A24" s="602"/>
+      <c r="A24" s="600"/>
       <c r="B24" s="79"/>
       <c r="C24" s="161"/>
       <c r="D24" s="81" t="s">
@@ -20071,17 +20074,17 @@
       <c r="K24" s="81"/>
       <c r="L24" s="76"/>
       <c r="M24" s="81"/>
-      <c r="N24" s="610" t="s">
+      <c r="N24" s="604" t="s">
         <v>91</v>
       </c>
-      <c r="O24" s="611"/>
-      <c r="P24" s="612"/>
+      <c r="O24" s="605"/>
+      <c r="P24" s="606"/>
       <c r="Q24" s="81"/>
       <c r="R24" s="81"/>
       <c r="S24" s="160"/>
     </row>
     <row r="25" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A25" s="600" t="s">
+      <c r="A25" s="598" t="s">
         <v>360</v>
       </c>
       <c r="B25" s="175" t="s">
@@ -20116,7 +20119,7 @@
       <c r="S25" s="172"/>
     </row>
     <row r="26" spans="1:19" ht="15.75">
-      <c r="A26" s="601"/>
+      <c r="A26" s="599"/>
       <c r="B26" s="158" t="s">
         <v>129</v>
       </c>
@@ -20139,7 +20142,7 @@
       <c r="S26" s="52"/>
     </row>
     <row r="27" spans="1:19" ht="15">
-      <c r="A27" s="601"/>
+      <c r="A27" s="599"/>
       <c r="B27" s="73"/>
       <c r="C27" s="124" t="s">
         <v>74</v>
@@ -20162,7 +20165,7 @@
       <c r="S27" s="52"/>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="601"/>
+      <c r="A28" s="599"/>
       <c r="B28" s="73"/>
       <c r="C28" s="124"/>
       <c r="D28" s="73" t="s">
@@ -20181,17 +20184,17 @@
       <c r="K28" s="70"/>
       <c r="L28" s="76"/>
       <c r="M28" s="73"/>
-      <c r="N28" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="O28" s="604"/>
-      <c r="P28" s="605"/>
+      <c r="N28" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="O28" s="602"/>
+      <c r="P28" s="603"/>
       <c r="Q28" s="73"/>
       <c r="R28" s="73"/>
       <c r="S28" s="52"/>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="601"/>
+      <c r="A29" s="599"/>
       <c r="B29" s="73"/>
       <c r="C29" s="52"/>
       <c r="D29" s="53" t="s">
@@ -20212,17 +20215,17 @@
       <c r="K29" s="70"/>
       <c r="L29" s="76"/>
       <c r="M29" s="73"/>
-      <c r="N29" s="603" t="s">
-        <v>63</v>
-      </c>
-      <c r="O29" s="604"/>
-      <c r="P29" s="605"/>
+      <c r="N29" s="601" t="s">
+        <v>63</v>
+      </c>
+      <c r="O29" s="602"/>
+      <c r="P29" s="603"/>
       <c r="Q29" s="73"/>
       <c r="R29" s="73"/>
       <c r="S29" s="52"/>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="601"/>
+      <c r="A30" s="599"/>
       <c r="B30" s="73"/>
       <c r="C30" s="52"/>
       <c r="D30" s="53" t="s">
@@ -20239,15 +20242,15 @@
       <c r="K30" s="70"/>
       <c r="L30" s="76"/>
       <c r="M30" s="73"/>
-      <c r="N30" s="603"/>
-      <c r="O30" s="604"/>
-      <c r="P30" s="605"/>
+      <c r="N30" s="601"/>
+      <c r="O30" s="602"/>
+      <c r="P30" s="603"/>
       <c r="Q30" s="73"/>
       <c r="R30" s="73"/>
       <c r="S30" s="52"/>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="601"/>
+      <c r="A31" s="599"/>
       <c r="B31" s="73"/>
       <c r="C31" s="52"/>
       <c r="D31" s="53" t="s">
@@ -20264,15 +20267,15 @@
       <c r="K31" s="70"/>
       <c r="L31" s="76"/>
       <c r="M31" s="73"/>
-      <c r="N31" s="603"/>
-      <c r="O31" s="604"/>
-      <c r="P31" s="605"/>
+      <c r="N31" s="601"/>
+      <c r="O31" s="602"/>
+      <c r="P31" s="603"/>
       <c r="Q31" s="73"/>
       <c r="R31" s="73"/>
       <c r="S31" s="52"/>
     </row>
     <row r="32" spans="1:19" ht="15">
-      <c r="A32" s="601"/>
+      <c r="A32" s="599"/>
       <c r="B32" s="73"/>
       <c r="C32" s="124" t="s">
         <v>76</v>
@@ -20295,7 +20298,7 @@
       <c r="S32" s="52"/>
     </row>
     <row r="33" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A33" s="601"/>
+      <c r="A33" s="599"/>
       <c r="B33" s="73"/>
       <c r="C33" s="124"/>
       <c r="D33" s="73" t="s">
@@ -20326,7 +20329,7 @@
       <c r="S33" s="52"/>
     </row>
     <row r="34" spans="1:19">
-      <c r="A34" s="601"/>
+      <c r="A34" s="599"/>
       <c r="B34" s="73"/>
       <c r="C34" s="52"/>
       <c r="D34" s="53" t="s">
@@ -20357,7 +20360,7 @@
       <c r="S34" s="52"/>
     </row>
     <row r="35" spans="1:19">
-      <c r="A35" s="601"/>
+      <c r="A35" s="599"/>
       <c r="B35" s="73"/>
       <c r="C35" s="52"/>
       <c r="D35" s="53" t="s">
@@ -20388,7 +20391,7 @@
       <c r="S35" s="52"/>
     </row>
     <row r="36" spans="1:19" ht="15">
-      <c r="A36" s="601"/>
+      <c r="A36" s="599"/>
       <c r="B36" s="73"/>
       <c r="C36" s="46"/>
       <c r="D36" s="53" t="s">
@@ -20419,7 +20422,7 @@
       <c r="S36" s="52"/>
     </row>
     <row r="37" spans="1:19">
-      <c r="A37" s="602"/>
+      <c r="A37" s="600"/>
       <c r="B37" s="73"/>
       <c r="C37" s="52"/>
       <c r="D37" s="53" t="s">
@@ -20679,16 +20682,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A24"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="N28:P28"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A25:A37"/>
     <mergeCell ref="N20:P20"/>
@@ -20705,6 +20698,16 @@
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="N31:P31"/>
     <mergeCell ref="N21:P21"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A24"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="N28:P28"/>
   </mergeCells>
   <conditionalFormatting sqref="E12:E22 E25:K38 E23:K23 F24:H24 E10 F8:K8 F10:K22 E7:K7 E5:K5">
     <cfRule type="cellIs" dxfId="77" priority="17" operator="equal">
@@ -24402,7 +24405,7 @@
       <c r="FA11" s="320"/>
     </row>
     <row r="12" spans="1:157" ht="15.75" customHeight="1">
-      <c r="A12" s="601" t="s">
+      <c r="A12" s="599" t="s">
         <v>358</v>
       </c>
       <c r="B12" s="426" t="s">
@@ -24564,7 +24567,7 @@
       <c r="EZ12" s="160"/>
     </row>
     <row r="13" spans="1:157" ht="15" customHeight="1">
-      <c r="A13" s="601"/>
+      <c r="A13" s="599"/>
       <c r="B13" s="74"/>
       <c r="C13" s="163" t="s">
         <v>116</v>
@@ -24635,7 +24638,7 @@
       <c r="BO13" s="353"/>
     </row>
     <row r="14" spans="1:157" ht="15" customHeight="1">
-      <c r="A14" s="601"/>
+      <c r="A14" s="599"/>
       <c r="B14" s="74"/>
       <c r="D14" s="85" t="s">
         <v>81</v>
@@ -25101,7 +25104,7 @@
       </c>
     </row>
     <row r="15" spans="1:157" ht="15" customHeight="1">
-      <c r="A15" s="601"/>
+      <c r="A15" s="599"/>
       <c r="B15" s="73"/>
       <c r="C15" s="164" t="s">
         <v>117</v>
@@ -25172,7 +25175,7 @@
       <c r="BO15" s="353"/>
     </row>
     <row r="16" spans="1:157">
-      <c r="A16" s="601"/>
+      <c r="A16" s="599"/>
       <c r="B16" s="73"/>
       <c r="C16" s="164"/>
       <c r="D16" s="85" t="s">
@@ -25639,7 +25642,7 @@
       </c>
     </row>
     <row r="17" spans="1:157" ht="15.75">
-      <c r="A17" s="600" t="s">
+      <c r="A17" s="598" t="s">
         <v>359</v>
       </c>
       <c r="B17" s="157" t="s">
@@ -25712,7 +25715,7 @@
       <c r="BO17" s="353"/>
     </row>
     <row r="18" spans="1:157" ht="15.75" customHeight="1">
-      <c r="A18" s="601"/>
+      <c r="A18" s="599"/>
       <c r="B18" s="73"/>
       <c r="C18" s="166" t="s">
         <v>71</v>
@@ -26179,7 +26182,7 @@
       </c>
     </row>
     <row r="19" spans="1:157">
-      <c r="A19" s="601"/>
+      <c r="A19" s="599"/>
       <c r="B19" s="73"/>
       <c r="C19" s="165" t="s">
         <v>3</v>
@@ -26646,7 +26649,7 @@
       </c>
     </row>
     <row r="20" spans="1:157">
-      <c r="A20" s="601"/>
+      <c r="A20" s="599"/>
       <c r="B20" s="73"/>
       <c r="C20" s="165" t="s">
         <v>35</v>
@@ -27113,7 +27116,7 @@
       </c>
     </row>
     <row r="21" spans="1:157" ht="15.75">
-      <c r="A21" s="601"/>
+      <c r="A21" s="599"/>
       <c r="B21" s="158" t="s">
         <v>127</v>
       </c>
@@ -27184,7 +27187,7 @@
       <c r="BO21" s="353"/>
     </row>
     <row r="22" spans="1:157" ht="15">
-      <c r="A22" s="601"/>
+      <c r="A22" s="599"/>
       <c r="B22" s="74"/>
       <c r="C22" s="165" t="s">
         <v>88</v>
@@ -27255,7 +27258,7 @@
       <c r="BO22" s="353"/>
     </row>
     <row r="23" spans="1:157" ht="15">
-      <c r="A23" s="601"/>
+      <c r="A23" s="599"/>
       <c r="B23" s="74"/>
       <c r="C23" s="165"/>
       <c r="D23" s="53" t="s">
@@ -27722,7 +27725,7 @@
       </c>
     </row>
     <row r="24" spans="1:157" ht="15">
-      <c r="A24" s="601"/>
+      <c r="A24" s="599"/>
       <c r="B24" s="74"/>
       <c r="C24" s="163"/>
       <c r="D24" s="53" t="s">
@@ -28189,7 +28192,7 @@
       </c>
     </row>
     <row r="25" spans="1:157" ht="15">
-      <c r="A25" s="601"/>
+      <c r="A25" s="599"/>
       <c r="B25" s="74"/>
       <c r="C25" s="163"/>
       <c r="D25" s="53" t="s">
@@ -28656,7 +28659,7 @@
       </c>
     </row>
     <row r="26" spans="1:157" ht="15">
-      <c r="A26" s="601"/>
+      <c r="A26" s="599"/>
       <c r="B26" s="74"/>
       <c r="C26" s="163"/>
       <c r="D26" s="53" t="s">
@@ -29123,7 +29126,7 @@
       </c>
     </row>
     <row r="27" spans="1:157" ht="15">
-      <c r="A27" s="601"/>
+      <c r="A27" s="599"/>
       <c r="B27" s="74"/>
       <c r="C27" s="165" t="s">
         <v>76</v>
@@ -29194,7 +29197,7 @@
       <c r="BO27" s="353"/>
     </row>
     <row r="28" spans="1:157" ht="15">
-      <c r="A28" s="601"/>
+      <c r="A28" s="599"/>
       <c r="B28" s="74"/>
       <c r="C28" s="165"/>
       <c r="D28" s="53" t="s">
@@ -29661,7 +29664,7 @@
       </c>
     </row>
     <row r="29" spans="1:157" ht="15">
-      <c r="A29" s="601"/>
+      <c r="A29" s="599"/>
       <c r="B29" s="74"/>
       <c r="C29" s="163"/>
       <c r="D29" s="53" t="s">
@@ -29753,7 +29756,7 @@
       <c r="BO29" s="353"/>
     </row>
     <row r="30" spans="1:157" ht="15">
-      <c r="A30" s="601"/>
+      <c r="A30" s="599"/>
       <c r="B30" s="74"/>
       <c r="C30" s="163"/>
       <c r="D30" s="53" t="s">
@@ -29845,7 +29848,7 @@
       <c r="BO30" s="353"/>
     </row>
     <row r="31" spans="1:157" ht="15">
-      <c r="A31" s="601"/>
+      <c r="A31" s="599"/>
       <c r="B31" s="74"/>
       <c r="C31" s="41"/>
       <c r="D31" s="53" t="s">
@@ -29937,7 +29940,7 @@
       <c r="BO31" s="353"/>
     </row>
     <row r="32" spans="1:157" ht="15">
-      <c r="A32" s="601"/>
+      <c r="A32" s="599"/>
       <c r="B32" s="74"/>
       <c r="C32" s="41"/>
       <c r="D32" s="53" t="s">
@@ -30405,7 +30408,7 @@
       <c r="FA32" s="353"/>
     </row>
     <row r="33" spans="1:156" ht="15">
-      <c r="A33" s="602"/>
+      <c r="A33" s="600"/>
       <c r="B33" s="79"/>
       <c r="C33" s="161"/>
       <c r="D33" s="81"/>
@@ -30870,7 +30873,7 @@
       </c>
     </row>
     <row r="34" spans="1:156" ht="15.75" customHeight="1">
-      <c r="A34" s="600" t="s">
+      <c r="A34" s="598" t="s">
         <v>360</v>
       </c>
       <c r="B34" s="175" t="s">
@@ -31341,7 +31344,7 @@
       </c>
     </row>
     <row r="35" spans="1:156" ht="15.75">
-      <c r="A35" s="601"/>
+      <c r="A35" s="599"/>
       <c r="B35" s="158" t="s">
         <v>129</v>
       </c>
@@ -31412,7 +31415,7 @@
       <c r="BO35" s="353"/>
     </row>
     <row r="36" spans="1:156" ht="15">
-      <c r="A36" s="601"/>
+      <c r="A36" s="599"/>
       <c r="B36" s="73"/>
       <c r="C36" s="124" t="s">
         <v>74</v>
@@ -31483,7 +31486,7 @@
       <c r="BO36" s="353"/>
     </row>
     <row r="37" spans="1:156">
-      <c r="A37" s="601"/>
+      <c r="A37" s="599"/>
       <c r="B37" s="73"/>
       <c r="C37" s="124"/>
       <c r="D37" s="73" t="s">
@@ -31950,7 +31953,7 @@
       </c>
     </row>
     <row r="38" spans="1:156">
-      <c r="A38" s="601"/>
+      <c r="A38" s="599"/>
       <c r="B38" s="73"/>
       <c r="C38" s="52"/>
       <c r="D38" s="53" t="s">
@@ -32043,7 +32046,7 @@
       </c>
     </row>
     <row r="39" spans="1:156">
-      <c r="A39" s="601"/>
+      <c r="A39" s="599"/>
       <c r="B39" s="73"/>
       <c r="C39" s="52"/>
       <c r="D39" s="53" t="s">
@@ -32510,7 +32513,7 @@
       </c>
     </row>
     <row r="40" spans="1:156">
-      <c r="A40" s="601"/>
+      <c r="A40" s="599"/>
       <c r="B40" s="73"/>
       <c r="C40" s="52"/>
       <c r="D40" s="53" t="s">
@@ -32977,7 +32980,7 @@
       </c>
     </row>
     <row r="41" spans="1:156" ht="15">
-      <c r="A41" s="601"/>
+      <c r="A41" s="599"/>
       <c r="B41" s="73"/>
       <c r="C41" s="124" t="s">
         <v>76</v>
@@ -33048,7 +33051,7 @@
       <c r="BO41" s="353"/>
     </row>
     <row r="42" spans="1:156" ht="15.75" customHeight="1">
-      <c r="A42" s="601"/>
+      <c r="A42" s="599"/>
       <c r="B42" s="73"/>
       <c r="C42" s="124"/>
       <c r="D42" s="73" t="s">
@@ -33515,7 +33518,7 @@
       </c>
     </row>
     <row r="43" spans="1:156">
-      <c r="A43" s="601"/>
+      <c r="A43" s="599"/>
       <c r="B43" s="73"/>
       <c r="C43" s="52"/>
       <c r="D43" s="53" t="s">
@@ -33982,7 +33985,7 @@
       </c>
     </row>
     <row r="44" spans="1:156">
-      <c r="A44" s="601"/>
+      <c r="A44" s="599"/>
       <c r="B44" s="73"/>
       <c r="C44" s="52"/>
       <c r="D44" s="53" t="s">
@@ -34078,7 +34081,7 @@
       </c>
     </row>
     <row r="45" spans="1:156" ht="15">
-      <c r="A45" s="601"/>
+      <c r="A45" s="599"/>
       <c r="B45" s="73"/>
       <c r="C45" s="46"/>
       <c r="D45" s="53" t="s">
@@ -34174,7 +34177,7 @@
       </c>
     </row>
     <row r="46" spans="1:156">
-      <c r="A46" s="602"/>
+      <c r="A46" s="600"/>
       <c r="B46" s="73"/>
       <c r="C46" s="52"/>
       <c r="D46" s="53" t="s">
@@ -42292,8 +42295,8 @@
   </sheetPr>
   <dimension ref="A1:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42338,7 +42341,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="570" t="s">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="579" t="s">
         <v>564</v>
@@ -42347,9 +42350,9 @@
       <c r="G2" s="590" t="s">
         <v>983</v>
       </c>
-      <c r="H2" s="562" t="str">
+      <c r="H2" s="562" t="e">
         <f>VLOOKUP(C2,sup_hiperlinks!$E$10:$G$39,3,0)</f>
-        <v>http://minutapiuriobranco.gestaourbana.prefeitura.sp.gov.br/wp-content/uploads/2016/04/PIU_RioBranco_ConsultaPublica_V03.pdf</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="552" customFormat="1">
@@ -45752,10 +45755,10 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="598"/>
-      <c r="B2" s="599"/>
-      <c r="C2" s="599"/>
-      <c r="D2" s="599"/>
+      <c r="A2" s="610"/>
+      <c r="B2" s="611"/>
+      <c r="C2" s="611"/>
+      <c r="D2" s="611"/>
       <c r="E2" s="58" t="s">
         <v>51</v>
       </c>
@@ -46681,18 +46684,18 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="598"/>
-      <c r="B3" s="599"/>
-      <c r="C3" s="599"/>
-      <c r="D3" s="599"/>
+      <c r="A3" s="610"/>
+      <c r="B3" s="611"/>
+      <c r="C3" s="611"/>
+      <c r="D3" s="611"/>
       <c r="E3" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="598" t="s">
+      <c r="F3" s="610" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="599"/>
-      <c r="H3" s="606"/>
+      <c r="G3" s="611"/>
+      <c r="H3" s="612"/>
       <c r="I3" s="61" t="s">
         <v>59</v>
       </c>
@@ -46728,11 +46731,11 @@
       </c>
       <c r="D5" s="74"/>
       <c r="E5" s="91"/>
-      <c r="F5" s="622" t="s">
+      <c r="F5" s="631" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="623"/>
-      <c r="H5" s="624"/>
+      <c r="G5" s="632"/>
+      <c r="H5" s="633"/>
       <c r="I5" s="91"/>
       <c r="J5" s="65"/>
       <c r="K5" s="65"/>
@@ -46745,11 +46748,11 @@
       </c>
       <c r="D6" s="92"/>
       <c r="E6" s="91"/>
-      <c r="F6" s="622" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="623"/>
-      <c r="H6" s="624"/>
+      <c r="F6" s="631" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="632"/>
+      <c r="H6" s="633"/>
       <c r="I6" s="91"/>
       <c r="J6" s="65"/>
       <c r="K6" s="65"/>
@@ -46762,11 +46765,11 @@
       </c>
       <c r="D7" s="75"/>
       <c r="E7" s="91"/>
-      <c r="F7" s="622" t="s">
+      <c r="F7" s="631" t="s">
         <v>96</v>
       </c>
-      <c r="G7" s="623"/>
-      <c r="H7" s="624"/>
+      <c r="G7" s="632"/>
+      <c r="H7" s="633"/>
       <c r="I7" s="91"/>
       <c r="J7" s="65"/>
       <c r="K7" s="65"/>
@@ -46779,11 +46782,11 @@
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="91"/>
-      <c r="F8" s="622" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="623"/>
-      <c r="H8" s="624"/>
+      <c r="F8" s="631" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="632"/>
+      <c r="H8" s="633"/>
       <c r="I8" s="91"/>
       <c r="J8" s="65"/>
       <c r="K8" s="65"/>
@@ -46796,11 +46799,11 @@
         <v>103</v>
       </c>
       <c r="E9" s="91"/>
-      <c r="F9" s="622" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="623"/>
-      <c r="H9" s="624"/>
+      <c r="F9" s="631" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="632"/>
+      <c r="H9" s="633"/>
       <c r="I9" s="91"/>
       <c r="J9" s="65"/>
       <c r="K9" s="65"/>
@@ -46843,11 +46846,11 @@
         <v>100</v>
       </c>
       <c r="E12" s="91"/>
-      <c r="F12" s="622" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="623"/>
-      <c r="H12" s="624"/>
+      <c r="F12" s="631" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="632"/>
+      <c r="H12" s="633"/>
       <c r="I12" s="91"/>
       <c r="J12" s="65"/>
       <c r="K12" s="65"/>
@@ -46860,11 +46863,11 @@
         <v>75</v>
       </c>
       <c r="E13" s="91"/>
-      <c r="F13" s="622" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="623"/>
-      <c r="H13" s="624"/>
+      <c r="F13" s="631" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="632"/>
+      <c r="H13" s="633"/>
       <c r="I13" s="91"/>
       <c r="J13" s="65"/>
       <c r="K13" s="65"/>
@@ -46877,11 +46880,11 @@
         <v>73</v>
       </c>
       <c r="E14" s="91"/>
-      <c r="F14" s="622" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="623"/>
-      <c r="H14" s="624"/>
+      <c r="F14" s="631" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="632"/>
+      <c r="H14" s="633"/>
       <c r="I14" s="91"/>
       <c r="J14" s="65"/>
       <c r="K14" s="65"/>
@@ -46894,11 +46897,11 @@
         <v>101</v>
       </c>
       <c r="E15" s="91"/>
-      <c r="F15" s="622" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="623"/>
-      <c r="H15" s="624"/>
+      <c r="F15" s="631" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="632"/>
+      <c r="H15" s="633"/>
       <c r="I15" s="91"/>
       <c r="J15" s="65"/>
       <c r="K15" s="65"/>
@@ -46926,11 +46929,11 @@
         <v>100</v>
       </c>
       <c r="E17" s="91"/>
-      <c r="F17" s="622" t="s">
+      <c r="F17" s="631" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="623"/>
-      <c r="H17" s="624"/>
+      <c r="G17" s="632"/>
+      <c r="H17" s="633"/>
       <c r="I17" s="91"/>
       <c r="J17" s="65"/>
       <c r="K17" s="65"/>
@@ -46943,11 +46946,11 @@
         <v>77</v>
       </c>
       <c r="E18" s="91"/>
-      <c r="F18" s="622" t="s">
+      <c r="F18" s="631" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="623"/>
-      <c r="H18" s="624"/>
+      <c r="G18" s="632"/>
+      <c r="H18" s="633"/>
       <c r="I18" s="91"/>
       <c r="J18" s="65"/>
       <c r="K18" s="65"/>
@@ -46960,11 +46963,11 @@
         <v>78</v>
       </c>
       <c r="E19" s="65"/>
-      <c r="F19" s="625" t="s">
+      <c r="F19" s="628" t="s">
         <v>91</v>
       </c>
-      <c r="G19" s="626"/>
-      <c r="H19" s="627"/>
+      <c r="G19" s="629"/>
+      <c r="H19" s="630"/>
       <c r="I19" s="65"/>
       <c r="J19" s="65"/>
       <c r="K19" s="65"/>
@@ -46977,11 +46980,11 @@
         <v>79</v>
       </c>
       <c r="E20" s="65"/>
-      <c r="F20" s="625" t="s">
+      <c r="F20" s="628" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="626"/>
-      <c r="H20" s="627"/>
+      <c r="G20" s="629"/>
+      <c r="H20" s="630"/>
       <c r="I20" s="65"/>
       <c r="J20" s="65"/>
       <c r="K20" s="65"/>
@@ -46994,11 +46997,11 @@
         <v>89</v>
       </c>
       <c r="E21" s="66"/>
-      <c r="F21" s="631" t="s">
+      <c r="F21" s="625" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="632"/>
-      <c r="H21" s="633"/>
+      <c r="G21" s="626"/>
+      <c r="H21" s="627"/>
       <c r="I21" s="66"/>
       <c r="J21" s="66"/>
       <c r="K21" s="66"/>
@@ -47028,11 +47031,11 @@
       </c>
       <c r="D23" s="53"/>
       <c r="E23" s="65"/>
-      <c r="F23" s="625" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="626"/>
-      <c r="H23" s="627"/>
+      <c r="F23" s="628" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="629"/>
+      <c r="H23" s="630"/>
       <c r="I23" s="65"/>
       <c r="J23" s="65"/>
       <c r="K23" s="65"/>
@@ -47045,11 +47048,11 @@
       </c>
       <c r="D24" s="53"/>
       <c r="E24" s="65"/>
-      <c r="F24" s="625" t="s">
+      <c r="F24" s="628" t="s">
         <v>96</v>
       </c>
-      <c r="G24" s="626"/>
-      <c r="H24" s="627"/>
+      <c r="G24" s="629"/>
+      <c r="H24" s="630"/>
       <c r="I24" s="65"/>
       <c r="J24" s="65"/>
       <c r="K24" s="65"/>
@@ -47062,11 +47065,11 @@
         <v>103</v>
       </c>
       <c r="E25" s="65"/>
-      <c r="F25" s="625" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="626"/>
-      <c r="H25" s="627"/>
+      <c r="F25" s="628" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="629"/>
+      <c r="H25" s="630"/>
       <c r="I25" s="65"/>
       <c r="J25" s="65"/>
       <c r="K25" s="65"/>
@@ -47079,11 +47082,11 @@
       </c>
       <c r="D26" s="53"/>
       <c r="E26" s="65"/>
-      <c r="F26" s="625" t="s">
+      <c r="F26" s="628" t="s">
         <v>96</v>
       </c>
-      <c r="G26" s="626"/>
-      <c r="H26" s="627"/>
+      <c r="G26" s="629"/>
+      <c r="H26" s="630"/>
       <c r="I26" s="65"/>
       <c r="J26" s="65"/>
       <c r="K26" s="65"/>
@@ -47096,11 +47099,11 @@
         <v>105</v>
       </c>
       <c r="E27" s="65"/>
-      <c r="F27" s="625" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="626"/>
-      <c r="H27" s="627"/>
+      <c r="F27" s="628" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="629"/>
+      <c r="H27" s="630"/>
       <c r="I27" s="65"/>
       <c r="J27" s="65"/>
       <c r="K27" s="65"/>
@@ -47113,11 +47116,11 @@
       </c>
       <c r="D28" s="100"/>
       <c r="E28" s="65"/>
-      <c r="F28" s="625" t="s">
+      <c r="F28" s="628" t="s">
         <v>64</v>
       </c>
-      <c r="G28" s="626"/>
-      <c r="H28" s="627"/>
+      <c r="G28" s="629"/>
+      <c r="H28" s="630"/>
       <c r="I28" s="65"/>
       <c r="J28" s="65"/>
       <c r="K28" s="65"/>
@@ -47160,11 +47163,11 @@
         <v>100</v>
       </c>
       <c r="E31" s="65"/>
-      <c r="F31" s="625" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="626"/>
-      <c r="H31" s="627"/>
+      <c r="F31" s="628" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="629"/>
+      <c r="H31" s="630"/>
       <c r="I31" s="65"/>
       <c r="J31" s="65"/>
       <c r="K31" s="65"/>
@@ -47177,11 +47180,11 @@
         <v>75</v>
       </c>
       <c r="E32" s="65"/>
-      <c r="F32" s="625" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="626"/>
-      <c r="H32" s="627"/>
+      <c r="F32" s="628" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="629"/>
+      <c r="H32" s="630"/>
       <c r="I32" s="65"/>
       <c r="J32" s="65"/>
       <c r="K32" s="65"/>
@@ -47194,11 +47197,11 @@
         <v>73</v>
       </c>
       <c r="E33" s="65"/>
-      <c r="F33" s="625" t="s">
+      <c r="F33" s="628" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="626"/>
-      <c r="H33" s="627"/>
+      <c r="G33" s="629"/>
+      <c r="H33" s="630"/>
       <c r="I33" s="65"/>
       <c r="J33" s="65"/>
       <c r="K33" s="65"/>
@@ -47344,9 +47347,9 @@
       <c r="C41" s="73"/>
       <c r="D41" s="53"/>
       <c r="E41" s="66"/>
-      <c r="F41" s="631"/>
-      <c r="G41" s="632"/>
-      <c r="H41" s="633"/>
+      <c r="F41" s="625"/>
+      <c r="G41" s="626"/>
+      <c r="H41" s="627"/>
       <c r="I41" s="66"/>
       <c r="J41" s="66"/>
       <c r="K41" s="66"/>
@@ -47361,9 +47364,9 @@
       <c r="C42" s="83"/>
       <c r="D42" s="55"/>
       <c r="E42" s="66"/>
-      <c r="F42" s="628"/>
-      <c r="G42" s="629"/>
-      <c r="H42" s="630"/>
+      <c r="F42" s="622"/>
+      <c r="G42" s="623"/>
+      <c r="H42" s="624"/>
       <c r="I42" s="66"/>
       <c r="J42" s="66"/>
       <c r="K42" s="66"/>
@@ -47424,19 +47427,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F23:H23"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A22:A41"/>
     <mergeCell ref="A4:A21"/>
@@ -47453,6 +47443,19 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F23:H23"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:D42">
     <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">

</xml_diff>